<commit_message>
tied teams top third
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
+++ b/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>goal_time</t>
+          <t>goal_minute</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -556,7 +556,7 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>['Belgium', 'France', 'Denmark']</t>
+          <t>['France', 'Denmark']</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>26</v>
@@ -630,7 +630,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>['Belgium', 'France', 'Denmark']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -649,13 +649,13 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q3" t="n">
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="R3" t="inlineStr"/>
     </row>
@@ -679,7 +679,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>32</v>
@@ -704,7 +704,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>['Belgium', 'France', 'Denmark']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -726,10 +726,10 @@
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q4" t="n">
-        <v>9</v>
+        <v>-5</v>
       </c>
       <c r="R4" t="inlineStr"/>
     </row>
@@ -753,7 +753,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>39</v>
@@ -778,7 +778,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>['Belgium', 'France', 'Denmark']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -800,10 +800,10 @@
         <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q5" t="n">
-        <v>8</v>
+        <v>-3</v>
       </c>
       <c r="R5" t="inlineStr"/>
     </row>
@@ -827,7 +827,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>41</v>
@@ -852,7 +852,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>['Belgium', 'France', 'Denmark']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -874,10 +874,10 @@
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q6" t="n">
-        <v>9</v>
+        <v>-5</v>
       </c>
       <c r="R6" t="inlineStr"/>
     </row>
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>59</v>
@@ -926,7 +926,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>['Belgium', 'France', 'Denmark']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -948,10 +948,10 @@
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q7" t="n">
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="R7" t="inlineStr"/>
     </row>
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>60</v>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>['Belgium', 'France', 'Denmark']</t>
+          <t>['France', 'Denmark']</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1019,13 +1019,13 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R8" t="inlineStr"/>
     </row>
@@ -1049,7 +1049,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>62</v>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>['Belgium', 'France', 'Denmark']</t>
+          <t>['France', 'Denmark']</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1096,10 +1096,10 @@
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R9" t="inlineStr"/>
     </row>
@@ -1123,7 +1123,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>77</v>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>['Belgium', 'France', 'Denmark']</t>
+          <t>['France', 'Denmark']</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1170,10 +1170,10 @@
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R10" t="inlineStr"/>
     </row>
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>84</v>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>['Belgium', 'France', 'Denmark']</t>
+          <t>['France', 'Denmark']</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1244,10 +1244,10 @@
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R11" t="inlineStr"/>
     </row>
@@ -1271,7 +1271,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>84</v>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>['Belgium', 'France', 'Denmark']</t>
+          <t>['France', 'Denmark']</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1321,7 +1321,7 @@
         <v>2</v>
       </c>
       <c r="Q12" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="R12" t="inlineStr"/>
     </row>
@@ -1356,7 +1356,7 @@
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
-          <t>['Spain', 'West Germany', 'Portugal']</t>
+          <t>['Spain', 'West Germany']</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1426,7 +1426,7 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>['Spain', 'West Germany', 'Portugal']</t>
+          <t>['Spain', 'West Germany']</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1448,10 +1448,10 @@
         <v>0</v>
       </c>
       <c r="P14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R14" t="inlineStr"/>
     </row>
@@ -1496,7 +1496,7 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
-          <t>['Spain', 'West Germany', 'Portugal']</t>
+          <t>['Spain', 'West Germany']</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1518,10 +1518,10 @@
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15" t="inlineStr"/>
     </row>
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>81</v>
@@ -1570,7 +1570,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>['Spain', 'West Germany', 'Portugal']</t>
+          <t>['Portugal', 'West Germany']</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1589,15 +1589,19 @@
         </is>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q16" t="n">
-        <v>2</v>
-      </c>
-      <c r="R16" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Spain</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1619,7 +1623,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>90</v>
@@ -1644,7 +1648,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>['Spain', 'West Germany', 'Portugal']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1663,13 +1667,13 @@
         </is>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R17" t="inlineStr"/>
     </row>
@@ -1704,7 +1708,7 @@
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
-          <t>['Spain', 'West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1774,7 +1778,7 @@
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
-          <t>['Spain', 'West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1796,12 +1800,16 @@
         <v>0</v>
       </c>
       <c r="P19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q19" t="n">
-        <v>3</v>
-      </c>
-      <c r="R19" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Spain</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1844,7 +1852,7 @@
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr">
         <is>
-          <t>['Spain', 'West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1866,12 +1874,16 @@
         <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q20" t="n">
-        <v>3</v>
-      </c>
-      <c r="R20" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Spain</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1918,7 +1930,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>['Spain', 'West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -1940,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="P21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q21" t="n">
         <v>2</v>
@@ -1992,7 +2004,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>['Spain', 'West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2014,10 +2026,10 @@
         <v>0</v>
       </c>
       <c r="P22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R22" t="inlineStr"/>
     </row>
@@ -2066,7 +2078,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>['Spain', 'West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2088,10 +2100,10 @@
         <v>0</v>
       </c>
       <c r="P23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q23" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R23" t="inlineStr"/>
     </row>
@@ -2140,7 +2152,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>['Spain', 'West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -2162,10 +2174,10 @@
         <v>0</v>
       </c>
       <c r="P24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q24" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R24" t="inlineStr"/>
     </row>
@@ -2200,7 +2212,7 @@
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Republic of Ireland', 'Netherlands']</t>
+          <t>['Soviet Union', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2270,7 +2282,7 @@
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Republic of Ireland', 'Netherlands']</t>
+          <t>['Soviet Union', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2292,12 +2304,16 @@
         <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q26" t="n">
-        <v>4</v>
-      </c>
-      <c r="R26" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2344,7 +2360,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Republic of Ireland', 'Netherlands']</t>
+          <t>['Soviet Union', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2366,12 +2382,16 @@
         <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q27" t="n">
-        <v>5</v>
-      </c>
-      <c r="R27" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2418,7 +2438,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Republic of Ireland', 'Netherlands']</t>
+          <t>['Soviet Union', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2440,12 +2460,16 @@
         <v>0</v>
       </c>
       <c r="P28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q28" t="n">
-        <v>4</v>
-      </c>
-      <c r="R28" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2492,7 +2516,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Republic of Ireland', 'Netherlands']</t>
+          <t>['Soviet Union', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2514,12 +2538,16 @@
         <v>0</v>
       </c>
       <c r="P29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q29" t="n">
-        <v>5</v>
-      </c>
-      <c r="R29" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2566,7 +2594,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Republic of Ireland', 'Netherlands']</t>
+          <t>['Soviet Union', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2588,12 +2616,16 @@
         <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q30" t="n">
-        <v>6</v>
-      </c>
-      <c r="R30" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2615,7 +2647,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>82</v>
@@ -2640,7 +2672,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Republic of Ireland', 'Netherlands']</t>
+          <t>['Soviet Union', 'Netherlands']</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2659,13 +2691,13 @@
         </is>
       </c>
       <c r="O31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q31" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R31" t="inlineStr"/>
     </row>
@@ -2700,7 +2732,7 @@
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr">
         <is>
-          <t>['Sweden', 'France', 'England']</t>
+          <t>['France', 'Sweden']</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2749,7 +2781,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>4</v>
@@ -2774,7 +2806,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>['Sweden', 'France', 'England']</t>
+          <t>['Sweden', 'England']</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2793,13 +2825,13 @@
         </is>
       </c>
       <c r="O33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R33" t="inlineStr"/>
     </row>
@@ -2848,7 +2880,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>['Sweden', 'England', 'Denmark']</t>
+          <t>['Sweden', 'England']</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2867,13 +2899,13 @@
         </is>
       </c>
       <c r="O34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R34" t="inlineStr"/>
     </row>
@@ -2922,7 +2954,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>['Sweden', 'England', 'Denmark']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -2944,10 +2976,10 @@
         <v>0</v>
       </c>
       <c r="P35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R35" t="inlineStr"/>
     </row>
@@ -2996,7 +3028,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>['Sweden', 'France', 'England']</t>
+          <t>['France', 'Sweden']</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3018,10 +3050,10 @@
         <v>1</v>
       </c>
       <c r="P36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R36" t="inlineStr"/>
     </row>
@@ -3070,7 +3102,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>['Sweden', 'England', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3092,10 +3124,10 @@
         <v>1</v>
       </c>
       <c r="P37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R37" t="inlineStr"/>
     </row>
@@ -3119,7 +3151,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>82</v>
@@ -3144,7 +3176,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>['Sweden', 'France', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3163,13 +3195,13 @@
         </is>
       </c>
       <c r="O38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R38" t="inlineStr"/>
     </row>
@@ -3204,7 +3236,7 @@
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany', 'CIS']</t>
+          <t>['Germany', 'Netherlands']</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3274,7 +3306,7 @@
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany', 'CIS']</t>
+          <t>['Germany', 'Netherlands']</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3296,12 +3328,16 @@
         <v>0</v>
       </c>
       <c r="P40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q40" t="n">
-        <v>3</v>
-      </c>
-      <c r="R40" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>CIS</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -3348,7 +3384,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany', 'CIS']</t>
+          <t>['Germany', 'Netherlands']</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3370,10 +3406,10 @@
         <v>0</v>
       </c>
       <c r="P41" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q41" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R41" t="inlineStr"/>
     </row>
@@ -3422,7 +3458,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany', 'CIS']</t>
+          <t>['Germany', 'Netherlands']</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3444,10 +3480,10 @@
         <v>0</v>
       </c>
       <c r="P42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R42" t="inlineStr"/>
     </row>
@@ -3496,7 +3532,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany', 'CIS']</t>
+          <t>['Germany', 'Netherlands']</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3518,7 +3554,7 @@
         <v>0</v>
       </c>
       <c r="P43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q43" t="n">
         <v>1</v>
@@ -3545,7 +3581,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
         <v>16</v>
@@ -3570,7 +3606,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>['Scotland', 'Netherlands', 'Germany']</t>
+          <t>['Germany', 'Netherlands']</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3589,10 +3625,10 @@
         </is>
       </c>
       <c r="O44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q44" t="n">
         <v>1</v>
@@ -3619,7 +3655,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" t="n">
         <v>53</v>
@@ -3644,7 +3680,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>['Scotland', 'Netherlands', 'Germany']</t>
+          <t>['Germany', 'Netherlands']</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3666,10 +3702,10 @@
         <v>0</v>
       </c>
       <c r="P45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R45" t="inlineStr"/>
     </row>
@@ -3693,7 +3729,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" t="n">
         <v>72</v>
@@ -3718,7 +3754,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>['Scotland', 'Netherlands', 'Germany']</t>
+          <t>['Germany', 'Netherlands']</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3740,7 +3776,7 @@
         <v>0</v>
       </c>
       <c r="P46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q46" t="n">
         <v>1</v>
@@ -3767,7 +3803,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" t="n">
         <v>84</v>
@@ -3792,7 +3828,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>['Scotland', 'Netherlands', 'Germany']</t>
+          <t>['Germany', 'Netherlands']</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3814,10 +3850,10 @@
         <v>0</v>
       </c>
       <c r="P47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q47" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R47" t="inlineStr"/>
     </row>
@@ -3852,7 +3888,7 @@
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr">
         <is>
-          <t>['France', 'Bulgaria']</t>
+          <t>['Bulgaria', 'France']</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -5648,7 +5684,7 @@
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr">
         <is>
-          <t>['Germany', 'Italy']</t>
+          <t>['Italy', 'Germany']</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -5718,7 +5754,7 @@
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr">
         <is>
-          <t>['Germany', 'Italy']</t>
+          <t>['Italy', 'Germany']</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -5792,7 +5828,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -5870,7 +5906,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -5948,7 +5984,7 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
@@ -6026,7 +6062,7 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>['Germany', 'Italy']</t>
+          <t>['Italy', 'Germany']</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
@@ -6100,7 +6136,7 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>['Germany', 'Italy']</t>
+          <t>['Italy', 'Germany']</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
@@ -6174,7 +6210,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>['Germany', 'Italy']</t>
+          <t>['Italy', 'Germany']</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
@@ -6234,7 +6270,7 @@
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr">
         <is>
-          <t>['Belgium', 'Italy']</t>
+          <t>['Italy', 'Belgium']</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
@@ -6304,7 +6340,7 @@
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="inlineStr">
         <is>
-          <t>['Belgium', 'Italy']</t>
+          <t>['Italy', 'Belgium']</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
@@ -6382,7 +6418,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>['Belgium', 'Italy']</t>
+          <t>['Italy', 'Belgium']</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -6460,7 +6496,7 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>['Turkey', 'Italy']</t>
+          <t>['Italy', 'Turkey']</t>
         </is>
       </c>
       <c r="L84" t="inlineStr">
@@ -6534,7 +6570,7 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>['Turkey', 'Italy']</t>
+          <t>['Italy', 'Turkey']</t>
         </is>
       </c>
       <c r="L85" t="inlineStr">
@@ -6608,7 +6644,7 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>['Turkey', 'Italy']</t>
+          <t>['Italy', 'Turkey']</t>
         </is>
       </c>
       <c r="L86" t="inlineStr">
@@ -6682,7 +6718,7 @@
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>['Turkey', 'Italy']</t>
+          <t>['Italy', 'Turkey']</t>
         </is>
       </c>
       <c r="L87" t="inlineStr">
@@ -7484,7 +7520,7 @@
       <c r="J98" t="inlineStr"/>
       <c r="K98" t="inlineStr">
         <is>
-          <t>['Spain', 'FR Yugoslavia']</t>
+          <t>['FR Yugoslavia', 'Spain']</t>
         </is>
       </c>
       <c r="L98" t="inlineStr">
@@ -7554,7 +7590,7 @@
       <c r="J99" t="inlineStr"/>
       <c r="K99" t="inlineStr">
         <is>
-          <t>['Spain', 'FR Yugoslavia']</t>
+          <t>['FR Yugoslavia', 'Spain']</t>
         </is>
       </c>
       <c r="L99" t="inlineStr">
@@ -7628,7 +7664,7 @@
       </c>
       <c r="K100" t="inlineStr">
         <is>
-          <t>['Norway', 'FR Yugoslavia']</t>
+          <t>['FR Yugoslavia', 'Norway']</t>
         </is>
       </c>
       <c r="L100" t="inlineStr">
@@ -7702,7 +7738,7 @@
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>['Spain', 'FR Yugoslavia']</t>
+          <t>['FR Yugoslavia', 'Spain']</t>
         </is>
       </c>
       <c r="L101" t="inlineStr">
@@ -7776,7 +7812,7 @@
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>['Norway', 'FR Yugoslavia']</t>
+          <t>['FR Yugoslavia', 'Norway']</t>
         </is>
       </c>
       <c r="L102" t="inlineStr">
@@ -7850,7 +7886,7 @@
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>['Spain', 'FR Yugoslavia']</t>
+          <t>['FR Yugoslavia', 'Spain']</t>
         </is>
       </c>
       <c r="L103" t="inlineStr">
@@ -7924,7 +7960,7 @@
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>['Norway', 'FR Yugoslavia']</t>
+          <t>['FR Yugoslavia', 'Norway']</t>
         </is>
       </c>
       <c r="L104" t="inlineStr">
@@ -7998,7 +8034,7 @@
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>['Spain', 'FR Yugoslavia']</t>
+          <t>['FR Yugoslavia', 'Spain']</t>
         </is>
       </c>
       <c r="L105" t="inlineStr">
@@ -8072,7 +8108,7 @@
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>['Spain', 'FR Yugoslavia']</t>
+          <t>['FR Yugoslavia', 'Spain']</t>
         </is>
       </c>
       <c r="L106" t="inlineStr">
@@ -8132,7 +8168,7 @@
       <c r="J107" t="inlineStr"/>
       <c r="K107" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L107" t="inlineStr">
@@ -8202,7 +8238,7 @@
       <c r="J108" t="inlineStr"/>
       <c r="K108" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L108" t="inlineStr">
@@ -8276,7 +8312,7 @@
       </c>
       <c r="K109" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L109" t="inlineStr">
@@ -8350,7 +8386,7 @@
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L110" t="inlineStr">
@@ -8424,7 +8460,7 @@
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L111" t="inlineStr">
@@ -8498,7 +8534,7 @@
       </c>
       <c r="K112" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L112" t="inlineStr">
@@ -8572,7 +8608,7 @@
       </c>
       <c r="K113" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L113" t="inlineStr">
@@ -8646,7 +8682,7 @@
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L114" t="inlineStr">
@@ -8720,7 +8756,7 @@
       </c>
       <c r="K115" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L115" t="inlineStr">
@@ -8780,7 +8816,7 @@
       <c r="J116" t="inlineStr"/>
       <c r="K116" t="inlineStr">
         <is>
-          <t>['Greece', 'Spain']</t>
+          <t>['Spain', 'Greece']</t>
         </is>
       </c>
       <c r="L116" t="inlineStr">
@@ -8850,7 +8886,7 @@
       <c r="J117" t="inlineStr"/>
       <c r="K117" t="inlineStr">
         <is>
-          <t>['Greece', 'Spain']</t>
+          <t>['Spain', 'Greece']</t>
         </is>
       </c>
       <c r="L117" t="inlineStr">
@@ -9146,7 +9182,7 @@
       </c>
       <c r="K121" t="inlineStr">
         <is>
-          <t>['Greece', 'Portugal']</t>
+          <t>['Portugal', 'Greece']</t>
         </is>
       </c>
       <c r="L121" t="inlineStr">
@@ -10006,7 +10042,7 @@
       <c r="J133" t="inlineStr"/>
       <c r="K133" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="L133" t="inlineStr">
@@ -10228,7 +10264,7 @@
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="L136" t="inlineStr">
@@ -10302,7 +10338,7 @@
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="L137" t="inlineStr">
@@ -10450,7 +10486,7 @@
       </c>
       <c r="K139" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="L139" t="inlineStr">
@@ -10524,7 +10560,7 @@
       </c>
       <c r="K140" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="L140" t="inlineStr">
@@ -10584,7 +10620,7 @@
       <c r="J141" t="inlineStr"/>
       <c r="K141" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="L141" t="inlineStr">
@@ -10654,7 +10690,7 @@
       <c r="J142" t="inlineStr"/>
       <c r="K142" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="L142" t="inlineStr">
@@ -10728,7 +10764,7 @@
       </c>
       <c r="K143" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="L143" t="inlineStr">
@@ -10802,7 +10838,7 @@
       </c>
       <c r="K144" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="L144" t="inlineStr">
@@ -10876,7 +10912,7 @@
       </c>
       <c r="K145" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Netherlands']</t>
         </is>
       </c>
       <c r="L145" t="inlineStr">
@@ -10950,7 +10986,7 @@
       </c>
       <c r="K146" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Netherlands']</t>
         </is>
       </c>
       <c r="L146" t="inlineStr">
@@ -11024,7 +11060,7 @@
       </c>
       <c r="K147" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Netherlands']</t>
         </is>
       </c>
       <c r="L147" t="inlineStr">
@@ -11098,7 +11134,7 @@
       </c>
       <c r="K148" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Netherlands']</t>
         </is>
       </c>
       <c r="L148" t="inlineStr">
@@ -11158,7 +11194,7 @@
       <c r="J149" t="inlineStr"/>
       <c r="K149" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="L149" t="inlineStr">
@@ -11228,7 +11264,7 @@
       <c r="J150" t="inlineStr"/>
       <c r="K150" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="L150" t="inlineStr">
@@ -11302,7 +11338,7 @@
       </c>
       <c r="K151" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="L151" t="inlineStr">
@@ -11376,7 +11412,7 @@
       </c>
       <c r="K152" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="L152" t="inlineStr">
@@ -11450,7 +11486,7 @@
       </c>
       <c r="K153" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="L153" t="inlineStr">
@@ -11524,7 +11560,7 @@
       </c>
       <c r="K154" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="L154" t="inlineStr">
@@ -11598,7 +11634,7 @@
       </c>
       <c r="K155" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="L155" t="inlineStr">
@@ -11672,7 +11708,7 @@
       </c>
       <c r="K156" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="L156" t="inlineStr">
@@ -11746,7 +11782,7 @@
       </c>
       <c r="K157" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal']</t>
+          <t>['Portugal', 'Turkey']</t>
         </is>
       </c>
       <c r="L157" t="inlineStr">
@@ -12154,7 +12190,7 @@
       <c r="J163" t="inlineStr"/>
       <c r="K163" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Romania']</t>
+          <t>['Romania', 'Netherlands']</t>
         </is>
       </c>
       <c r="L163" t="inlineStr">
@@ -12224,7 +12260,7 @@
       <c r="J164" t="inlineStr"/>
       <c r="K164" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Romania']</t>
+          <t>['Romania', 'Netherlands']</t>
         </is>
       </c>
       <c r="L164" t="inlineStr">
@@ -12294,7 +12330,7 @@
       <c r="J165" t="inlineStr"/>
       <c r="K165" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Romania']</t>
+          <t>['Romania', 'Netherlands']</t>
         </is>
       </c>
       <c r="L165" t="inlineStr">
@@ -12368,7 +12404,7 @@
       </c>
       <c r="K166" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Italy']</t>
+          <t>['Italy', 'Netherlands']</t>
         </is>
       </c>
       <c r="L166" t="inlineStr">
@@ -12442,7 +12478,7 @@
       </c>
       <c r="K167" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Italy']</t>
+          <t>['Italy', 'Netherlands']</t>
         </is>
       </c>
       <c r="L167" t="inlineStr">
@@ -12516,7 +12552,7 @@
       </c>
       <c r="K168" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Italy']</t>
+          <t>['Italy', 'Netherlands']</t>
         </is>
       </c>
       <c r="L168" t="inlineStr">
@@ -12590,7 +12626,7 @@
       </c>
       <c r="K169" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Italy']</t>
+          <t>['Italy', 'Netherlands']</t>
         </is>
       </c>
       <c r="L169" t="inlineStr">
@@ -12650,7 +12686,7 @@
       <c r="J170" t="inlineStr"/>
       <c r="K170" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="L170" t="inlineStr">
@@ -12720,7 +12756,7 @@
       <c r="J171" t="inlineStr"/>
       <c r="K171" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="L171" t="inlineStr">
@@ -12794,7 +12830,7 @@
       </c>
       <c r="K172" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="L172" t="inlineStr">
@@ -12868,7 +12904,7 @@
       </c>
       <c r="K173" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="L173" t="inlineStr">
@@ -12942,7 +12978,7 @@
       </c>
       <c r="K174" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="L174" t="inlineStr">
@@ -13016,7 +13052,7 @@
       </c>
       <c r="K175" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="L175" t="inlineStr">
@@ -13090,7 +13126,7 @@
       </c>
       <c r="K176" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="L176" t="inlineStr">
@@ -13438,7 +13474,7 @@
       </c>
       <c r="K181" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="L181" t="inlineStr">
@@ -13498,7 +13534,7 @@
       <c r="J182" t="inlineStr"/>
       <c r="K182" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="L182" t="inlineStr">
@@ -13646,7 +13682,7 @@
       </c>
       <c r="K184" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="L184" t="inlineStr">
@@ -13794,7 +13830,7 @@
       </c>
       <c r="K186" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="L186" t="inlineStr">
@@ -13868,7 +13904,7 @@
       </c>
       <c r="K187" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="L187" t="inlineStr">
@@ -13946,7 +13982,7 @@
       </c>
       <c r="K188" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="L188" t="inlineStr">
@@ -14006,7 +14042,7 @@
       <c r="J189" t="inlineStr"/>
       <c r="K189" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="L189" t="inlineStr">
@@ -14076,7 +14112,7 @@
       <c r="J190" t="inlineStr"/>
       <c r="K190" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="L190" t="inlineStr">
@@ -14146,7 +14182,7 @@
       <c r="J191" t="inlineStr"/>
       <c r="K191" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="L191" t="inlineStr">
@@ -14220,7 +14256,7 @@
       </c>
       <c r="K192" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Italy', 'Spain']</t>
         </is>
       </c>
       <c r="L192" t="inlineStr">
@@ -14850,7 +14886,7 @@
       <c r="J201" t="inlineStr"/>
       <c r="K201" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['Romania', 'Switzerland', 'France']</t>
         </is>
       </c>
       <c r="L201" t="inlineStr">
@@ -14920,7 +14956,7 @@
       <c r="J202" t="inlineStr"/>
       <c r="K202" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['Romania', 'Switzerland', 'France']</t>
         </is>
       </c>
       <c r="L202" t="inlineStr">
@@ -14942,7 +14978,7 @@
         <v>0</v>
       </c>
       <c r="P202" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q202" t="n">
         <v>2</v>
@@ -14990,7 +15026,7 @@
       <c r="J203" t="inlineStr"/>
       <c r="K203" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['Romania', 'Switzerland', 'France']</t>
         </is>
       </c>
       <c r="L203" t="inlineStr">
@@ -15012,7 +15048,7 @@
         <v>0</v>
       </c>
       <c r="P203" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q203" t="n">
         <v>2</v>
@@ -15039,7 +15075,7 @@
         </is>
       </c>
       <c r="E204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F204" t="n">
         <v>43</v>
@@ -15064,7 +15100,7 @@
       </c>
       <c r="K204" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['Switzerland', 'France', 'Albania']</t>
         </is>
       </c>
       <c r="L204" t="inlineStr">
@@ -15083,13 +15119,13 @@
         </is>
       </c>
       <c r="O204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P204" t="n">
         <v>2</v>
       </c>
       <c r="Q204" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R204" t="inlineStr"/>
     </row>
@@ -15124,7 +15160,7 @@
       <c r="J205" t="inlineStr"/>
       <c r="K205" t="inlineStr">
         <is>
-          <t>['Wales', 'England']</t>
+          <t>['Wales', 'Slovakia', 'England']</t>
         </is>
       </c>
       <c r="L205" t="inlineStr">
@@ -15194,7 +15230,7 @@
       <c r="J206" t="inlineStr"/>
       <c r="K206" t="inlineStr">
         <is>
-          <t>['Wales', 'England']</t>
+          <t>['Wales', 'Slovakia', 'England']</t>
         </is>
       </c>
       <c r="L206" t="inlineStr">
@@ -15216,12 +15252,16 @@
         <v>0</v>
       </c>
       <c r="P206" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q206" t="n">
-        <v>0</v>
-      </c>
-      <c r="R206" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="R206" t="inlineStr">
+        <is>
+          <t>Slovakia</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
@@ -15264,7 +15304,7 @@
       <c r="J207" t="inlineStr"/>
       <c r="K207" t="inlineStr">
         <is>
-          <t>['Wales', 'England']</t>
+          <t>['Wales', 'Slovakia', 'England']</t>
         </is>
       </c>
       <c r="L207" t="inlineStr">
@@ -15286,12 +15326,16 @@
         <v>0</v>
       </c>
       <c r="P207" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q207" t="n">
-        <v>0</v>
-      </c>
-      <c r="R207" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="R207" t="inlineStr">
+        <is>
+          <t>Slovakia</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
@@ -15338,7 +15382,7 @@
       </c>
       <c r="K208" t="inlineStr">
         <is>
-          <t>['Wales', 'England']</t>
+          <t>['Wales', 'Slovakia', 'England']</t>
         </is>
       </c>
       <c r="L208" t="inlineStr">
@@ -15360,10 +15404,10 @@
         <v>0</v>
       </c>
       <c r="P208" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q208" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R208" t="inlineStr"/>
     </row>
@@ -15412,7 +15456,7 @@
       </c>
       <c r="K209" t="inlineStr">
         <is>
-          <t>['Wales', 'England']</t>
+          <t>['Wales', 'Slovakia', 'England']</t>
         </is>
       </c>
       <c r="L209" t="inlineStr">
@@ -15434,10 +15478,10 @@
         <v>0</v>
       </c>
       <c r="P209" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q209" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R209" t="inlineStr"/>
     </row>
@@ -15486,7 +15530,7 @@
       </c>
       <c r="K210" t="inlineStr">
         <is>
-          <t>['Wales', 'England']</t>
+          <t>['Wales', 'Slovakia', 'England']</t>
         </is>
       </c>
       <c r="L210" t="inlineStr">
@@ -15508,10 +15552,10 @@
         <v>0</v>
       </c>
       <c r="P210" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q210" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R210" t="inlineStr"/>
     </row>
@@ -15546,7 +15590,7 @@
       <c r="J211" t="inlineStr"/>
       <c r="K211" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland']</t>
+          <t>['Northern Ireland', 'Poland', 'Germany']</t>
         </is>
       </c>
       <c r="L211" t="inlineStr">
@@ -15616,7 +15660,7 @@
       <c r="J212" t="inlineStr"/>
       <c r="K212" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland']</t>
+          <t>['Northern Ireland', 'Poland', 'Germany']</t>
         </is>
       </c>
       <c r="L212" t="inlineStr">
@@ -15638,10 +15682,10 @@
         <v>0</v>
       </c>
       <c r="P212" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q212" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R212" t="inlineStr"/>
     </row>
@@ -15686,7 +15730,7 @@
       <c r="J213" t="inlineStr"/>
       <c r="K213" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland']</t>
+          <t>['Northern Ireland', 'Poland', 'Germany']</t>
         </is>
       </c>
       <c r="L213" t="inlineStr">
@@ -15708,10 +15752,10 @@
         <v>0</v>
       </c>
       <c r="P213" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q213" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R213" t="inlineStr"/>
     </row>
@@ -15760,7 +15804,7 @@
       </c>
       <c r="K214" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland']</t>
+          <t>['Northern Ireland', 'Poland', 'Germany']</t>
         </is>
       </c>
       <c r="L214" t="inlineStr">
@@ -15785,7 +15829,7 @@
         <v>2</v>
       </c>
       <c r="Q214" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R214" t="inlineStr"/>
     </row>
@@ -15834,7 +15878,7 @@
       </c>
       <c r="K215" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland']</t>
+          <t>['Northern Ireland', 'Poland', 'Germany']</t>
         </is>
       </c>
       <c r="L215" t="inlineStr">
@@ -15856,10 +15900,10 @@
         <v>0</v>
       </c>
       <c r="P215" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q215" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R215" t="inlineStr"/>
     </row>
@@ -15894,7 +15938,7 @@
       <c r="J216" t="inlineStr"/>
       <c r="K216" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Czech Republic', 'Croatia']</t>
         </is>
       </c>
       <c r="L216" t="inlineStr">
@@ -15964,7 +16008,7 @@
       <c r="J217" t="inlineStr"/>
       <c r="K217" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Czech Republic', 'Croatia']</t>
         </is>
       </c>
       <c r="L217" t="inlineStr">
@@ -15986,10 +16030,10 @@
         <v>0</v>
       </c>
       <c r="P217" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q217" t="n">
         <v>3</v>
-      </c>
-      <c r="Q217" t="n">
-        <v>2</v>
       </c>
       <c r="R217" t="inlineStr"/>
     </row>
@@ -16038,7 +16082,7 @@
       </c>
       <c r="K218" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Czech Republic', 'Croatia']</t>
         </is>
       </c>
       <c r="L218" t="inlineStr">
@@ -16060,16 +16104,12 @@
         <v>0</v>
       </c>
       <c r="P218" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q218" t="n">
-        <v>1</v>
-      </c>
-      <c r="R218" t="inlineStr">
-        <is>
-          <t>tie</t>
-        </is>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="R218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -16091,7 +16131,7 @@
         </is>
       </c>
       <c r="E219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F219" t="n">
         <v>10</v>
@@ -16116,7 +16156,7 @@
       </c>
       <c r="K219" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Turkey', 'Croatia']</t>
         </is>
       </c>
       <c r="L219" t="inlineStr">
@@ -16135,13 +16175,13 @@
         </is>
       </c>
       <c r="O219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P219" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q219" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="R219" t="inlineStr"/>
     </row>
@@ -16165,7 +16205,7 @@
         </is>
       </c>
       <c r="E220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F220" t="n">
         <v>45</v>
@@ -16190,7 +16230,7 @@
       </c>
       <c r="K220" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Turkey', 'Croatia']</t>
         </is>
       </c>
       <c r="L220" t="inlineStr">
@@ -16215,7 +16255,7 @@
         <v>2</v>
       </c>
       <c r="Q220" t="n">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="R220" t="inlineStr"/>
     </row>
@@ -16239,7 +16279,7 @@
         </is>
       </c>
       <c r="E221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F221" t="n">
         <v>65</v>
@@ -16264,7 +16304,7 @@
       </c>
       <c r="K221" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Turkey', 'Croatia']</t>
         </is>
       </c>
       <c r="L221" t="inlineStr">
@@ -16289,7 +16329,7 @@
         <v>2</v>
       </c>
       <c r="Q221" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R221" t="inlineStr"/>
     </row>
@@ -16313,7 +16353,7 @@
         </is>
       </c>
       <c r="E222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F222" t="n">
         <v>87</v>
@@ -16338,7 +16378,7 @@
       </c>
       <c r="K222" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Croatia', 'Spain', 'Turkey']</t>
         </is>
       </c>
       <c r="L222" t="inlineStr">
@@ -16360,10 +16400,10 @@
         <v>0</v>
       </c>
       <c r="P222" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q222" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R222" t="inlineStr"/>
     </row>
@@ -16398,7 +16438,7 @@
       <c r="J223" t="inlineStr"/>
       <c r="K223" t="inlineStr">
         <is>
-          <t>['Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Portugal', 'Iceland']</t>
         </is>
       </c>
       <c r="L223" t="inlineStr">
@@ -16472,7 +16512,7 @@
       </c>
       <c r="K224" t="inlineStr">
         <is>
-          <t>['Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Portugal', 'Iceland']</t>
         </is>
       </c>
       <c r="L224" t="inlineStr">
@@ -16497,13 +16537,9 @@
         <v>2</v>
       </c>
       <c r="Q224" t="n">
-        <v>1</v>
-      </c>
-      <c r="R224" t="inlineStr">
-        <is>
-          <t>Iceland</t>
-        </is>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="R224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="n">
@@ -16550,7 +16586,7 @@
       </c>
       <c r="K225" t="inlineStr">
         <is>
-          <t>['Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Portugal', 'Iceland']</t>
         </is>
       </c>
       <c r="L225" t="inlineStr">
@@ -16572,7 +16608,7 @@
         <v>0</v>
       </c>
       <c r="P225" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q225" t="n">
         <v>2</v>
@@ -16624,7 +16660,7 @@
       </c>
       <c r="K226" t="inlineStr">
         <is>
-          <t>['Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Portugal', 'Iceland']</t>
         </is>
       </c>
       <c r="L226" t="inlineStr">
@@ -16649,13 +16685,9 @@
         <v>2</v>
       </c>
       <c r="Q226" t="n">
-        <v>1</v>
-      </c>
-      <c r="R226" t="inlineStr">
-        <is>
-          <t>tie</t>
-        </is>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="R226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="n">
@@ -16702,7 +16734,7 @@
       </c>
       <c r="K227" t="inlineStr">
         <is>
-          <t>['Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Portugal', 'Iceland']</t>
         </is>
       </c>
       <c r="L227" t="inlineStr">
@@ -16724,7 +16756,7 @@
         <v>0</v>
       </c>
       <c r="P227" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q227" t="n">
         <v>2</v>
@@ -16776,7 +16808,7 @@
       </c>
       <c r="K228" t="inlineStr">
         <is>
-          <t>['Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Portugal', 'Iceland']</t>
         </is>
       </c>
       <c r="L228" t="inlineStr">
@@ -16801,13 +16833,9 @@
         <v>2</v>
       </c>
       <c r="Q228" t="n">
-        <v>1</v>
-      </c>
-      <c r="R228" t="inlineStr">
-        <is>
-          <t>Portugal</t>
-        </is>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="R228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="n">
@@ -16854,7 +16882,7 @@
       </c>
       <c r="K229" t="inlineStr">
         <is>
-          <t>['Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Portugal', 'Iceland']</t>
         </is>
       </c>
       <c r="L229" t="inlineStr">
@@ -16876,7 +16904,7 @@
         <v>0</v>
       </c>
       <c r="P229" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q229" t="n">
         <v>2</v>
@@ -16928,7 +16956,7 @@
       </c>
       <c r="K230" t="inlineStr">
         <is>
-          <t>['Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Portugal', 'Iceland']</t>
         </is>
       </c>
       <c r="L230" t="inlineStr">
@@ -16950,7 +16978,7 @@
         <v>0</v>
       </c>
       <c r="P230" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q230" t="n">
         <v>1</v>
@@ -16977,7 +17005,7 @@
         </is>
       </c>
       <c r="E231" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F231" t="n">
         <v>62</v>
@@ -17002,7 +17030,7 @@
       </c>
       <c r="K231" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary']</t>
+          <t>['Hungary', 'Portugal', 'Iceland']</t>
         </is>
       </c>
       <c r="L231" t="inlineStr">
@@ -17021,13 +17049,13 @@
         </is>
       </c>
       <c r="O231" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q231" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R231" t="inlineStr"/>
     </row>
@@ -17051,7 +17079,7 @@
         </is>
       </c>
       <c r="E232" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F232" t="n">
         <v>94</v>
@@ -17076,7 +17104,7 @@
       </c>
       <c r="K232" t="inlineStr">
         <is>
-          <t>['Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Portugal', 'Iceland']</t>
         </is>
       </c>
       <c r="L232" t="inlineStr">
@@ -17095,19 +17123,15 @@
         </is>
       </c>
       <c r="O232" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P232" t="n">
         <v>2</v>
       </c>
       <c r="Q232" t="n">
-        <v>1</v>
-      </c>
-      <c r="R232" t="inlineStr">
-        <is>
-          <t>Portugal</t>
-        </is>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="R232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="n">
@@ -17140,7 +17164,7 @@
       <c r="J233" t="inlineStr"/>
       <c r="K233" t="inlineStr">
         <is>
-          <t>['Belgium', 'Italy']</t>
+          <t>['Italy', 'Belgium', 'Sweden']</t>
         </is>
       </c>
       <c r="L233" t="inlineStr">
@@ -17210,7 +17234,7 @@
       <c r="J234" t="inlineStr"/>
       <c r="K234" t="inlineStr">
         <is>
-          <t>['Belgium', 'Italy']</t>
+          <t>['Italy', 'Belgium', 'Sweden']</t>
         </is>
       </c>
       <c r="L234" t="inlineStr">
@@ -17232,7 +17256,7 @@
         <v>0</v>
       </c>
       <c r="P234" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q234" t="n">
         <v>2</v>
@@ -17280,7 +17304,7 @@
       <c r="J235" t="inlineStr"/>
       <c r="K235" t="inlineStr">
         <is>
-          <t>['Belgium', 'Italy']</t>
+          <t>['Italy', 'Belgium', 'Sweden']</t>
         </is>
       </c>
       <c r="L235" t="inlineStr">
@@ -17302,7 +17326,7 @@
         <v>0</v>
       </c>
       <c r="P235" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q235" t="n">
         <v>2</v>
@@ -17329,7 +17353,7 @@
         </is>
       </c>
       <c r="E236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F236" t="n">
         <v>84</v>
@@ -17354,7 +17378,7 @@
       </c>
       <c r="K236" t="inlineStr">
         <is>
-          <t>['Belgium', 'Italy']</t>
+          <t>['Italy', 'Belgium', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="L236" t="inlineStr">
@@ -17373,13 +17397,13 @@
         </is>
       </c>
       <c r="O236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P236" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q236" t="n">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="R236" t="inlineStr"/>
     </row>
@@ -17403,7 +17427,7 @@
         </is>
       </c>
       <c r="E237" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F237" t="n">
         <v>85</v>
@@ -17428,7 +17452,7 @@
       </c>
       <c r="K237" t="inlineStr">
         <is>
-          <t>['Belgium', 'Italy']</t>
+          <t>['Italy', 'Belgium', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="L237" t="inlineStr">
@@ -17450,10 +17474,10 @@
         <v>0</v>
       </c>
       <c r="P237" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q237" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R237" t="inlineStr"/>
     </row>
@@ -17488,7 +17512,7 @@
       <c r="J238" t="inlineStr"/>
       <c r="K238" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="L238" t="inlineStr">
@@ -17558,7 +17582,7 @@
       <c r="J239" t="inlineStr"/>
       <c r="K239" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="L239" t="inlineStr">
@@ -17580,10 +17604,10 @@
         <v>0</v>
       </c>
       <c r="P239" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q239" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R239" t="inlineStr"/>
     </row>
@@ -17632,7 +17656,7 @@
       </c>
       <c r="K240" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="L240" t="inlineStr">
@@ -17654,7 +17678,7 @@
         <v>0</v>
       </c>
       <c r="P240" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q240" t="n">
         <v>4</v>
@@ -17706,7 +17730,7 @@
       </c>
       <c r="K241" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="L241" t="inlineStr">
@@ -17728,10 +17752,10 @@
         <v>0</v>
       </c>
       <c r="P241" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q241" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R241" t="inlineStr"/>
     </row>
@@ -17780,7 +17804,7 @@
       </c>
       <c r="K242" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="L242" t="inlineStr">
@@ -17802,10 +17826,10 @@
         <v>0</v>
       </c>
       <c r="P242" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q242" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R242" t="inlineStr"/>
     </row>
@@ -17854,7 +17878,7 @@
       </c>
       <c r="K243" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="L243" t="inlineStr">
@@ -17876,10 +17900,10 @@
         <v>0</v>
       </c>
       <c r="P243" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q243" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R243" t="inlineStr"/>
     </row>
@@ -17928,7 +17952,7 @@
       </c>
       <c r="K244" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="L244" t="inlineStr">
@@ -17950,10 +17974,10 @@
         <v>0</v>
       </c>
       <c r="P244" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q244" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R244" t="inlineStr"/>
     </row>
@@ -17988,7 +18012,7 @@
       <c r="J245" t="inlineStr"/>
       <c r="K245" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Ukraine']</t>
+          <t>['Ukraine', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="L245" t="inlineStr">
@@ -18058,7 +18082,7 @@
       <c r="J246" t="inlineStr"/>
       <c r="K246" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Ukraine']</t>
+          <t>['Ukraine', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="L246" t="inlineStr">
@@ -18080,10 +18104,10 @@
         <v>0</v>
       </c>
       <c r="P246" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q246" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R246" t="inlineStr"/>
     </row>
@@ -18128,7 +18152,7 @@
       <c r="J247" t="inlineStr"/>
       <c r="K247" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Ukraine']</t>
+          <t>['Ukraine', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="L247" t="inlineStr">
@@ -18150,10 +18174,10 @@
         <v>0</v>
       </c>
       <c r="P247" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q247" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R247" t="inlineStr"/>
     </row>
@@ -18177,7 +18201,7 @@
         </is>
       </c>
       <c r="E248" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F248" t="n">
         <v>21</v>
@@ -18202,7 +18226,7 @@
       </c>
       <c r="K248" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="L248" t="inlineStr">
@@ -18221,10 +18245,10 @@
         </is>
       </c>
       <c r="O248" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P248" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q248" t="n">
         <v>2</v>
@@ -18251,7 +18275,7 @@
         </is>
       </c>
       <c r="E249" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F249" t="n">
         <v>24</v>
@@ -18276,7 +18300,7 @@
       </c>
       <c r="K249" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="L249" t="inlineStr">
@@ -18301,7 +18325,7 @@
         <v>3</v>
       </c>
       <c r="Q249" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R249" t="inlineStr"/>
     </row>
@@ -18325,7 +18349,7 @@
         </is>
       </c>
       <c r="E250" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F250" t="n">
         <v>50</v>
@@ -18350,7 +18374,7 @@
       </c>
       <c r="K250" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="L250" t="inlineStr">
@@ -18375,7 +18399,7 @@
         <v>3</v>
       </c>
       <c r="Q250" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R250" t="inlineStr"/>
     </row>
@@ -18399,7 +18423,7 @@
         </is>
       </c>
       <c r="E251" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F251" t="n">
         <v>58</v>
@@ -18424,7 +18448,7 @@
       </c>
       <c r="K251" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="L251" t="inlineStr">
@@ -18449,7 +18473,7 @@
         <v>3</v>
       </c>
       <c r="Q251" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R251" t="inlineStr"/>
     </row>
@@ -18484,7 +18508,7 @@
       <c r="J252" t="inlineStr"/>
       <c r="K252" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium']</t>
+          <t>['Finland', 'Belgium', 'Russia']</t>
         </is>
       </c>
       <c r="L252" t="inlineStr">
@@ -18554,7 +18578,7 @@
       <c r="J253" t="inlineStr"/>
       <c r="K253" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium']</t>
+          <t>['Finland', 'Belgium', 'Russia']</t>
         </is>
       </c>
       <c r="L253" t="inlineStr">
@@ -18576,10 +18600,10 @@
         <v>0</v>
       </c>
       <c r="P253" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q253" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R253" t="inlineStr"/>
     </row>
@@ -18603,7 +18627,7 @@
         </is>
       </c>
       <c r="E254" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F254" t="n">
         <v>38</v>
@@ -18628,7 +18652,7 @@
       </c>
       <c r="K254" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium']</t>
+          <t>['Finland', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="L254" t="inlineStr">
@@ -18647,13 +18671,13 @@
         </is>
       </c>
       <c r="O254" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P254" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q254" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R254" t="inlineStr"/>
     </row>
@@ -18677,7 +18701,7 @@
         </is>
       </c>
       <c r="E255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F255" t="n">
         <v>59</v>
@@ -18702,7 +18726,7 @@
       </c>
       <c r="K255" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium']</t>
+          <t>['Finland', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="L255" t="inlineStr">
@@ -18724,10 +18748,10 @@
         <v>0</v>
       </c>
       <c r="P255" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q255" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R255" t="inlineStr"/>
     </row>
@@ -18751,7 +18775,7 @@
         </is>
       </c>
       <c r="E256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F256" t="n">
         <v>70</v>
@@ -18776,7 +18800,7 @@
       </c>
       <c r="K256" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium']</t>
+          <t>['Finland', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="L256" t="inlineStr">
@@ -18798,10 +18822,10 @@
         <v>0</v>
       </c>
       <c r="P256" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q256" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R256" t="inlineStr"/>
     </row>
@@ -18825,7 +18849,7 @@
         </is>
       </c>
       <c r="E257" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F257" t="n">
         <v>74</v>
@@ -18850,7 +18874,7 @@
       </c>
       <c r="K257" t="inlineStr">
         <is>
-          <t>['Belgium', 'Denmark']</t>
+          <t>['Russia', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="L257" t="inlineStr">
@@ -18875,7 +18899,7 @@
         <v>0</v>
       </c>
       <c r="Q257" t="n">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="R257" t="inlineStr"/>
     </row>
@@ -18899,7 +18923,7 @@
         </is>
       </c>
       <c r="E258" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F258" t="n">
         <v>79</v>
@@ -18924,7 +18948,7 @@
       </c>
       <c r="K258" t="inlineStr">
         <is>
-          <t>['Belgium', 'Denmark']</t>
+          <t>['Finland', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="L258" t="inlineStr">
@@ -18943,13 +18967,13 @@
         </is>
       </c>
       <c r="O258" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P258" t="n">
         <v>0</v>
       </c>
       <c r="Q258" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R258" t="inlineStr"/>
     </row>
@@ -18973,7 +18997,7 @@
         </is>
       </c>
       <c r="E259" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F259" t="n">
         <v>81</v>
@@ -18998,7 +19022,7 @@
       </c>
       <c r="K259" t="inlineStr">
         <is>
-          <t>['Belgium', 'Denmark']</t>
+          <t>['Finland', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="L259" t="inlineStr">
@@ -19047,7 +19071,7 @@
         </is>
       </c>
       <c r="E260" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F260" t="n">
         <v>82</v>
@@ -19072,7 +19096,7 @@
       </c>
       <c r="K260" t="inlineStr">
         <is>
-          <t>['Belgium', 'Denmark']</t>
+          <t>['Finland', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="L260" t="inlineStr">
@@ -19132,7 +19156,7 @@
       <c r="J261" t="inlineStr"/>
       <c r="K261" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'England']</t>
+          <t>['Croatia', 'Czech Republic', 'England']</t>
         </is>
       </c>
       <c r="L261" t="inlineStr">
@@ -19202,7 +19226,7 @@
       <c r="J262" t="inlineStr"/>
       <c r="K262" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'England']</t>
+          <t>['Croatia', 'Czech Republic', 'England']</t>
         </is>
       </c>
       <c r="L262" t="inlineStr">
@@ -19224,10 +19248,10 @@
         <v>0</v>
       </c>
       <c r="P262" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q262" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R262" t="inlineStr"/>
     </row>
@@ -19276,7 +19300,7 @@
       </c>
       <c r="K263" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'England']</t>
+          <t>['Croatia', 'Czech Republic', 'England']</t>
         </is>
       </c>
       <c r="L263" t="inlineStr">
@@ -19298,10 +19322,10 @@
         <v>0</v>
       </c>
       <c r="P263" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q263" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R263" t="inlineStr"/>
     </row>
@@ -19350,7 +19374,7 @@
       </c>
       <c r="K264" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'England']</t>
+          <t>['Croatia', 'Czech Republic', 'England']</t>
         </is>
       </c>
       <c r="L264" t="inlineStr">
@@ -19372,10 +19396,10 @@
         <v>0</v>
       </c>
       <c r="P264" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q264" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R264" t="inlineStr"/>
     </row>
@@ -19424,7 +19448,7 @@
       </c>
       <c r="K265" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'England']</t>
+          <t>['Croatia', 'Czech Republic', 'England']</t>
         </is>
       </c>
       <c r="L265" t="inlineStr">
@@ -19446,10 +19470,10 @@
         <v>0</v>
       </c>
       <c r="P265" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q265" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R265" t="inlineStr"/>
     </row>
@@ -19498,7 +19522,7 @@
       </c>
       <c r="K266" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'England']</t>
+          <t>['Croatia', 'Czech Republic', 'England']</t>
         </is>
       </c>
       <c r="L266" t="inlineStr">
@@ -19520,10 +19544,10 @@
         <v>0</v>
       </c>
       <c r="P266" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q266" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R266" t="inlineStr"/>
     </row>
@@ -19547,7 +19571,7 @@
         </is>
       </c>
       <c r="E267" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F267" t="n">
         <v>77</v>
@@ -19572,7 +19596,7 @@
       </c>
       <c r="K267" t="inlineStr">
         <is>
-          <t>['Croatia', 'England']</t>
+          <t>['Croatia', 'Czech Republic', 'England']</t>
         </is>
       </c>
       <c r="L267" t="inlineStr">
@@ -19591,13 +19615,13 @@
         </is>
       </c>
       <c r="O267" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P267" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q267" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R267" t="inlineStr"/>
     </row>
@@ -19632,7 +19656,7 @@
       <c r="J268" t="inlineStr"/>
       <c r="K268" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="L268" t="inlineStr">
@@ -19702,7 +19726,7 @@
       <c r="J269" t="inlineStr"/>
       <c r="K269" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="L269" t="inlineStr">
@@ -19727,7 +19751,7 @@
         <v>1</v>
       </c>
       <c r="Q269" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R269" t="inlineStr"/>
     </row>
@@ -19776,7 +19800,7 @@
       </c>
       <c r="K270" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="L270" t="inlineStr">
@@ -19798,10 +19822,10 @@
         <v>0</v>
       </c>
       <c r="P270" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q270" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R270" t="inlineStr"/>
     </row>
@@ -19825,7 +19849,7 @@
         </is>
       </c>
       <c r="E271" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F271" t="n">
         <v>30</v>
@@ -19850,7 +19874,7 @@
       </c>
       <c r="K271" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="L271" t="inlineStr">
@@ -19869,13 +19893,13 @@
         </is>
       </c>
       <c r="O271" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P271" t="n">
         <v>2</v>
       </c>
       <c r="Q271" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R271" t="inlineStr"/>
     </row>
@@ -19899,7 +19923,7 @@
         </is>
       </c>
       <c r="E272" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F272" t="n">
         <v>48</v>
@@ -19924,7 +19948,7 @@
       </c>
       <c r="K272" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="L272" t="inlineStr">
@@ -19949,7 +19973,7 @@
         <v>2</v>
       </c>
       <c r="Q272" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R272" t="inlineStr"/>
     </row>
@@ -19973,7 +19997,7 @@
         </is>
       </c>
       <c r="E273" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F273" t="n">
         <v>56</v>
@@ -19998,7 +20022,7 @@
       </c>
       <c r="K273" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="L273" t="inlineStr">
@@ -20023,7 +20047,7 @@
         <v>2</v>
       </c>
       <c r="Q273" t="n">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="R273" t="inlineStr"/>
     </row>
@@ -20047,7 +20071,7 @@
         </is>
       </c>
       <c r="E274" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F274" t="n">
         <v>59</v>
@@ -20072,7 +20096,7 @@
       </c>
       <c r="K274" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="L274" t="inlineStr">
@@ -20097,7 +20121,7 @@
         <v>2</v>
       </c>
       <c r="Q274" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="R274" t="inlineStr"/>
     </row>
@@ -20121,7 +20145,7 @@
         </is>
       </c>
       <c r="E275" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F275" t="n">
         <v>61</v>
@@ -20146,7 +20170,7 @@
       </c>
       <c r="K275" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="L275" t="inlineStr">
@@ -20171,7 +20195,7 @@
         <v>2</v>
       </c>
       <c r="Q275" t="n">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="R275" t="inlineStr"/>
     </row>
@@ -20195,7 +20219,7 @@
         </is>
       </c>
       <c r="E276" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F276" t="n">
         <v>67</v>
@@ -20220,7 +20244,7 @@
       </c>
       <c r="K276" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="L276" t="inlineStr">
@@ -20245,7 +20269,7 @@
         <v>2</v>
       </c>
       <c r="Q276" t="n">
-        <v>8</v>
+        <v>-2</v>
       </c>
       <c r="R276" t="inlineStr"/>
     </row>
@@ -20269,7 +20293,7 @@
         </is>
       </c>
       <c r="E277" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F277" t="n">
         <v>71</v>
@@ -20294,7 +20318,7 @@
       </c>
       <c r="K277" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="L277" t="inlineStr">
@@ -20319,7 +20343,7 @@
         <v>2</v>
       </c>
       <c r="Q277" t="n">
-        <v>10</v>
+        <v>-3</v>
       </c>
       <c r="R277" t="inlineStr"/>
     </row>
@@ -20343,7 +20367,7 @@
         </is>
       </c>
       <c r="E278" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F278" t="n">
         <v>84</v>
@@ -20368,7 +20392,7 @@
       </c>
       <c r="K278" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="L278" t="inlineStr">
@@ -20390,10 +20414,10 @@
         <v>0</v>
       </c>
       <c r="P278" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q278" t="n">
-        <v>6</v>
+        <v>-4</v>
       </c>
       <c r="R278" t="inlineStr"/>
     </row>
@@ -20417,7 +20441,7 @@
         </is>
       </c>
       <c r="E279" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F279" t="n">
         <v>94</v>
@@ -20442,7 +20466,7 @@
       </c>
       <c r="K279" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="L279" t="inlineStr">
@@ -20467,7 +20491,7 @@
         <v>2</v>
       </c>
       <c r="Q279" t="n">
-        <v>10</v>
+        <v>-3</v>
       </c>
       <c r="R279" t="inlineStr"/>
     </row>
@@ -20502,7 +20526,7 @@
       <c r="J280" t="inlineStr"/>
       <c r="K280" t="inlineStr">
         <is>
-          <t>['Portugal', 'France']</t>
+          <t>['Portugal', 'France', 'Germany']</t>
         </is>
       </c>
       <c r="L280" t="inlineStr">
@@ -20551,7 +20575,7 @@
         </is>
       </c>
       <c r="E281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F281" t="n">
         <v>11</v>
@@ -20576,7 +20600,7 @@
       </c>
       <c r="K281" t="inlineStr">
         <is>
-          <t>['Portugal', 'France']</t>
+          <t>['Hungary', 'Portugal', 'France']</t>
         </is>
       </c>
       <c r="L281" t="inlineStr">
@@ -20595,13 +20619,13 @@
         </is>
       </c>
       <c r="O281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q281" t="n">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="R281" t="inlineStr"/>
     </row>
@@ -20625,7 +20649,7 @@
         </is>
       </c>
       <c r="E282" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F282" t="n">
         <v>31</v>
@@ -20650,7 +20674,7 @@
       </c>
       <c r="K282" t="inlineStr">
         <is>
-          <t>['France', 'Portugal']</t>
+          <t>['Hungary', 'Portugal', 'France']</t>
         </is>
       </c>
       <c r="L282" t="inlineStr">
@@ -20672,10 +20696,10 @@
         <v>0</v>
       </c>
       <c r="P282" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q282" t="n">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="R282" t="inlineStr"/>
     </row>
@@ -20699,7 +20723,7 @@
         </is>
       </c>
       <c r="E283" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F283" t="n">
         <v>47</v>
@@ -20724,7 +20748,7 @@
       </c>
       <c r="K283" t="inlineStr">
         <is>
-          <t>['Portugal', 'France']</t>
+          <t>['Hungary', 'Portugal', 'France']</t>
         </is>
       </c>
       <c r="L283" t="inlineStr">
@@ -20746,10 +20770,10 @@
         <v>0</v>
       </c>
       <c r="P283" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q283" t="n">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="R283" t="inlineStr"/>
     </row>
@@ -20798,7 +20822,7 @@
       </c>
       <c r="K284" t="inlineStr">
         <is>
-          <t>['France', 'Hungary']</t>
+          <t>['Hungary', 'Portugal', 'France']</t>
         </is>
       </c>
       <c r="L284" t="inlineStr">
@@ -20817,13 +20841,13 @@
         </is>
       </c>
       <c r="O284" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P284" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q284" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="R284" t="inlineStr"/>
     </row>
@@ -20847,7 +20871,7 @@
         </is>
       </c>
       <c r="E285" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F285" t="n">
         <v>60</v>
@@ -20872,7 +20896,7 @@
       </c>
       <c r="K285" t="inlineStr">
         <is>
-          <t>['Portugal', 'France']</t>
+          <t>['Hungary', 'Portugal', 'France']</t>
         </is>
       </c>
       <c r="L285" t="inlineStr">
@@ -20891,13 +20915,13 @@
         </is>
       </c>
       <c r="O285" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P285" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q285" t="n">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="R285" t="inlineStr"/>
     </row>
@@ -20946,7 +20970,7 @@
       </c>
       <c r="K286" t="inlineStr">
         <is>
-          <t>['Portugal', 'France']</t>
+          <t>['Portugal', 'France', 'Germany']</t>
         </is>
       </c>
       <c r="L286" t="inlineStr">
@@ -20965,13 +20989,13 @@
         </is>
       </c>
       <c r="O286" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P286" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q286" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R286" t="inlineStr"/>
     </row>
@@ -20995,7 +21019,7 @@
         </is>
       </c>
       <c r="E287" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F287" t="n">
         <v>68</v>
@@ -21020,7 +21044,7 @@
       </c>
       <c r="K287" t="inlineStr">
         <is>
-          <t>['Portugal', 'France']</t>
+          <t>['Hungary', 'Portugal', 'France']</t>
         </is>
       </c>
       <c r="L287" t="inlineStr">
@@ -21039,13 +21063,13 @@
         </is>
       </c>
       <c r="O287" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P287" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q287" t="n">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="R287" t="inlineStr"/>
     </row>
@@ -21069,7 +21093,7 @@
         </is>
       </c>
       <c r="E288" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F288" t="n">
         <v>84</v>
@@ -21094,7 +21118,7 @@
       </c>
       <c r="K288" t="inlineStr">
         <is>
-          <t>['Portugal', 'France']</t>
+          <t>['Portugal', 'France', 'Germany']</t>
         </is>
       </c>
       <c r="L288" t="inlineStr">
@@ -21113,13 +21137,13 @@
         </is>
       </c>
       <c r="O288" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P288" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q288" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R288" t="inlineStr"/>
     </row>
@@ -21154,7 +21178,7 @@
       <c r="J289" t="inlineStr"/>
       <c r="K289" t="inlineStr">
         <is>
-          <t>['Germany', 'Switzerland']</t>
+          <t>['Scotland', 'Switzerland', 'Germany']</t>
         </is>
       </c>
       <c r="L289" t="inlineStr">
@@ -21224,7 +21248,7 @@
       <c r="J290" t="inlineStr"/>
       <c r="K290" t="inlineStr">
         <is>
-          <t>['Germany', 'Switzerland']</t>
+          <t>['Scotland', 'Switzerland', 'Germany']</t>
         </is>
       </c>
       <c r="L290" t="inlineStr">
@@ -21246,10 +21270,10 @@
         <v>0</v>
       </c>
       <c r="P290" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q290" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="R290" t="inlineStr"/>
     </row>
@@ -21298,7 +21322,7 @@
       </c>
       <c r="K291" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Germany']</t>
+          <t>['Scotland', 'Switzerland', 'Germany']</t>
         </is>
       </c>
       <c r="L291" t="inlineStr">
@@ -21320,10 +21344,10 @@
         <v>0</v>
       </c>
       <c r="P291" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q291" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="R291" t="inlineStr"/>
     </row>
@@ -21372,7 +21396,7 @@
       </c>
       <c r="K292" t="inlineStr">
         <is>
-          <t>['Germany', 'Switzerland']</t>
+          <t>['Scotland', 'Switzerland', 'Germany']</t>
         </is>
       </c>
       <c r="L292" t="inlineStr">
@@ -21394,10 +21418,10 @@
         <v>0</v>
       </c>
       <c r="P292" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q292" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="R292" t="inlineStr"/>
     </row>
@@ -21421,7 +21445,7 @@
         </is>
       </c>
       <c r="E293" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F293" t="n">
         <v>100</v>
@@ -21446,7 +21470,7 @@
       </c>
       <c r="K293" t="inlineStr">
         <is>
-          <t>['Germany', 'Switzerland']</t>
+          <t>['Hungary', 'Switzerland', 'Germany']</t>
         </is>
       </c>
       <c r="L293" t="inlineStr">
@@ -21465,13 +21489,13 @@
         </is>
       </c>
       <c r="O293" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P293" t="n">
         <v>2</v>
       </c>
       <c r="Q293" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R293" t="inlineStr"/>
     </row>
@@ -21506,7 +21530,7 @@
       <c r="J294" t="inlineStr"/>
       <c r="K294" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Albania', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="L294" t="inlineStr">
@@ -21576,7 +21600,7 @@
       <c r="J295" t="inlineStr"/>
       <c r="K295" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Albania', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="L295" t="inlineStr">
@@ -21598,16 +21622,12 @@
         <v>0</v>
       </c>
       <c r="P295" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q295" t="n">
-        <v>1</v>
-      </c>
-      <c r="R295" t="inlineStr">
-        <is>
-          <t>Albania</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="R295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" t="n">
@@ -21629,7 +21649,7 @@
         </is>
       </c>
       <c r="E296" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F296" t="n">
         <v>13</v>
@@ -21654,7 +21674,7 @@
       </c>
       <c r="K296" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Spain', 'Croatia', 'Italy']</t>
         </is>
       </c>
       <c r="L296" t="inlineStr">
@@ -21673,13 +21693,13 @@
         </is>
       </c>
       <c r="O296" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P296" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q296" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="R296" t="inlineStr"/>
     </row>
@@ -21728,7 +21748,7 @@
       </c>
       <c r="K297" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Croatia', 'Italy']</t>
         </is>
       </c>
       <c r="L297" t="inlineStr">
@@ -21747,13 +21767,13 @@
         </is>
       </c>
       <c r="O297" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P297" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q297" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R297" t="inlineStr"/>
     </row>
@@ -21777,7 +21797,7 @@
         </is>
       </c>
       <c r="E298" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F298" t="n">
         <v>98</v>
@@ -21802,7 +21822,7 @@
       </c>
       <c r="K298" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Spain', 'Croatia', 'Italy']</t>
         </is>
       </c>
       <c r="L298" t="inlineStr">
@@ -21821,13 +21841,13 @@
         </is>
       </c>
       <c r="O298" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P298" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q298" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="R298" t="inlineStr"/>
     </row>
@@ -21862,7 +21882,7 @@
       <c r="J299" t="inlineStr"/>
       <c r="K299" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['Austria', 'France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L299" t="inlineStr">
@@ -21911,7 +21931,7 @@
         </is>
       </c>
       <c r="E300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F300" t="n">
         <v>6</v>
@@ -21936,7 +21956,7 @@
       </c>
       <c r="K300" t="inlineStr">
         <is>
-          <t>['Austria', 'France']</t>
+          <t>['France', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="L300" t="inlineStr">
@@ -21955,13 +21975,13 @@
         </is>
       </c>
       <c r="O300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P300" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q300" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R300" t="inlineStr"/>
     </row>
@@ -21985,7 +22005,7 @@
         </is>
       </c>
       <c r="E301" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F301" t="n">
         <v>47</v>
@@ -22010,7 +22030,7 @@
       </c>
       <c r="K301" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['Austria', 'France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L301" t="inlineStr">
@@ -22029,13 +22049,13 @@
         </is>
       </c>
       <c r="O301" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P301" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q301" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R301" t="inlineStr"/>
     </row>
@@ -22059,7 +22079,7 @@
         </is>
       </c>
       <c r="E302" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F302" t="n">
         <v>56</v>
@@ -22084,7 +22104,7 @@
       </c>
       <c r="K302" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['Austria', 'France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L302" t="inlineStr">
@@ -22106,10 +22126,10 @@
         <v>0</v>
       </c>
       <c r="P302" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q302" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R302" t="inlineStr"/>
     </row>
@@ -22133,7 +22153,7 @@
         </is>
       </c>
       <c r="E303" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F303" t="n">
         <v>59</v>
@@ -22158,7 +22178,7 @@
       </c>
       <c r="K303" t="inlineStr">
         <is>
-          <t>['Austria', 'France']</t>
+          <t>['Austria', 'France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L303" t="inlineStr">
@@ -22177,13 +22197,13 @@
         </is>
       </c>
       <c r="O303" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P303" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q303" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R303" t="inlineStr"/>
     </row>
@@ -22207,7 +22227,7 @@
         </is>
       </c>
       <c r="E304" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F304" t="n">
         <v>75</v>
@@ -22232,7 +22252,7 @@
       </c>
       <c r="K304" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['Austria', 'France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L304" t="inlineStr">
@@ -22251,13 +22271,13 @@
         </is>
       </c>
       <c r="O304" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P304" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q304" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R304" t="inlineStr"/>
     </row>
@@ -22281,7 +22301,7 @@
         </is>
       </c>
       <c r="E305" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F305" t="n">
         <v>79</v>
@@ -22306,7 +22326,7 @@
       </c>
       <c r="K305" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['Austria', 'France', 'Netherlands']</t>
         </is>
       </c>
       <c r="L305" t="inlineStr">
@@ -22328,10 +22348,10 @@
         <v>0</v>
       </c>
       <c r="P305" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q305" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R305" t="inlineStr"/>
     </row>
@@ -22355,7 +22375,7 @@
         </is>
       </c>
       <c r="E306" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F306" t="n">
         <v>80</v>
@@ -22380,7 +22400,7 @@
       </c>
       <c r="K306" t="inlineStr">
         <is>
-          <t>['Austria', 'France']</t>
+          <t>['France', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="L306" t="inlineStr">
@@ -22399,13 +22419,13 @@
         </is>
       </c>
       <c r="O306" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P306" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q306" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R306" t="inlineStr"/>
     </row>
@@ -22440,7 +22460,7 @@
       <c r="J307" t="inlineStr"/>
       <c r="K307" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England']</t>
+          <t>['Slovenia', 'Denmark', 'England']</t>
         </is>
       </c>
       <c r="L307" t="inlineStr">
@@ -22510,7 +22530,7 @@
       <c r="J308" t="inlineStr"/>
       <c r="K308" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England']</t>
+          <t>['Slovenia', 'Denmark', 'England']</t>
         </is>
       </c>
       <c r="L308" t="inlineStr">
@@ -22532,10 +22552,10 @@
         <v>0</v>
       </c>
       <c r="P308" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q308" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R308" t="inlineStr"/>
     </row>
@@ -22580,7 +22600,7 @@
       <c r="J309" t="inlineStr"/>
       <c r="K309" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England']</t>
+          <t>['Slovenia', 'Denmark', 'England']</t>
         </is>
       </c>
       <c r="L309" t="inlineStr">
@@ -22602,10 +22622,10 @@
         <v>0</v>
       </c>
       <c r="P309" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q309" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R309" t="inlineStr"/>
     </row>
@@ -22640,7 +22660,7 @@
       <c r="J310" t="inlineStr"/>
       <c r="K310" t="inlineStr">
         <is>
-          <t>['Belgium', 'Romania']</t>
+          <t>['Romania', 'Belgium', 'Slovakia']</t>
         </is>
       </c>
       <c r="L310" t="inlineStr">
@@ -22710,7 +22730,7 @@
       <c r="J311" t="inlineStr"/>
       <c r="K311" t="inlineStr">
         <is>
-          <t>['Belgium', 'Romania']</t>
+          <t>['Romania', 'Belgium', 'Slovakia']</t>
         </is>
       </c>
       <c r="L311" t="inlineStr">
@@ -22735,7 +22755,7 @@
         <v>0</v>
       </c>
       <c r="Q311" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R311" t="inlineStr"/>
     </row>
@@ -22784,7 +22804,7 @@
       </c>
       <c r="K312" t="inlineStr">
         <is>
-          <t>['Belgium', 'Slovakia']</t>
+          <t>['Ukraine', 'Belgium', 'Slovakia']</t>
         </is>
       </c>
       <c r="L312" t="inlineStr">
@@ -22806,10 +22826,10 @@
         <v>1</v>
       </c>
       <c r="P312" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q312" t="n">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="R312" t="inlineStr"/>
     </row>
@@ -22858,7 +22878,7 @@
       </c>
       <c r="K313" t="inlineStr">
         <is>
-          <t>['Belgium', 'Romania']</t>
+          <t>['Romania', 'Belgium', 'Slovakia']</t>
         </is>
       </c>
       <c r="L313" t="inlineStr">
@@ -22883,7 +22903,7 @@
         <v>0</v>
       </c>
       <c r="Q313" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R313" t="inlineStr"/>
     </row>
@@ -22918,7 +22938,7 @@
       <c r="J314" t="inlineStr"/>
       <c r="K314" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic', 'Turkey']</t>
         </is>
       </c>
       <c r="L314" t="inlineStr">
@@ -22988,7 +23008,7 @@
       <c r="J315" t="inlineStr"/>
       <c r="K315" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic', 'Turkey']</t>
         </is>
       </c>
       <c r="L315" t="inlineStr">
@@ -23010,16 +23030,12 @@
         <v>0</v>
       </c>
       <c r="P315" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q315" t="n">
-        <v>0</v>
-      </c>
-      <c r="R315" t="inlineStr">
-        <is>
-          <t>Czech Republic</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="R315" t="inlineStr"/>
     </row>
     <row r="316">
       <c r="A316" t="n">
@@ -23041,7 +23057,7 @@
         </is>
       </c>
       <c r="E316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F316" t="n">
         <v>2</v>
@@ -23066,7 +23082,7 @@
       </c>
       <c r="K316" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="L316" t="inlineStr">
@@ -23085,15 +23101,19 @@
         </is>
       </c>
       <c r="O316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P316" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q316" t="n">
         <v>0</v>
       </c>
-      <c r="R316" t="inlineStr"/>
+      <c r="R316" t="inlineStr">
+        <is>
+          <t>Czech Republic</t>
+        </is>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
@@ -23115,7 +23135,7 @@
         </is>
       </c>
       <c r="E317" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F317" t="n">
         <v>51</v>
@@ -23140,7 +23160,7 @@
       </c>
       <c r="K317" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="L317" t="inlineStr">
@@ -23162,7 +23182,7 @@
         <v>0</v>
       </c>
       <c r="P317" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q317" t="n">
         <v>1</v>
@@ -23189,7 +23209,7 @@
         </is>
       </c>
       <c r="E318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F318" t="n">
         <v>57</v>
@@ -23214,7 +23234,7 @@
       </c>
       <c r="K318" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="L318" t="inlineStr">
@@ -23236,10 +23256,10 @@
         <v>0</v>
       </c>
       <c r="P318" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q318" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R318" t="inlineStr"/>
     </row>
@@ -23288,7 +23308,7 @@
       </c>
       <c r="K319" t="inlineStr">
         <is>
-          <t>['Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="L319" t="inlineStr">
@@ -23307,15 +23327,19 @@
         </is>
       </c>
       <c r="O319" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P319" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q319" t="n">
-        <v>1</v>
-      </c>
-      <c r="R319" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="R319" t="inlineStr">
+        <is>
+          <t>Czech Republic</t>
+        </is>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
@@ -23337,7 +23361,7 @@
         </is>
       </c>
       <c r="E320" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F320" t="n">
         <v>94</v>
@@ -23362,7 +23386,7 @@
       </c>
       <c r="K320" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="L320" t="inlineStr">
@@ -23381,13 +23405,13 @@
         </is>
       </c>
       <c r="O320" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P320" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q320" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R320" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
stage in top third teams
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
+++ b/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -727,7 +727,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -815,7 +815,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -903,7 +903,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -991,7 +991,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1431,7 +1431,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -3147,7 +3147,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal']</t>
+          <t>['Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -3235,7 +3235,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal']</t>
+          <t>['Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -4505,7 +4505,7 @@
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4585,7 +4585,7 @@
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4663,7 +4663,7 @@
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4743,7 +4743,7 @@
       <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4835,7 +4835,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4927,7 +4927,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -5019,7 +5019,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -5111,7 +5111,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -5203,7 +5203,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -5295,7 +5295,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -5387,7 +5387,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -5479,7 +5479,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -5733,7 +5733,7 @@
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr">
         <is>
-          <t>['Sweden', 'France']</t>
+          <t>['France', 'Sweden']</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -5803,7 +5803,7 @@
       <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr">
         <is>
-          <t>['Sweden', 'France']</t>
+          <t>['France', 'Sweden']</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5887,7 +5887,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5975,7 +5975,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -6063,7 +6063,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -6151,7 +6151,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -6239,7 +6239,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -6327,7 +6327,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -6415,7 +6415,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>['Sweden', 'France']</t>
+          <t>['France', 'Sweden']</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -6503,7 +6503,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>['Sweden', 'France']</t>
+          <t>['France', 'Sweden']</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -9503,7 +9503,7 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>['Scotland', 'England']</t>
+          <t>['England', 'Scotland']</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
@@ -9591,7 +9591,7 @@
       </c>
       <c r="J107" t="inlineStr">
         <is>
-          <t>['Scotland', 'England']</t>
+          <t>['England', 'Scotland']</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
@@ -10171,7 +10171,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>['Spain', 'France']</t>
+          <t>['France', 'Spain']</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
@@ -10259,7 +10259,7 @@
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>['Spain', 'France']</t>
+          <t>['France', 'Spain']</t>
         </is>
       </c>
       <c r="K115" t="inlineStr">
@@ -10875,7 +10875,7 @@
       </c>
       <c r="J122" t="inlineStr">
         <is>
-          <t>['Spain', 'France']</t>
+          <t>['France', 'Spain']</t>
         </is>
       </c>
       <c r="K122" t="inlineStr">
@@ -10963,7 +10963,7 @@
       </c>
       <c r="J123" t="inlineStr">
         <is>
-          <t>['Spain', 'France']</t>
+          <t>['France', 'Spain']</t>
         </is>
       </c>
       <c r="K123" t="inlineStr">
@@ -11051,7 +11051,7 @@
       </c>
       <c r="J124" t="inlineStr">
         <is>
-          <t>['Spain', 'France']</t>
+          <t>['France', 'Spain']</t>
         </is>
       </c>
       <c r="K124" t="inlineStr">
@@ -11139,7 +11139,7 @@
       </c>
       <c r="J125" t="inlineStr">
         <is>
-          <t>['Spain', 'France']</t>
+          <t>['France', 'Spain']</t>
         </is>
       </c>
       <c r="K125" t="inlineStr">
@@ -14463,7 +14463,7 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>['Romania', 'Portugal']</t>
+          <t>['Portugal', 'Romania']</t>
         </is>
       </c>
       <c r="K164" t="inlineStr">
@@ -14551,7 +14551,7 @@
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>['Romania', 'Portugal']</t>
+          <t>['Portugal', 'Romania']</t>
         </is>
       </c>
       <c r="K165" t="inlineStr">
@@ -14639,7 +14639,7 @@
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>['Romania', 'Portugal']</t>
+          <t>['Portugal', 'Romania']</t>
         </is>
       </c>
       <c r="K166" t="inlineStr">
@@ -14727,7 +14727,7 @@
       </c>
       <c r="J167" t="inlineStr">
         <is>
-          <t>['Romania', 'Portugal']</t>
+          <t>['Portugal', 'Romania']</t>
         </is>
       </c>
       <c r="K167" t="inlineStr">
@@ -15727,7 +15727,7 @@
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>['Romania', 'Portugal']</t>
+          <t>['Portugal', 'Romania']</t>
         </is>
       </c>
       <c r="K178" t="inlineStr">
@@ -15815,7 +15815,7 @@
       </c>
       <c r="J179" t="inlineStr">
         <is>
-          <t>['Romania', 'Portugal']</t>
+          <t>['Portugal', 'Romania']</t>
         </is>
       </c>
       <c r="K179" t="inlineStr">
@@ -15889,7 +15889,7 @@
       <c r="I180" t="inlineStr"/>
       <c r="J180" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K180" t="inlineStr">
@@ -15969,7 +15969,7 @@
       <c r="I181" t="inlineStr"/>
       <c r="J181" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
@@ -16047,7 +16047,7 @@
       <c r="I182" t="inlineStr"/>
       <c r="J182" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K182" t="inlineStr">
@@ -16127,7 +16127,7 @@
       <c r="I183" t="inlineStr"/>
       <c r="J183" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K183" t="inlineStr">
@@ -16219,7 +16219,7 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
@@ -16311,7 +16311,7 @@
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K185" t="inlineStr">
@@ -18471,7 +18471,7 @@
       </c>
       <c r="J210" t="inlineStr">
         <is>
-          <t>['Spain', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Spain']</t>
         </is>
       </c>
       <c r="K210" t="inlineStr">
@@ -18559,7 +18559,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>['Spain', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Spain']</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
@@ -20173,7 +20173,7 @@
       <c r="I230" t="inlineStr"/>
       <c r="J230" t="inlineStr">
         <is>
-          <t>['Spain', 'Greece']</t>
+          <t>['Greece', 'Spain']</t>
         </is>
       </c>
       <c r="K230" t="inlineStr">
@@ -20253,7 +20253,7 @@
       <c r="I231" t="inlineStr"/>
       <c r="J231" t="inlineStr">
         <is>
-          <t>['Spain', 'Greece']</t>
+          <t>['Greece', 'Spain']</t>
         </is>
       </c>
       <c r="K231" t="inlineStr">
@@ -20327,7 +20327,7 @@
       <c r="I232" t="inlineStr"/>
       <c r="J232" t="inlineStr">
         <is>
-          <t>['Spain', 'Greece']</t>
+          <t>['Greece', 'Spain']</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
@@ -20407,7 +20407,7 @@
       <c r="I233" t="inlineStr"/>
       <c r="J233" t="inlineStr">
         <is>
-          <t>['Spain', 'Greece']</t>
+          <t>['Greece', 'Spain']</t>
         </is>
       </c>
       <c r="K233" t="inlineStr">
@@ -20495,7 +20495,7 @@
       </c>
       <c r="J234" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal']</t>
+          <t>['Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="K234" t="inlineStr">
@@ -20583,7 +20583,7 @@
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal']</t>
+          <t>['Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="K235" t="inlineStr">
@@ -20671,7 +20671,7 @@
       </c>
       <c r="J236" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal']</t>
+          <t>['Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="K236" t="inlineStr">
@@ -20759,7 +20759,7 @@
       </c>
       <c r="J237" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal']</t>
+          <t>['Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="K237" t="inlineStr">
@@ -20847,7 +20847,7 @@
       </c>
       <c r="J238" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal']</t>
+          <t>['Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="K238" t="inlineStr">
@@ -20935,7 +20935,7 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal']</t>
+          <t>['Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="K239" t="inlineStr">
@@ -21185,7 +21185,7 @@
       <c r="I242" t="inlineStr"/>
       <c r="J242" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K242" t="inlineStr">
@@ -21255,7 +21255,7 @@
       <c r="I243" t="inlineStr"/>
       <c r="J243" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K243" t="inlineStr">
@@ -21867,7 +21867,7 @@
       </c>
       <c r="J250" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K250" t="inlineStr">
@@ -21955,7 +21955,7 @@
       </c>
       <c r="J251" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K251" t="inlineStr">
@@ -22043,7 +22043,7 @@
       </c>
       <c r="J252" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K252" t="inlineStr">
@@ -22131,7 +22131,7 @@
       </c>
       <c r="J253" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K253" t="inlineStr">
@@ -22219,7 +22219,7 @@
       </c>
       <c r="J254" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K254" t="inlineStr">
@@ -22307,7 +22307,7 @@
       </c>
       <c r="J255" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K255" t="inlineStr">
@@ -22395,7 +22395,7 @@
       </c>
       <c r="J256" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K256" t="inlineStr">
@@ -22483,7 +22483,7 @@
       </c>
       <c r="J257" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K257" t="inlineStr">
@@ -22571,7 +22571,7 @@
       </c>
       <c r="J258" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K258" t="inlineStr">
@@ -22659,7 +22659,7 @@
       </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K259" t="inlineStr">
@@ -22747,7 +22747,7 @@
       </c>
       <c r="J260" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K260" t="inlineStr">
@@ -22835,7 +22835,7 @@
       </c>
       <c r="J261" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K261" t="inlineStr">
@@ -22923,7 +22923,7 @@
       </c>
       <c r="J262" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K262" t="inlineStr">
@@ -23011,7 +23011,7 @@
       </c>
       <c r="J263" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K263" t="inlineStr">
@@ -25131,7 +25131,7 @@
       </c>
       <c r="J288" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K288" t="inlineStr">
@@ -25219,7 +25219,7 @@
       </c>
       <c r="J289" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K289" t="inlineStr">
@@ -25307,7 +25307,7 @@
       </c>
       <c r="J290" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K290" t="inlineStr">
@@ -25395,7 +25395,7 @@
       </c>
       <c r="J291" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K291" t="inlineStr">
@@ -25483,7 +25483,7 @@
       </c>
       <c r="J292" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K292" t="inlineStr">
@@ -25571,7 +25571,7 @@
       </c>
       <c r="J293" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K293" t="inlineStr">
@@ -25659,7 +25659,7 @@
       </c>
       <c r="J294" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K294" t="inlineStr">
@@ -25747,7 +25747,7 @@
       </c>
       <c r="J295" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K295" t="inlineStr">
@@ -27199,7 +27199,7 @@
       </c>
       <c r="J312" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal']</t>
+          <t>['Portugal', 'Turkey']</t>
         </is>
       </c>
       <c r="K312" t="inlineStr">
@@ -27287,7 +27287,7 @@
       </c>
       <c r="J313" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal']</t>
+          <t>['Portugal', 'Turkey']</t>
         </is>
       </c>
       <c r="K313" t="inlineStr">
@@ -30557,7 +30557,7 @@
       <c r="I352" t="inlineStr"/>
       <c r="J352" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="K352" t="inlineStr">
@@ -30637,7 +30637,7 @@
       <c r="I353" t="inlineStr"/>
       <c r="J353" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="K353" t="inlineStr">
@@ -30721,7 +30721,7 @@
       <c r="I354" t="inlineStr"/>
       <c r="J354" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="K354" t="inlineStr">
@@ -30795,7 +30795,7 @@
       <c r="I355" t="inlineStr"/>
       <c r="J355" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="K355" t="inlineStr">
@@ -30875,7 +30875,7 @@
       <c r="I356" t="inlineStr"/>
       <c r="J356" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="K356" t="inlineStr">
@@ -30959,7 +30959,7 @@
       <c r="I357" t="inlineStr"/>
       <c r="J357" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="K357" t="inlineStr">
@@ -31047,7 +31047,7 @@
       </c>
       <c r="J358" t="inlineStr">
         <is>
-          <t>['Russia', 'Greece']</t>
+          <t>['Greece', 'Russia']</t>
         </is>
       </c>
       <c r="K358" t="inlineStr">
@@ -31135,7 +31135,7 @@
       </c>
       <c r="J359" t="inlineStr">
         <is>
-          <t>['Russia', 'Greece']</t>
+          <t>['Greece', 'Russia']</t>
         </is>
       </c>
       <c r="K359" t="inlineStr">
@@ -31223,7 +31223,7 @@
       </c>
       <c r="J360" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="K360" t="inlineStr">
@@ -31311,7 +31311,7 @@
       </c>
       <c r="J361" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="K361" t="inlineStr">
@@ -31385,7 +31385,7 @@
       <c r="I362" t="inlineStr"/>
       <c r="J362" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K362" t="inlineStr">
@@ -31455,7 +31455,7 @@
       <c r="I363" t="inlineStr"/>
       <c r="J363" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K363" t="inlineStr">
@@ -31715,7 +31715,7 @@
       </c>
       <c r="J366" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K366" t="inlineStr">
@@ -31803,7 +31803,7 @@
       </c>
       <c r="J367" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K367" t="inlineStr">
@@ -32067,7 +32067,7 @@
       </c>
       <c r="J370" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K370" t="inlineStr">
@@ -32155,7 +32155,7 @@
       </c>
       <c r="J371" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K371" t="inlineStr">
@@ -32243,7 +32243,7 @@
       </c>
       <c r="J372" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K372" t="inlineStr">
@@ -32335,7 +32335,7 @@
       </c>
       <c r="J373" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K373" t="inlineStr">
@@ -32427,7 +32427,7 @@
       </c>
       <c r="J374" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K374" t="inlineStr">
@@ -32515,7 +32515,7 @@
       </c>
       <c r="J375" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K375" t="inlineStr">
@@ -32589,7 +32589,7 @@
       <c r="I376" t="inlineStr"/>
       <c r="J376" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia']</t>
+          <t>['Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K376" t="inlineStr">
@@ -32669,7 +32669,7 @@
       <c r="I377" t="inlineStr"/>
       <c r="J377" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia']</t>
+          <t>['Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K377" t="inlineStr">
@@ -32753,7 +32753,7 @@
       <c r="I378" t="inlineStr"/>
       <c r="J378" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia']</t>
+          <t>['Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K378" t="inlineStr">
@@ -32827,7 +32827,7 @@
       <c r="I379" t="inlineStr"/>
       <c r="J379" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia']</t>
+          <t>['Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K379" t="inlineStr">
@@ -32907,7 +32907,7 @@
       <c r="I380" t="inlineStr"/>
       <c r="J380" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia']</t>
+          <t>['Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K380" t="inlineStr">
@@ -32991,7 +32991,7 @@
       <c r="I381" t="inlineStr"/>
       <c r="J381" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia']</t>
+          <t>['Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K381" t="inlineStr">
@@ -33079,7 +33079,7 @@
       </c>
       <c r="J382" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Italy', 'Spain']</t>
         </is>
       </c>
       <c r="K382" t="inlineStr">
@@ -33167,7 +33167,7 @@
       </c>
       <c r="J383" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Italy', 'Spain']</t>
         </is>
       </c>
       <c r="K383" t="inlineStr">
@@ -33255,7 +33255,7 @@
       </c>
       <c r="J384" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Italy', 'Spain']</t>
         </is>
       </c>
       <c r="K384" t="inlineStr">
@@ -33343,7 +33343,7 @@
       </c>
       <c r="J385" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Italy', 'Spain']</t>
         </is>
       </c>
       <c r="K385" t="inlineStr">
@@ -33431,7 +33431,7 @@
       </c>
       <c r="J386" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Italy', 'Spain']</t>
         </is>
       </c>
       <c r="K386" t="inlineStr">
@@ -33519,7 +33519,7 @@
       </c>
       <c r="J387" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Italy', 'Spain']</t>
         </is>
       </c>
       <c r="K387" t="inlineStr">
@@ -33593,7 +33593,7 @@
       <c r="I388" t="inlineStr"/>
       <c r="J388" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K388" t="inlineStr">
@@ -33673,7 +33673,7 @@
       <c r="I389" t="inlineStr"/>
       <c r="J389" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K389" t="inlineStr">
@@ -33757,7 +33757,7 @@
       <c r="I390" t="inlineStr"/>
       <c r="J390" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K390" t="inlineStr">
@@ -33831,7 +33831,7 @@
       <c r="I391" t="inlineStr"/>
       <c r="J391" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K391" t="inlineStr">
@@ -33911,7 +33911,7 @@
       <c r="I392" t="inlineStr"/>
       <c r="J392" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K392" t="inlineStr">
@@ -33995,7 +33995,7 @@
       <c r="I393" t="inlineStr"/>
       <c r="J393" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K393" t="inlineStr">
@@ -34083,7 +34083,7 @@
       </c>
       <c r="J394" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K394" t="inlineStr">
@@ -34171,7 +34171,7 @@
       </c>
       <c r="J395" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K395" t="inlineStr">
@@ -34259,7 +34259,7 @@
       </c>
       <c r="J396" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K396" t="inlineStr">
@@ -34347,7 +34347,7 @@
       </c>
       <c r="J397" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K397" t="inlineStr">
@@ -34435,7 +34435,7 @@
       </c>
       <c r="J398" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K398" t="inlineStr">
@@ -34523,7 +34523,7 @@
       </c>
       <c r="J399" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K399" t="inlineStr">
@@ -34597,7 +34597,7 @@
       <c r="I400" t="inlineStr"/>
       <c r="J400" t="inlineStr">
         <is>
-          <t>['Romania', 'France', 'Switzerland']</t>
+          <t>['Switzerland', 'Romania', 'France']</t>
         </is>
       </c>
       <c r="K400" t="inlineStr">
@@ -34677,7 +34677,7 @@
       <c r="I401" t="inlineStr"/>
       <c r="J401" t="inlineStr">
         <is>
-          <t>['Romania', 'France', 'Switzerland']</t>
+          <t>['Switzerland', 'Romania', 'France']</t>
         </is>
       </c>
       <c r="K401" t="inlineStr">
@@ -34761,7 +34761,7 @@
       <c r="I402" t="inlineStr"/>
       <c r="J402" t="inlineStr">
         <is>
-          <t>['Romania', 'France', 'Switzerland']</t>
+          <t>['Switzerland', 'Romania', 'France']</t>
         </is>
       </c>
       <c r="K402" t="inlineStr">
@@ -34849,7 +34849,7 @@
       </c>
       <c r="J403" t="inlineStr">
         <is>
-          <t>['Albania', 'France', 'Switzerland']</t>
+          <t>['Switzerland', 'France', 'Albania']</t>
         </is>
       </c>
       <c r="K403" t="inlineStr">
@@ -34923,7 +34923,7 @@
       <c r="I404" t="inlineStr"/>
       <c r="J404" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K404" t="inlineStr">
@@ -35003,7 +35003,7 @@
       <c r="I405" t="inlineStr"/>
       <c r="J405" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K405" t="inlineStr">
@@ -35091,7 +35091,7 @@
       <c r="I406" t="inlineStr"/>
       <c r="J406" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K406" t="inlineStr">
@@ -35169,7 +35169,7 @@
       <c r="I407" t="inlineStr"/>
       <c r="J407" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K407" t="inlineStr">
@@ -35249,7 +35249,7 @@
       <c r="I408" t="inlineStr"/>
       <c r="J408" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K408" t="inlineStr">
@@ -35337,7 +35337,7 @@
       <c r="I409" t="inlineStr"/>
       <c r="J409" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K409" t="inlineStr">
@@ -35429,7 +35429,7 @@
       </c>
       <c r="J410" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K410" t="inlineStr">
@@ -35517,7 +35517,7 @@
       </c>
       <c r="J411" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K411" t="inlineStr">
@@ -35605,7 +35605,7 @@
       </c>
       <c r="J412" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K412" t="inlineStr">
@@ -35693,7 +35693,7 @@
       </c>
       <c r="J413" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K413" t="inlineStr">
@@ -35781,7 +35781,7 @@
       </c>
       <c r="J414" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K414" t="inlineStr">
@@ -35869,7 +35869,7 @@
       </c>
       <c r="J415" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K415" t="inlineStr">
@@ -35943,7 +35943,7 @@
       <c r="I416" t="inlineStr"/>
       <c r="J416" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K416" t="inlineStr">
@@ -36023,7 +36023,7 @@
       <c r="I417" t="inlineStr"/>
       <c r="J417" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K417" t="inlineStr">
@@ -36107,7 +36107,7 @@
       <c r="I418" t="inlineStr"/>
       <c r="J418" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K418" t="inlineStr">
@@ -36181,7 +36181,7 @@
       <c r="I419" t="inlineStr"/>
       <c r="J419" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K419" t="inlineStr">
@@ -36261,7 +36261,7 @@
       <c r="I420" t="inlineStr"/>
       <c r="J420" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K420" t="inlineStr">
@@ -36345,7 +36345,7 @@
       <c r="I421" t="inlineStr"/>
       <c r="J421" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K421" t="inlineStr">
@@ -36433,7 +36433,7 @@
       </c>
       <c r="J422" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K422" t="inlineStr">
@@ -36521,7 +36521,7 @@
       </c>
       <c r="J423" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K423" t="inlineStr">
@@ -36609,7 +36609,7 @@
       </c>
       <c r="J424" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K424" t="inlineStr">
@@ -36697,7 +36697,7 @@
       </c>
       <c r="J425" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K425" t="inlineStr">
@@ -36771,7 +36771,7 @@
       <c r="I426" t="inlineStr"/>
       <c r="J426" t="inlineStr">
         <is>
-          <t>['Spain', 'Czech Republic', 'Croatia']</t>
+          <t>['Croatia', 'Spain', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K426" t="inlineStr">
@@ -36851,7 +36851,7 @@
       <c r="I427" t="inlineStr"/>
       <c r="J427" t="inlineStr">
         <is>
-          <t>['Spain', 'Czech Republic', 'Croatia']</t>
+          <t>['Croatia', 'Spain', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K427" t="inlineStr">
@@ -36925,7 +36925,7 @@
       <c r="I428" t="inlineStr"/>
       <c r="J428" t="inlineStr">
         <is>
-          <t>['Spain', 'Czech Republic', 'Croatia']</t>
+          <t>['Croatia', 'Spain', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K428" t="inlineStr">
@@ -37005,7 +37005,7 @@
       <c r="I429" t="inlineStr"/>
       <c r="J429" t="inlineStr">
         <is>
-          <t>['Spain', 'Czech Republic', 'Croatia']</t>
+          <t>['Croatia', 'Spain', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K429" t="inlineStr">
@@ -37093,7 +37093,7 @@
       </c>
       <c r="J430" t="inlineStr">
         <is>
-          <t>['Spain', 'Czech Republic', 'Croatia']</t>
+          <t>['Croatia', 'Spain', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K430" t="inlineStr">
@@ -37181,7 +37181,7 @@
       </c>
       <c r="J431" t="inlineStr">
         <is>
-          <t>['Spain', 'Czech Republic', 'Croatia']</t>
+          <t>['Croatia', 'Spain', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K431" t="inlineStr">
@@ -37269,7 +37269,7 @@
       </c>
       <c r="J432" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K432" t="inlineStr">
@@ -37357,7 +37357,7 @@
       </c>
       <c r="J433" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K433" t="inlineStr">
@@ -37445,7 +37445,7 @@
       </c>
       <c r="J434" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K434" t="inlineStr">
@@ -37533,7 +37533,7 @@
       </c>
       <c r="J435" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K435" t="inlineStr">
@@ -37621,7 +37621,7 @@
       </c>
       <c r="J436" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K436" t="inlineStr">
@@ -37709,7 +37709,7 @@
       </c>
       <c r="J437" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K437" t="inlineStr">
@@ -37797,7 +37797,7 @@
       </c>
       <c r="J438" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K438" t="inlineStr">
@@ -37885,7 +37885,7 @@
       </c>
       <c r="J439" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K439" t="inlineStr">
@@ -37959,7 +37959,7 @@
       <c r="I440" t="inlineStr"/>
       <c r="J440" t="inlineStr">
         <is>
-          <t>['Sweden', 'Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy', 'Sweden']</t>
         </is>
       </c>
       <c r="K440" t="inlineStr">
@@ -38039,7 +38039,7 @@
       <c r="I441" t="inlineStr"/>
       <c r="J441" t="inlineStr">
         <is>
-          <t>['Sweden', 'Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy', 'Sweden']</t>
         </is>
       </c>
       <c r="K441" t="inlineStr">
@@ -38123,7 +38123,7 @@
       <c r="I442" t="inlineStr"/>
       <c r="J442" t="inlineStr">
         <is>
-          <t>['Sweden', 'Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy', 'Sweden']</t>
         </is>
       </c>
       <c r="K442" t="inlineStr">
@@ -38197,7 +38197,7 @@
       <c r="I443" t="inlineStr"/>
       <c r="J443" t="inlineStr">
         <is>
-          <t>['Sweden', 'Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy', 'Sweden']</t>
         </is>
       </c>
       <c r="K443" t="inlineStr">
@@ -38277,7 +38277,7 @@
       <c r="I444" t="inlineStr"/>
       <c r="J444" t="inlineStr">
         <is>
-          <t>['Sweden', 'Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy', 'Sweden']</t>
         </is>
       </c>
       <c r="K444" t="inlineStr">
@@ -38361,7 +38361,7 @@
       <c r="I445" t="inlineStr"/>
       <c r="J445" t="inlineStr">
         <is>
-          <t>['Sweden', 'Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy', 'Sweden']</t>
         </is>
       </c>
       <c r="K445" t="inlineStr">
@@ -38449,7 +38449,7 @@
       </c>
       <c r="J446" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium', 'Ireland']</t>
+          <t>['Belgium', 'Ireland', 'Italy']</t>
         </is>
       </c>
       <c r="K446" t="inlineStr">
@@ -38537,7 +38537,7 @@
       </c>
       <c r="J447" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium', 'Ireland']</t>
+          <t>['Belgium', 'Ireland', 'Italy']</t>
         </is>
       </c>
       <c r="K447" t="inlineStr">
@@ -38625,7 +38625,7 @@
       </c>
       <c r="J448" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium', 'Ireland']</t>
+          <t>['Belgium', 'Ireland', 'Italy']</t>
         </is>
       </c>
       <c r="K448" t="inlineStr">
@@ -38713,7 +38713,7 @@
       </c>
       <c r="J449" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium', 'Ireland']</t>
+          <t>['Belgium', 'Ireland', 'Italy']</t>
         </is>
       </c>
       <c r="K449" t="inlineStr">
@@ -38787,7 +38787,7 @@
       <c r="I450" t="inlineStr"/>
       <c r="J450" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K450" t="inlineStr">
@@ -38857,7 +38857,7 @@
       <c r="I451" t="inlineStr"/>
       <c r="J451" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K451" t="inlineStr">
@@ -38941,7 +38941,7 @@
       </c>
       <c r="J452" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K452" t="inlineStr">
@@ -39029,7 +39029,7 @@
       </c>
       <c r="J453" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K453" t="inlineStr">
@@ -39117,7 +39117,7 @@
       </c>
       <c r="J454" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K454" t="inlineStr">
@@ -39205,7 +39205,7 @@
       </c>
       <c r="J455" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K455" t="inlineStr">
@@ -39293,7 +39293,7 @@
       </c>
       <c r="J456" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K456" t="inlineStr">
@@ -39381,7 +39381,7 @@
       </c>
       <c r="J457" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K457" t="inlineStr">
@@ -39469,7 +39469,7 @@
       </c>
       <c r="J458" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K458" t="inlineStr">
@@ -39557,7 +39557,7 @@
       </c>
       <c r="J459" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K459" t="inlineStr">
@@ -39645,7 +39645,7 @@
       </c>
       <c r="J460" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K460" t="inlineStr">
@@ -39733,7 +39733,7 @@
       </c>
       <c r="J461" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K461" t="inlineStr">
@@ -39821,7 +39821,7 @@
       </c>
       <c r="J462" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K462" t="inlineStr">
@@ -39909,7 +39909,7 @@
       </c>
       <c r="J463" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K463" t="inlineStr">
@@ -39997,7 +39997,7 @@
       </c>
       <c r="J464" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K464" t="inlineStr">
@@ -40085,7 +40085,7 @@
       </c>
       <c r="J465" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K465" t="inlineStr">
@@ -40173,7 +40173,7 @@
       </c>
       <c r="J466" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K466" t="inlineStr">
@@ -40261,7 +40261,7 @@
       </c>
       <c r="J467" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K467" t="inlineStr">
@@ -40349,7 +40349,7 @@
       </c>
       <c r="J468" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K468" t="inlineStr">
@@ -40437,7 +40437,7 @@
       </c>
       <c r="J469" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K469" t="inlineStr">
@@ -40511,7 +40511,7 @@
       <c r="I470" t="inlineStr"/>
       <c r="J470" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K470" t="inlineStr">
@@ -40591,7 +40591,7 @@
       <c r="I471" t="inlineStr"/>
       <c r="J471" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K471" t="inlineStr">
@@ -40665,7 +40665,7 @@
       <c r="I472" t="inlineStr"/>
       <c r="J472" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K472" t="inlineStr">
@@ -40745,7 +40745,7 @@
       <c r="I473" t="inlineStr"/>
       <c r="J473" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K473" t="inlineStr">
@@ -40819,7 +40819,7 @@
       <c r="I474" t="inlineStr"/>
       <c r="J474" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K474" t="inlineStr">
@@ -40899,7 +40899,7 @@
       <c r="I475" t="inlineStr"/>
       <c r="J475" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K475" t="inlineStr">
@@ -40987,7 +40987,7 @@
       </c>
       <c r="J476" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K476" t="inlineStr">
@@ -41075,7 +41075,7 @@
       </c>
       <c r="J477" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K477" t="inlineStr">
@@ -41163,7 +41163,7 @@
       </c>
       <c r="J478" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K478" t="inlineStr">
@@ -41251,7 +41251,7 @@
       </c>
       <c r="J479" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K479" t="inlineStr">
@@ -41339,7 +41339,7 @@
       </c>
       <c r="J480" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K480" t="inlineStr">
@@ -41427,7 +41427,7 @@
       </c>
       <c r="J481" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K481" t="inlineStr">
@@ -41515,7 +41515,7 @@
       </c>
       <c r="J482" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K482" t="inlineStr">
@@ -41603,7 +41603,7 @@
       </c>
       <c r="J483" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K483" t="inlineStr">
@@ -41691,7 +41691,7 @@
       </c>
       <c r="J484" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K484" t="inlineStr">
@@ -41779,7 +41779,7 @@
       </c>
       <c r="J485" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K485" t="inlineStr">
@@ -41867,7 +41867,7 @@
       </c>
       <c r="J486" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K486" t="inlineStr">
@@ -41955,7 +41955,7 @@
       </c>
       <c r="J487" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K487" t="inlineStr">
@@ -42043,7 +42043,7 @@
       </c>
       <c r="J488" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K488" t="inlineStr">
@@ -42131,7 +42131,7 @@
       </c>
       <c r="J489" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K489" t="inlineStr">
@@ -42219,7 +42219,7 @@
       </c>
       <c r="J490" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales', 'Switzerland']</t>
+          <t>['Wales', 'Italy', 'Switzerland']</t>
         </is>
       </c>
       <c r="K490" t="inlineStr">
@@ -42293,7 +42293,7 @@
       <c r="I491" t="inlineStr"/>
       <c r="J491" t="inlineStr">
         <is>
-          <t>['Russia', 'Finland', 'Belgium']</t>
+          <t>['Belgium', 'Russia', 'Finland']</t>
         </is>
       </c>
       <c r="K491" t="inlineStr">
@@ -42373,7 +42373,7 @@
       <c r="I492" t="inlineStr"/>
       <c r="J492" t="inlineStr">
         <is>
-          <t>['Russia', 'Finland', 'Belgium']</t>
+          <t>['Belgium', 'Russia', 'Finland']</t>
         </is>
       </c>
       <c r="K492" t="inlineStr">
@@ -42447,7 +42447,7 @@
       <c r="I493" t="inlineStr"/>
       <c r="J493" t="inlineStr">
         <is>
-          <t>['Russia', 'Finland', 'Belgium']</t>
+          <t>['Belgium', 'Russia', 'Finland']</t>
         </is>
       </c>
       <c r="K493" t="inlineStr">
@@ -42527,7 +42527,7 @@
       <c r="I494" t="inlineStr"/>
       <c r="J494" t="inlineStr">
         <is>
-          <t>['Russia', 'Finland', 'Belgium']</t>
+          <t>['Belgium', 'Russia', 'Finland']</t>
         </is>
       </c>
       <c r="K494" t="inlineStr">
@@ -42601,7 +42601,7 @@
       <c r="I495" t="inlineStr"/>
       <c r="J495" t="inlineStr">
         <is>
-          <t>['Russia', 'Finland', 'Belgium']</t>
+          <t>['Belgium', 'Russia', 'Finland']</t>
         </is>
       </c>
       <c r="K495" t="inlineStr">
@@ -42681,7 +42681,7 @@
       <c r="I496" t="inlineStr"/>
       <c r="J496" t="inlineStr">
         <is>
-          <t>['Russia', 'Finland', 'Belgium']</t>
+          <t>['Belgium', 'Russia', 'Finland']</t>
         </is>
       </c>
       <c r="K496" t="inlineStr">
@@ -42755,7 +42755,7 @@
       <c r="I497" t="inlineStr"/>
       <c r="J497" t="inlineStr">
         <is>
-          <t>['Russia', 'Finland', 'Belgium']</t>
+          <t>['Belgium', 'Russia', 'Finland']</t>
         </is>
       </c>
       <c r="K497" t="inlineStr">
@@ -42835,7 +42835,7 @@
       <c r="I498" t="inlineStr"/>
       <c r="J498" t="inlineStr">
         <is>
-          <t>['Russia', 'Finland', 'Belgium']</t>
+          <t>['Belgium', 'Russia', 'Finland']</t>
         </is>
       </c>
       <c r="K498" t="inlineStr">
@@ -42923,7 +42923,7 @@
       </c>
       <c r="J499" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K499" t="inlineStr">
@@ -43011,7 +43011,7 @@
       </c>
       <c r="J500" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K500" t="inlineStr">
@@ -43099,7 +43099,7 @@
       </c>
       <c r="J501" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K501" t="inlineStr">
@@ -43187,7 +43187,7 @@
       </c>
       <c r="J502" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K502" t="inlineStr">
@@ -43275,7 +43275,7 @@
       </c>
       <c r="J503" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K503" t="inlineStr">
@@ -43363,7 +43363,7 @@
       </c>
       <c r="J504" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K504" t="inlineStr">
@@ -43451,7 +43451,7 @@
       </c>
       <c r="J505" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K505" t="inlineStr">
@@ -43539,7 +43539,7 @@
       </c>
       <c r="J506" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K506" t="inlineStr">
@@ -43627,7 +43627,7 @@
       </c>
       <c r="J507" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K507" t="inlineStr">
@@ -43715,7 +43715,7 @@
       </c>
       <c r="J508" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K508" t="inlineStr">
@@ -43803,7 +43803,7 @@
       </c>
       <c r="J509" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K509" t="inlineStr">
@@ -43891,7 +43891,7 @@
       </c>
       <c r="J510" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K510" t="inlineStr">
@@ -43979,7 +43979,7 @@
       </c>
       <c r="J511" t="inlineStr">
         <is>
-          <t>['Russia', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Russia']</t>
         </is>
       </c>
       <c r="K511" t="inlineStr">
@@ -44067,7 +44067,7 @@
       </c>
       <c r="J512" t="inlineStr">
         <is>
-          <t>['Russia', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Russia']</t>
         </is>
       </c>
       <c r="K512" t="inlineStr">
@@ -44155,7 +44155,7 @@
       </c>
       <c r="J513" t="inlineStr">
         <is>
-          <t>['Russia', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Russia']</t>
         </is>
       </c>
       <c r="K513" t="inlineStr">
@@ -44243,7 +44243,7 @@
       </c>
       <c r="J514" t="inlineStr">
         <is>
-          <t>['Russia', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Russia']</t>
         </is>
       </c>
       <c r="K514" t="inlineStr">
@@ -44331,7 +44331,7 @@
       </c>
       <c r="J515" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K515" t="inlineStr">
@@ -44419,7 +44419,7 @@
       </c>
       <c r="J516" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K516" t="inlineStr">
@@ -44507,7 +44507,7 @@
       </c>
       <c r="J517" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K517" t="inlineStr">
@@ -44595,7 +44595,7 @@
       </c>
       <c r="J518" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K518" t="inlineStr">
@@ -44683,7 +44683,7 @@
       </c>
       <c r="J519" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K519" t="inlineStr">
@@ -44771,7 +44771,7 @@
       </c>
       <c r="J520" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K520" t="inlineStr">
@@ -44859,7 +44859,7 @@
       </c>
       <c r="J521" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K521" t="inlineStr">
@@ -44947,7 +44947,7 @@
       </c>
       <c r="J522" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K522" t="inlineStr">
@@ -45035,7 +45035,7 @@
       </c>
       <c r="J523" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K523" t="inlineStr">
@@ -45123,7 +45123,7 @@
       </c>
       <c r="J524" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K524" t="inlineStr">
@@ -45211,7 +45211,7 @@
       </c>
       <c r="J525" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K525" t="inlineStr">
@@ -45299,7 +45299,7 @@
       </c>
       <c r="J526" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Finland']</t>
         </is>
       </c>
       <c r="K526" t="inlineStr">
@@ -45373,7 +45373,7 @@
       <c r="I527" t="inlineStr"/>
       <c r="J527" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K527" t="inlineStr">
@@ -45453,7 +45453,7 @@
       <c r="I528" t="inlineStr"/>
       <c r="J528" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K528" t="inlineStr">
@@ -45527,7 +45527,7 @@
       <c r="I529" t="inlineStr"/>
       <c r="J529" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K529" t="inlineStr">
@@ -45607,7 +45607,7 @@
       <c r="I530" t="inlineStr"/>
       <c r="J530" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K530" t="inlineStr">
@@ -45681,7 +45681,7 @@
       <c r="I531" t="inlineStr"/>
       <c r="J531" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K531" t="inlineStr">
@@ -45761,7 +45761,7 @@
       <c r="I532" t="inlineStr"/>
       <c r="J532" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K532" t="inlineStr">
@@ -45845,7 +45845,7 @@
       <c r="I533" t="inlineStr"/>
       <c r="J533" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K533" t="inlineStr">
@@ -45929,7 +45929,7 @@
       <c r="I534" t="inlineStr"/>
       <c r="J534" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K534" t="inlineStr">
@@ -46013,7 +46013,7 @@
       <c r="I535" t="inlineStr"/>
       <c r="J535" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K535" t="inlineStr">
@@ -46101,7 +46101,7 @@
       </c>
       <c r="J536" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K536" t="inlineStr">
@@ -46189,7 +46189,7 @@
       </c>
       <c r="J537" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K537" t="inlineStr">
@@ -46277,7 +46277,7 @@
       </c>
       <c r="J538" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K538" t="inlineStr">
@@ -46365,7 +46365,7 @@
       </c>
       <c r="J539" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K539" t="inlineStr">
@@ -46453,7 +46453,7 @@
       </c>
       <c r="J540" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K540" t="inlineStr">
@@ -46541,7 +46541,7 @@
       </c>
       <c r="J541" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K541" t="inlineStr">
@@ -46629,7 +46629,7 @@
       </c>
       <c r="J542" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K542" t="inlineStr">
@@ -46717,7 +46717,7 @@
       </c>
       <c r="J543" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K543" t="inlineStr">
@@ -46805,7 +46805,7 @@
       </c>
       <c r="J544" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K544" t="inlineStr">
@@ -46893,7 +46893,7 @@
       </c>
       <c r="J545" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K545" t="inlineStr">
@@ -46981,7 +46981,7 @@
       </c>
       <c r="J546" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K546" t="inlineStr">
@@ -47069,7 +47069,7 @@
       </c>
       <c r="J547" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Austria', 'Netherlands']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K547" t="inlineStr">
@@ -47143,7 +47143,7 @@
       <c r="I548" t="inlineStr"/>
       <c r="J548" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K548" t="inlineStr">
@@ -47223,7 +47223,7 @@
       <c r="I549" t="inlineStr"/>
       <c r="J549" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K549" t="inlineStr">
@@ -47297,7 +47297,7 @@
       <c r="I550" t="inlineStr"/>
       <c r="J550" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K550" t="inlineStr">
@@ -47377,7 +47377,7 @@
       <c r="I551" t="inlineStr"/>
       <c r="J551" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K551" t="inlineStr">
@@ -47465,7 +47465,7 @@
       </c>
       <c r="J552" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K552" t="inlineStr">
@@ -47553,7 +47553,7 @@
       </c>
       <c r="J553" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K553" t="inlineStr">
@@ -47641,7 +47641,7 @@
       </c>
       <c r="J554" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K554" t="inlineStr">
@@ -47729,7 +47729,7 @@
       </c>
       <c r="J555" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K555" t="inlineStr">
@@ -47817,7 +47817,7 @@
       </c>
       <c r="J556" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K556" t="inlineStr">
@@ -47905,7 +47905,7 @@
       </c>
       <c r="J557" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K557" t="inlineStr">
@@ -47993,7 +47993,7 @@
       </c>
       <c r="J558" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K558" t="inlineStr">
@@ -48081,7 +48081,7 @@
       </c>
       <c r="J559" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K559" t="inlineStr">
@@ -48169,7 +48169,7 @@
       </c>
       <c r="J560" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K560" t="inlineStr">
@@ -48257,7 +48257,7 @@
       </c>
       <c r="J561" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K561" t="inlineStr">
@@ -48331,7 +48331,7 @@
       <c r="I562" t="inlineStr"/>
       <c r="J562" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K562" t="inlineStr">
@@ -48411,7 +48411,7 @@
       <c r="I563" t="inlineStr"/>
       <c r="J563" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K563" t="inlineStr">
@@ -48485,7 +48485,7 @@
       <c r="I564" t="inlineStr"/>
       <c r="J564" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K564" t="inlineStr">
@@ -48565,7 +48565,7 @@
       <c r="I565" t="inlineStr"/>
       <c r="J565" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K565" t="inlineStr">
@@ -48639,7 +48639,7 @@
       <c r="I566" t="inlineStr"/>
       <c r="J566" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K566" t="inlineStr">
@@ -48719,7 +48719,7 @@
       <c r="I567" t="inlineStr"/>
       <c r="J567" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K567" t="inlineStr">
@@ -48793,7 +48793,7 @@
       <c r="I568" t="inlineStr"/>
       <c r="J568" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K568" t="inlineStr">
@@ -48873,7 +48873,7 @@
       <c r="I569" t="inlineStr"/>
       <c r="J569" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K569" t="inlineStr">
@@ -48961,7 +48961,7 @@
       </c>
       <c r="J570" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K570" t="inlineStr">
@@ -49049,7 +49049,7 @@
       </c>
       <c r="J571" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K571" t="inlineStr">
@@ -49137,7 +49137,7 @@
       </c>
       <c r="J572" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K572" t="inlineStr">
@@ -49225,7 +49225,7 @@
       </c>
       <c r="J573" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K573" t="inlineStr">
@@ -49313,7 +49313,7 @@
       </c>
       <c r="J574" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K574" t="inlineStr">
@@ -49401,7 +49401,7 @@
       </c>
       <c r="J575" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K575" t="inlineStr">
@@ -49489,7 +49489,7 @@
       </c>
       <c r="J576" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K576" t="inlineStr">
@@ -49577,7 +49577,7 @@
       </c>
       <c r="J577" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K577" t="inlineStr">
@@ -49665,7 +49665,7 @@
       </c>
       <c r="J578" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K578" t="inlineStr">
@@ -49753,7 +49753,7 @@
       </c>
       <c r="J579" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K579" t="inlineStr">
@@ -49841,7 +49841,7 @@
       </c>
       <c r="J580" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K580" t="inlineStr">
@@ -49929,7 +49929,7 @@
       </c>
       <c r="J581" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K581" t="inlineStr">
@@ -50017,7 +50017,7 @@
       </c>
       <c r="J582" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K582" t="inlineStr">
@@ -50105,7 +50105,7 @@
       </c>
       <c r="J583" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K583" t="inlineStr">
@@ -50193,7 +50193,7 @@
       </c>
       <c r="J584" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K584" t="inlineStr">
@@ -50281,7 +50281,7 @@
       </c>
       <c r="J585" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K585" t="inlineStr">
@@ -50369,7 +50369,7 @@
       </c>
       <c r="J586" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K586" t="inlineStr">
@@ -50457,7 +50457,7 @@
       </c>
       <c r="J587" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K587" t="inlineStr">
@@ -50545,7 +50545,7 @@
       </c>
       <c r="J588" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K588" t="inlineStr">
@@ -50633,7 +50633,7 @@
       </c>
       <c r="J589" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K589" t="inlineStr">
@@ -50721,7 +50721,7 @@
       </c>
       <c r="J590" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K590" t="inlineStr">
@@ -50809,7 +50809,7 @@
       </c>
       <c r="J591" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K591" t="inlineStr">
@@ -50897,7 +50897,7 @@
       </c>
       <c r="J592" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K592" t="inlineStr">
@@ -50985,7 +50985,7 @@
       </c>
       <c r="J593" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K593" t="inlineStr">
@@ -51073,7 +51073,7 @@
       </c>
       <c r="J594" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K594" t="inlineStr">
@@ -51161,7 +51161,7 @@
       </c>
       <c r="J595" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K595" t="inlineStr">
@@ -51249,7 +51249,7 @@
       </c>
       <c r="J596" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K596" t="inlineStr">
@@ -51337,7 +51337,7 @@
       </c>
       <c r="J597" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K597" t="inlineStr">
@@ -51425,7 +51425,7 @@
       </c>
       <c r="J598" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K598" t="inlineStr">
@@ -51513,7 +51513,7 @@
       </c>
       <c r="J599" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K599" t="inlineStr">
@@ -51601,7 +51601,7 @@
       </c>
       <c r="J600" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K600" t="inlineStr">
@@ -51689,7 +51689,7 @@
       </c>
       <c r="J601" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K601" t="inlineStr">
@@ -51777,7 +51777,7 @@
       </c>
       <c r="J602" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K602" t="inlineStr">
@@ -51865,7 +51865,7 @@
       </c>
       <c r="J603" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K603" t="inlineStr">
@@ -51953,7 +51953,7 @@
       </c>
       <c r="J604" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K604" t="inlineStr">
@@ -52041,7 +52041,7 @@
       </c>
       <c r="J605" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K605" t="inlineStr">
@@ -52129,7 +52129,7 @@
       </c>
       <c r="J606" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K606" t="inlineStr">
@@ -52217,7 +52217,7 @@
       </c>
       <c r="J607" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K607" t="inlineStr">
@@ -52305,7 +52305,7 @@
       </c>
       <c r="J608" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K608" t="inlineStr">
@@ -52393,7 +52393,7 @@
       </c>
       <c r="J609" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K609" t="inlineStr">
@@ -52467,7 +52467,7 @@
       <c r="I610" t="inlineStr"/>
       <c r="J610" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal', 'France']</t>
+          <t>['Portugal', 'Germany', 'France']</t>
         </is>
       </c>
       <c r="K610" t="inlineStr">
@@ -52537,7 +52537,7 @@
       <c r="I611" t="inlineStr"/>
       <c r="J611" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal', 'France']</t>
+          <t>['Portugal', 'Germany', 'France']</t>
         </is>
       </c>
       <c r="K611" t="inlineStr">
@@ -52621,7 +52621,7 @@
       </c>
       <c r="J612" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K612" t="inlineStr">
@@ -52709,7 +52709,7 @@
       </c>
       <c r="J613" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K613" t="inlineStr">
@@ -52797,7 +52797,7 @@
       </c>
       <c r="J614" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K614" t="inlineStr">
@@ -52885,7 +52885,7 @@
       </c>
       <c r="J615" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K615" t="inlineStr">
@@ -52973,7 +52973,7 @@
       </c>
       <c r="J616" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K616" t="inlineStr">
@@ -53061,7 +53061,7 @@
       </c>
       <c r="J617" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K617" t="inlineStr">
@@ -53149,7 +53149,7 @@
       </c>
       <c r="J618" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K618" t="inlineStr">
@@ -53237,7 +53237,7 @@
       </c>
       <c r="J619" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K619" t="inlineStr">
@@ -53325,7 +53325,7 @@
       </c>
       <c r="J620" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K620" t="inlineStr">
@@ -53413,7 +53413,7 @@
       </c>
       <c r="J621" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K621" t="inlineStr">
@@ -53501,7 +53501,7 @@
       </c>
       <c r="J622" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal', 'France']</t>
+          <t>['Portugal', 'Germany', 'France']</t>
         </is>
       </c>
       <c r="K622" t="inlineStr">
@@ -53589,7 +53589,7 @@
       </c>
       <c r="J623" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal', 'France']</t>
+          <t>['Portugal', 'Germany', 'France']</t>
         </is>
       </c>
       <c r="K623" t="inlineStr">
@@ -53677,7 +53677,7 @@
       </c>
       <c r="J624" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K624" t="inlineStr">
@@ -53765,7 +53765,7 @@
       </c>
       <c r="J625" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K625" t="inlineStr">
@@ -53853,7 +53853,7 @@
       </c>
       <c r="J626" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal', 'France']</t>
+          <t>['Portugal', 'Germany', 'France']</t>
         </is>
       </c>
       <c r="K626" t="inlineStr">
@@ -53941,7 +53941,7 @@
       </c>
       <c r="J627" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal', 'France']</t>
+          <t>['Portugal', 'Germany', 'France']</t>
         </is>
       </c>
       <c r="K627" t="inlineStr">
@@ -54015,7 +54015,7 @@
       <c r="I628" t="inlineStr"/>
       <c r="J628" t="inlineStr">
         <is>
-          <t>['Germany', 'Scotland', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="K628" t="inlineStr">
@@ -54095,7 +54095,7 @@
       <c r="I629" t="inlineStr"/>
       <c r="J629" t="inlineStr">
         <is>
-          <t>['Germany', 'Scotland', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="K629" t="inlineStr">
@@ -54169,7 +54169,7 @@
       <c r="I630" t="inlineStr"/>
       <c r="J630" t="inlineStr">
         <is>
-          <t>['Germany', 'Scotland', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="K630" t="inlineStr">
@@ -54249,7 +54249,7 @@
       <c r="I631" t="inlineStr"/>
       <c r="J631" t="inlineStr">
         <is>
-          <t>['Germany', 'Scotland', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="K631" t="inlineStr">
@@ -54337,7 +54337,7 @@
       </c>
       <c r="J632" t="inlineStr">
         <is>
-          <t>['Germany', 'Scotland', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="K632" t="inlineStr">
@@ -54425,7 +54425,7 @@
       </c>
       <c r="J633" t="inlineStr">
         <is>
-          <t>['Germany', 'Scotland', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="K633" t="inlineStr">
@@ -54513,7 +54513,7 @@
       </c>
       <c r="J634" t="inlineStr">
         <is>
-          <t>['Germany', 'Scotland', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="K634" t="inlineStr">
@@ -54601,7 +54601,7 @@
       </c>
       <c r="J635" t="inlineStr">
         <is>
-          <t>['Germany', 'Scotland', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="K635" t="inlineStr">
@@ -54689,7 +54689,7 @@
       </c>
       <c r="J636" t="inlineStr">
         <is>
-          <t>['Germany', 'Hungary', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Hungary']</t>
         </is>
       </c>
       <c r="K636" t="inlineStr">
@@ -54777,7 +54777,7 @@
       </c>
       <c r="J637" t="inlineStr">
         <is>
-          <t>['Germany', 'Hungary', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Hungary']</t>
         </is>
       </c>
       <c r="K637" t="inlineStr">
@@ -54851,7 +54851,7 @@
       <c r="I638" t="inlineStr"/>
       <c r="J638" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy', 'Albania']</t>
+          <t>['Italy', 'Spain', 'Albania']</t>
         </is>
       </c>
       <c r="K638" t="inlineStr">
@@ -54931,7 +54931,7 @@
       <c r="I639" t="inlineStr"/>
       <c r="J639" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy', 'Albania']</t>
+          <t>['Italy', 'Spain', 'Albania']</t>
         </is>
       </c>
       <c r="K639" t="inlineStr">
@@ -55005,7 +55005,7 @@
       <c r="I640" t="inlineStr"/>
       <c r="J640" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy', 'Albania']</t>
+          <t>['Italy', 'Spain', 'Albania']</t>
         </is>
       </c>
       <c r="K640" t="inlineStr">
@@ -55085,7 +55085,7 @@
       <c r="I641" t="inlineStr"/>
       <c r="J641" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy', 'Albania']</t>
+          <t>['Italy', 'Spain', 'Albania']</t>
         </is>
       </c>
       <c r="K641" t="inlineStr">
@@ -55173,7 +55173,7 @@
       </c>
       <c r="J642" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy', 'Croatia']</t>
+          <t>['Croatia', 'Italy', 'Spain']</t>
         </is>
       </c>
       <c r="K642" t="inlineStr">
@@ -55261,7 +55261,7 @@
       </c>
       <c r="J643" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy', 'Croatia']</t>
+          <t>['Croatia', 'Italy', 'Spain']</t>
         </is>
       </c>
       <c r="K643" t="inlineStr">
@@ -55349,7 +55349,7 @@
       </c>
       <c r="J644" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy', 'Croatia']</t>
+          <t>['Croatia', 'Italy', 'Spain']</t>
         </is>
       </c>
       <c r="K644" t="inlineStr">
@@ -55437,7 +55437,7 @@
       </c>
       <c r="J645" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy', 'Croatia']</t>
+          <t>['Croatia', 'Italy', 'Spain']</t>
         </is>
       </c>
       <c r="K645" t="inlineStr">
@@ -55525,7 +55525,7 @@
       </c>
       <c r="J646" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy', 'Croatia']</t>
+          <t>['Croatia', 'Italy', 'Spain']</t>
         </is>
       </c>
       <c r="K646" t="inlineStr">
@@ -55613,7 +55613,7 @@
       </c>
       <c r="J647" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy', 'Croatia']</t>
+          <t>['Croatia', 'Italy', 'Spain']</t>
         </is>
       </c>
       <c r="K647" t="inlineStr">
@@ -55687,7 +55687,7 @@
       <c r="I648" t="inlineStr"/>
       <c r="J648" t="inlineStr">
         <is>
-          <t>['Denmark', 'Slovenia', 'England']</t>
+          <t>['Slovenia', 'England', 'Denmark']</t>
         </is>
       </c>
       <c r="K648" t="inlineStr">
@@ -55767,7 +55767,7 @@
       <c r="I649" t="inlineStr"/>
       <c r="J649" t="inlineStr">
         <is>
-          <t>['Denmark', 'Slovenia', 'England']</t>
+          <t>['Slovenia', 'England', 'Denmark']</t>
         </is>
       </c>
       <c r="K649" t="inlineStr">
@@ -55851,7 +55851,7 @@
       <c r="I650" t="inlineStr"/>
       <c r="J650" t="inlineStr">
         <is>
-          <t>['Denmark', 'Slovenia', 'England']</t>
+          <t>['Slovenia', 'England', 'Denmark']</t>
         </is>
       </c>
       <c r="K650" t="inlineStr">
@@ -55925,7 +55925,7 @@
       <c r="I651" t="inlineStr"/>
       <c r="J651" t="inlineStr">
         <is>
-          <t>['Austria', 'France', 'Netherlands']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K651" t="inlineStr">
@@ -55995,7 +55995,7 @@
       <c r="I652" t="inlineStr"/>
       <c r="J652" t="inlineStr">
         <is>
-          <t>['Austria', 'France', 'Netherlands']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K652" t="inlineStr">
@@ -56079,7 +56079,7 @@
       </c>
       <c r="J653" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K653" t="inlineStr">
@@ -56167,7 +56167,7 @@
       </c>
       <c r="J654" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K654" t="inlineStr">
@@ -56255,7 +56255,7 @@
       </c>
       <c r="J655" t="inlineStr">
         <is>
-          <t>['Austria', 'France', 'Netherlands']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K655" t="inlineStr">
@@ -56343,7 +56343,7 @@
       </c>
       <c r="J656" t="inlineStr">
         <is>
-          <t>['Austria', 'France', 'Netherlands']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K656" t="inlineStr">
@@ -56431,7 +56431,7 @@
       </c>
       <c r="J657" t="inlineStr">
         <is>
-          <t>['Austria', 'France', 'Netherlands']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K657" t="inlineStr">
@@ -56519,7 +56519,7 @@
       </c>
       <c r="J658" t="inlineStr">
         <is>
-          <t>['Austria', 'France', 'Netherlands']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K658" t="inlineStr">
@@ -56607,7 +56607,7 @@
       </c>
       <c r="J659" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K659" t="inlineStr">
@@ -56695,7 +56695,7 @@
       </c>
       <c r="J660" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K660" t="inlineStr">
@@ -56783,7 +56783,7 @@
       </c>
       <c r="J661" t="inlineStr">
         <is>
-          <t>['Austria', 'France', 'Netherlands']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K661" t="inlineStr">
@@ -56871,7 +56871,7 @@
       </c>
       <c r="J662" t="inlineStr">
         <is>
-          <t>['Austria', 'France', 'Netherlands']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K662" t="inlineStr">
@@ -56959,7 +56959,7 @@
       </c>
       <c r="J663" t="inlineStr">
         <is>
-          <t>['Austria', 'France', 'Netherlands']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K663" t="inlineStr">
@@ -57047,7 +57047,7 @@
       </c>
       <c r="J664" t="inlineStr">
         <is>
-          <t>['Austria', 'France', 'Netherlands']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K664" t="inlineStr">
@@ -57135,7 +57135,7 @@
       </c>
       <c r="J665" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K665" t="inlineStr">
@@ -57223,7 +57223,7 @@
       </c>
       <c r="J666" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K666" t="inlineStr">
@@ -57297,7 +57297,7 @@
       <c r="I667" t="inlineStr"/>
       <c r="J667" t="inlineStr">
         <is>
-          <t>['Romania', 'Belgium', 'Slovakia']</t>
+          <t>['Belgium', 'Romania', 'Slovakia']</t>
         </is>
       </c>
       <c r="K667" t="inlineStr">
@@ -57377,7 +57377,7 @@
       <c r="I668" t="inlineStr"/>
       <c r="J668" t="inlineStr">
         <is>
-          <t>['Romania', 'Belgium', 'Slovakia']</t>
+          <t>['Belgium', 'Romania', 'Slovakia']</t>
         </is>
       </c>
       <c r="K668" t="inlineStr">
@@ -57465,7 +57465,7 @@
       </c>
       <c r="J669" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Slovakia', 'Belgium']</t>
+          <t>['Ukraine', 'Belgium', 'Slovakia']</t>
         </is>
       </c>
       <c r="K669" t="inlineStr">
@@ -57553,7 +57553,7 @@
       </c>
       <c r="J670" t="inlineStr">
         <is>
-          <t>['Romania', 'Belgium', 'Slovakia']</t>
+          <t>['Belgium', 'Romania', 'Slovakia']</t>
         </is>
       </c>
       <c r="K670" t="inlineStr">
@@ -57627,7 +57627,7 @@
       <c r="I671" t="inlineStr"/>
       <c r="J671" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Czech Republic']</t>
+          <t>['Portugal', 'Turkey', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K671" t="inlineStr">
@@ -57707,7 +57707,7 @@
       <c r="I672" t="inlineStr"/>
       <c r="J672" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Czech Republic']</t>
+          <t>['Portugal', 'Turkey', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K672" t="inlineStr">
@@ -57781,7 +57781,7 @@
       <c r="I673" t="inlineStr"/>
       <c r="J673" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Czech Republic']</t>
+          <t>['Portugal', 'Turkey', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K673" t="inlineStr">
@@ -57861,7 +57861,7 @@
       <c r="I674" t="inlineStr"/>
       <c r="J674" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Czech Republic']</t>
+          <t>['Portugal', 'Turkey', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K674" t="inlineStr">
@@ -57949,7 +57949,7 @@
       </c>
       <c r="J675" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K675" t="inlineStr">
@@ -58041,7 +58041,7 @@
       </c>
       <c r="J676" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K676" t="inlineStr">
@@ -58133,7 +58133,7 @@
       </c>
       <c r="J677" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K677" t="inlineStr">
@@ -58221,7 +58221,7 @@
       </c>
       <c r="J678" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K678" t="inlineStr">
@@ -58309,7 +58309,7 @@
       </c>
       <c r="J679" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K679" t="inlineStr">
@@ -58397,7 +58397,7 @@
       </c>
       <c r="J680" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K680" t="inlineStr">
@@ -58485,7 +58485,7 @@
       </c>
       <c r="J681" t="inlineStr">
         <is>
-          <t>['Georgia', 'Portugal', 'Turkey']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K681" t="inlineStr">
@@ -58577,7 +58577,7 @@
       </c>
       <c r="J682" t="inlineStr">
         <is>
-          <t>['Georgia', 'Portugal', 'Turkey']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K682" t="inlineStr">
@@ -58669,7 +58669,7 @@
       </c>
       <c r="J683" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K683" t="inlineStr">
@@ -58757,7 +58757,7 @@
       </c>
       <c r="J684" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K684" t="inlineStr">

</xml_diff>

<commit_message>
third team goal minute 0
Now, at goal minute zero, when a team starts playing the last gameday one point is added for the current draw
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
+++ b/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
@@ -1995,7 +1995,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t>['West Germany', 'Spain']</t>
+          <t>['Spain', 'West Germany']</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -2091,7 +2091,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>['Portugal', 'West Germany']</t>
+          <t>['West Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -3535,7 +3535,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Netherlands']</t>
+          <t>['Netherlands', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -4499,7 +4499,7 @@
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany']</t>
+          <t>['Germany', 'Netherlands']</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -4595,7 +4595,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -4723,7 +4723,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -4851,7 +4851,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -4979,7 +4979,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -5107,7 +5107,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -5235,7 +5235,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -5363,7 +5363,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -6455,7 +6455,7 @@
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -6551,7 +6551,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -6679,7 +6679,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -6807,7 +6807,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -6935,7 +6935,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -7063,7 +7063,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>['England', 'Scotland']</t>
+          <t>['Scotland', 'England']</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -7191,7 +7191,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -7305,7 +7305,7 @@
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -7401,7 +7401,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -7529,7 +7529,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -7657,7 +7657,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -7785,7 +7785,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -7913,7 +7913,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -8041,7 +8041,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -8251,7 +8251,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -8379,7 +8379,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -8507,7 +8507,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -9823,7 +9823,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>['Portugal', 'Romania']</t>
+          <t>['Romania', 'Portugal']</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -9951,7 +9951,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>['Portugal', 'Romania']</t>
+          <t>['Romania', 'Portugal']</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -10719,7 +10719,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>['Portugal', 'Romania']</t>
+          <t>['Romania', 'Portugal']</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -10833,7 +10833,7 @@
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr">
         <is>
-          <t>['Yugoslavia', 'Spain']</t>
+          <t>['Spain', 'Yugoslavia']</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -10929,7 +10929,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>['Yugoslavia', 'Norway']</t>
+          <t>['Norway', 'Yugoslavia']</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -11057,7 +11057,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>['Yugoslavia', 'Spain']</t>
+          <t>['Spain', 'Yugoslavia']</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -11185,7 +11185,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>['Yugoslavia', 'Norway']</t>
+          <t>['Norway', 'Yugoslavia']</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
@@ -11313,7 +11313,7 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>['Yugoslavia', 'Spain']</t>
+          <t>['Spain', 'Yugoslavia']</t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
@@ -11441,7 +11441,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>['Yugoslavia', 'Norway']</t>
+          <t>['Norway', 'Yugoslavia']</t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
@@ -11569,7 +11569,7 @@
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>['Yugoslavia', 'Spain']</t>
+          <t>['Spain', 'Yugoslavia']</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
@@ -11697,7 +11697,7 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>['Yugoslavia', 'Spain']</t>
+          <t>['Spain', 'Yugoslavia']</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
@@ -12419,7 +12419,7 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K99" t="inlineStr">
@@ -12547,7 +12547,7 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">
@@ -12675,7 +12675,7 @@
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K101" t="inlineStr">
@@ -12885,7 +12885,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -13013,7 +13013,7 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
@@ -13141,7 +13141,7 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
@@ -13269,7 +13269,7 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>['Portugal', 'Greece']</t>
+          <t>['Greece', 'Portugal']</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
@@ -13383,7 +13383,7 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
@@ -13863,7 +13863,7 @@
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K111" t="inlineStr">
@@ -13991,7 +13991,7 @@
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K112" t="inlineStr">
@@ -14119,7 +14119,7 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K113" t="inlineStr">
@@ -14247,7 +14247,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
@@ -14375,7 +14375,7 @@
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K115" t="inlineStr">
@@ -14503,7 +14503,7 @@
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K116" t="inlineStr">
@@ -14631,7 +14631,7 @@
       </c>
       <c r="J117" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K117" t="inlineStr">
@@ -15723,7 +15723,7 @@
       <c r="I126" t="inlineStr"/>
       <c r="J126" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K126" t="inlineStr">
@@ -15819,7 +15819,7 @@
       </c>
       <c r="J127" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K127" t="inlineStr">
@@ -15947,7 +15947,7 @@
       </c>
       <c r="J128" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K128" t="inlineStr">
@@ -16075,7 +16075,7 @@
       </c>
       <c r="J129" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K129" t="inlineStr">
@@ -16203,7 +16203,7 @@
       </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K130" t="inlineStr">
@@ -16331,7 +16331,7 @@
       </c>
       <c r="J131" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K131" t="inlineStr">
@@ -16459,7 +16459,7 @@
       </c>
       <c r="J132" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K132" t="inlineStr">
@@ -17437,7 +17437,7 @@
       </c>
       <c r="J140" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey']</t>
+          <t>['Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K140" t="inlineStr">
@@ -18579,7 +18579,7 @@
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="K150" t="inlineStr">
@@ -18707,7 +18707,7 @@
       </c>
       <c r="J151" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="K151" t="inlineStr">
@@ -18835,7 +18835,7 @@
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="K152" t="inlineStr">
@@ -18963,7 +18963,7 @@
       </c>
       <c r="J153" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="K153" t="inlineStr">
@@ -19091,7 +19091,7 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="K154" t="inlineStr">
@@ -19205,7 +19205,7 @@
       <c r="I155" t="inlineStr"/>
       <c r="J155" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Russia']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
@@ -19301,7 +19301,7 @@
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>['Greece', 'Russia']</t>
+          <t>['Russia', 'Greece']</t>
         </is>
       </c>
       <c r="K156" t="inlineStr">
@@ -19429,7 +19429,7 @@
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Russia']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K157" t="inlineStr">
@@ -19543,7 +19543,7 @@
       <c r="I158" t="inlineStr"/>
       <c r="J158" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany']</t>
+          <t>['Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K158" t="inlineStr">
@@ -19639,7 +19639,7 @@
       </c>
       <c r="J159" t="inlineStr">
         <is>
-          <t>['Denmark', 'Germany']</t>
+          <t>['Germany', 'Denmark']</t>
         </is>
       </c>
       <c r="K159" t="inlineStr">
@@ -19767,7 +19767,7 @@
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany']</t>
+          <t>['Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K160" t="inlineStr">
@@ -19895,7 +19895,7 @@
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>['Denmark', 'Germany']</t>
+          <t>['Germany', 'Denmark']</t>
         </is>
       </c>
       <c r="K161" t="inlineStr">
@@ -20023,7 +20023,7 @@
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany']</t>
+          <t>['Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K162" t="inlineStr">
@@ -20151,7 +20151,7 @@
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany']</t>
+          <t>['Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K163" t="inlineStr">
@@ -20279,7 +20279,7 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany']</t>
+          <t>['Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K164" t="inlineStr">
@@ -20859,7 +20859,7 @@
       <c r="I169" t="inlineStr"/>
       <c r="J169" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K169" t="inlineStr">
@@ -20955,7 +20955,7 @@
       </c>
       <c r="J170" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K170" t="inlineStr">
@@ -21083,7 +21083,7 @@
       </c>
       <c r="J171" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K171" t="inlineStr">
@@ -21211,7 +21211,7 @@
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K172" t="inlineStr">
@@ -21325,7 +21325,7 @@
       <c r="I173" t="inlineStr"/>
       <c r="J173" t="inlineStr">
         <is>
-          <t>['France', 'Switzerland', 'Romania']</t>
+          <t>['France', 'Romania', 'Switzerland']</t>
         </is>
       </c>
       <c r="K173" t="inlineStr">
@@ -21535,7 +21535,7 @@
       <c r="I175" t="inlineStr"/>
       <c r="J175" t="inlineStr">
         <is>
-          <t>['England', 'Wales', 'Slovakia']</t>
+          <t>['Slovakia', 'Wales', 'England']</t>
         </is>
       </c>
       <c r="K175" t="inlineStr">
@@ -21631,7 +21631,7 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>['England', 'Wales', 'Slovakia']</t>
+          <t>['Slovakia', 'England', 'Wales']</t>
         </is>
       </c>
       <c r="K176" t="inlineStr">
@@ -21759,7 +21759,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>['England', 'Wales', 'Slovakia']</t>
+          <t>['Slovakia', 'England', 'Wales']</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -21887,7 +21887,7 @@
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>['England', 'Wales', 'Slovakia']</t>
+          <t>['Slovakia', 'England', 'Wales']</t>
         </is>
       </c>
       <c r="K178" t="inlineStr">
@@ -22001,7 +22001,7 @@
       <c r="I179" t="inlineStr"/>
       <c r="J179" t="inlineStr">
         <is>
-          <t>['Poland', 'Germany', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K179" t="inlineStr">
@@ -22097,7 +22097,7 @@
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>['Poland', 'Germany', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K180" t="inlineStr">
@@ -22225,7 +22225,7 @@
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>['Poland', 'Germany', 'Northern Ireland']</t>
+          <t>['Germany', 'Northern Ireland', 'Poland']</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
@@ -22375,11 +22375,11 @@
       <c r="Y182" t="inlineStr"/>
       <c r="Z182" t="inlineStr"/>
       <c r="AA182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB182" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia']</t>
+          <t>['Spain', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="AC182" t="n">
@@ -22503,10 +22503,10 @@
         </is>
       </c>
       <c r="AC183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE183" t="n">
         <v>-2</v>
@@ -22563,7 +22563,7 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
@@ -22634,7 +22634,7 @@
         <v>1</v>
       </c>
       <c r="AD184" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE184" t="n">
         <v>-2</v>
@@ -22691,7 +22691,7 @@
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K185" t="inlineStr">
@@ -22762,7 +22762,7 @@
         <v>0</v>
       </c>
       <c r="AD185" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE185" t="n">
         <v>-2</v>
@@ -22819,7 +22819,7 @@
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K186" t="inlineStr">
@@ -22890,7 +22890,7 @@
         <v>0</v>
       </c>
       <c r="AD186" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE186" t="n">
         <v>-2</v>
@@ -22947,7 +22947,7 @@
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K187" t="inlineStr">
@@ -23018,7 +23018,7 @@
         <v>0</v>
       </c>
       <c r="AD187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE187" t="n">
         <v>-2</v>
@@ -23061,7 +23061,7 @@
       <c r="I188" t="inlineStr"/>
       <c r="J188" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Iceland', 'Portugal']</t>
         </is>
       </c>
       <c r="K188" t="inlineStr">
@@ -23097,11 +23097,11 @@
       <c r="Y188" t="inlineStr"/>
       <c r="Z188" t="inlineStr"/>
       <c r="AA188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB188" t="inlineStr">
         <is>
-          <t>['Hungary', 'Iceland']</t>
+          <t>['Hungary', 'Iceland', 'Portugal']</t>
         </is>
       </c>
       <c r="AC188" t="n">
@@ -23157,7 +23157,7 @@
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Iceland', 'Portugal']</t>
         </is>
       </c>
       <c r="K189" t="inlineStr">
@@ -23225,10 +23225,10 @@
         </is>
       </c>
       <c r="AC189" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD189" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE189" t="n">
         <v>-2</v>
@@ -23285,7 +23285,7 @@
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Iceland', 'Portugal']</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
@@ -23356,7 +23356,7 @@
         <v>1</v>
       </c>
       <c r="AD190" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE190" t="n">
         <v>-3</v>
@@ -23413,7 +23413,7 @@
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Iceland', 'Portugal']</t>
         </is>
       </c>
       <c r="K191" t="inlineStr">
@@ -23484,7 +23484,7 @@
         <v>1</v>
       </c>
       <c r="AD191" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE191" t="n">
         <v>-2</v>
@@ -23541,7 +23541,7 @@
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Iceland', 'Portugal']</t>
         </is>
       </c>
       <c r="K192" t="inlineStr">
@@ -23612,7 +23612,7 @@
         <v>1</v>
       </c>
       <c r="AD192" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE192" t="n">
         <v>-3</v>
@@ -23669,7 +23669,7 @@
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Iceland', 'Portugal']</t>
         </is>
       </c>
       <c r="K193" t="inlineStr">
@@ -23740,7 +23740,7 @@
         <v>1</v>
       </c>
       <c r="AD193" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE193" t="n">
         <v>-2</v>
@@ -23797,7 +23797,7 @@
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Iceland', 'Portugal']</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
@@ -23868,7 +23868,7 @@
         <v>1</v>
       </c>
       <c r="AD194" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AE194" t="n">
         <v>-3</v>
@@ -23925,7 +23925,7 @@
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Iceland', 'Portugal']</t>
         </is>
       </c>
       <c r="K195" t="inlineStr">
@@ -23996,7 +23996,7 @@
         <v>0</v>
       </c>
       <c r="AD195" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AE195" t="n">
         <v>-1</v>
@@ -24053,7 +24053,7 @@
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Iceland', 'Portugal']</t>
         </is>
       </c>
       <c r="K196" t="inlineStr">
@@ -24124,7 +24124,7 @@
         <v>1</v>
       </c>
       <c r="AD196" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE196" t="n">
         <v>-1</v>
@@ -24181,7 +24181,7 @@
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Hungary', 'Iceland', 'Portugal']</t>
         </is>
       </c>
       <c r="K197" t="inlineStr">
@@ -24252,7 +24252,7 @@
         <v>0</v>
       </c>
       <c r="AD197" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE197" t="n">
         <v>-2</v>
@@ -24295,7 +24295,7 @@
       <c r="I198" t="inlineStr"/>
       <c r="J198" t="inlineStr">
         <is>
-          <t>['Sweden', 'Belgium', 'Italy']</t>
+          <t>['Belgium', 'Italy', 'Sweden']</t>
         </is>
       </c>
       <c r="K198" t="inlineStr">
@@ -24331,11 +24331,11 @@
       <c r="Y198" t="inlineStr"/>
       <c r="Z198" t="inlineStr"/>
       <c r="AA198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB198" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Italy', 'Belgium', 'Sweden']</t>
         </is>
       </c>
       <c r="AC198" t="n">
@@ -24391,7 +24391,7 @@
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>['Belgium', 'Ireland', 'Italy']</t>
+          <t>['Belgium', 'Italy', 'Ireland']</t>
         </is>
       </c>
       <c r="K199" t="inlineStr">
@@ -24459,10 +24459,10 @@
         </is>
       </c>
       <c r="AC199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE199" t="n">
         <v>-4</v>
@@ -24519,7 +24519,7 @@
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>['Belgium', 'Ireland', 'Italy']</t>
+          <t>['Belgium', 'Italy', 'Ireland']</t>
         </is>
       </c>
       <c r="K200" t="inlineStr">
@@ -24590,7 +24590,7 @@
         <v>1</v>
       </c>
       <c r="AD200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE200" t="n">
         <v>-3</v>
@@ -24633,7 +24633,7 @@
       <c r="I201" t="inlineStr"/>
       <c r="J201" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy', 'Switzerland']</t>
+          <t>['Switzerland', 'Italy', 'Wales']</t>
         </is>
       </c>
       <c r="K201" t="inlineStr">
@@ -24669,11 +24669,11 @@
       <c r="Y201" t="inlineStr"/>
       <c r="Z201" t="inlineStr"/>
       <c r="AA201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB201" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="AC201" t="n">
@@ -24729,7 +24729,7 @@
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy', 'Switzerland']</t>
+          <t>['Switzerland', 'Italy', 'Wales']</t>
         </is>
       </c>
       <c r="K202" t="inlineStr">
@@ -24797,10 +24797,10 @@
         </is>
       </c>
       <c r="AC202" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD202" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE202" t="n">
         <v>-4</v>
@@ -24857,7 +24857,7 @@
       </c>
       <c r="J203" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy', 'Switzerland']</t>
+          <t>['Switzerland', 'Italy', 'Wales']</t>
         </is>
       </c>
       <c r="K203" t="inlineStr">
@@ -24928,7 +24928,7 @@
         <v>0</v>
       </c>
       <c r="AD203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE203" t="n">
         <v>-4</v>
@@ -24985,7 +24985,7 @@
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy', 'Switzerland']</t>
+          <t>['Switzerland', 'Italy', 'Wales']</t>
         </is>
       </c>
       <c r="K204" t="inlineStr">
@@ -25056,7 +25056,7 @@
         <v>0</v>
       </c>
       <c r="AD204" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE204" t="n">
         <v>-4</v>
@@ -25113,7 +25113,7 @@
       </c>
       <c r="J205" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy', 'Switzerland']</t>
+          <t>['Switzerland', 'Italy', 'Wales']</t>
         </is>
       </c>
       <c r="K205" t="inlineStr">
@@ -25184,7 +25184,7 @@
         <v>0</v>
       </c>
       <c r="AD205" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE205" t="n">
         <v>-4</v>
@@ -25241,7 +25241,7 @@
       </c>
       <c r="J206" t="inlineStr">
         <is>
-          <t>['Wales', 'Italy', 'Switzerland']</t>
+          <t>['Switzerland', 'Italy', 'Wales']</t>
         </is>
       </c>
       <c r="K206" t="inlineStr">
@@ -25312,7 +25312,7 @@
         <v>0</v>
       </c>
       <c r="AD206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE206" t="n">
         <v>-4</v>
@@ -25355,7 +25355,7 @@
       <c r="I207" t="inlineStr"/>
       <c r="J207" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'Ukraine']</t>
+          <t>['Netherlands', 'Austria', 'Ukraine']</t>
         </is>
       </c>
       <c r="K207" t="inlineStr">
@@ -25451,7 +25451,7 @@
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'Ukraine']</t>
+          <t>['Netherlands', 'Austria', 'Ukraine']</t>
         </is>
       </c>
       <c r="K208" t="inlineStr">
@@ -25579,7 +25579,7 @@
       </c>
       <c r="J209" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'Ukraine']</t>
+          <t>['Netherlands', 'Austria', 'Ukraine']</t>
         </is>
       </c>
       <c r="K209" t="inlineStr">
@@ -25707,7 +25707,7 @@
       </c>
       <c r="J210" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'Ukraine']</t>
+          <t>['Netherlands', 'Austria', 'Ukraine']</t>
         </is>
       </c>
       <c r="K210" t="inlineStr">
@@ -25835,7 +25835,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'Ukraine']</t>
+          <t>['Netherlands', 'Austria', 'Ukraine']</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
@@ -25949,7 +25949,7 @@
       <c r="I212" t="inlineStr"/>
       <c r="J212" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Russia']</t>
+          <t>['Russia', 'Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K212" t="inlineStr">
@@ -26045,7 +26045,7 @@
       </c>
       <c r="J213" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Denmark', 'Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K213" t="inlineStr">
@@ -26173,7 +26173,7 @@
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Denmark', 'Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K214" t="inlineStr">
@@ -26301,7 +26301,7 @@
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Denmark', 'Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K215" t="inlineStr">
@@ -26429,7 +26429,7 @@
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>['Belgium', 'Russia', 'Denmark']</t>
+          <t>['Denmark', 'Russia', 'Belgium']</t>
         </is>
       </c>
       <c r="K216" t="inlineStr">
@@ -26557,7 +26557,7 @@
       </c>
       <c r="J217" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Denmark', 'Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K217" t="inlineStr">
@@ -26685,7 +26685,7 @@
       </c>
       <c r="J218" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Denmark', 'Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K218" t="inlineStr">
@@ -26813,7 +26813,7 @@
       </c>
       <c r="J219" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Denmark', 'Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K219" t="inlineStr">
@@ -26927,7 +26927,7 @@
       <c r="I220" t="inlineStr"/>
       <c r="J220" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'England', 'Croatia']</t>
+          <t>['Czech Republic', 'Croatia', 'England']</t>
         </is>
       </c>
       <c r="K220" t="inlineStr">
@@ -26963,11 +26963,11 @@
       <c r="Y220" t="inlineStr"/>
       <c r="Z220" t="inlineStr"/>
       <c r="AA220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB220" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'England']</t>
+          <t>['Czech Republic', 'England', 'Croatia']</t>
         </is>
       </c>
       <c r="AC220" t="n">
@@ -27023,7 +27023,7 @@
       </c>
       <c r="J221" t="inlineStr">
         <is>
-          <t>['England', 'Croatia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Croatia', 'England']</t>
         </is>
       </c>
       <c r="K221" t="inlineStr">
@@ -27091,10 +27091,10 @@
         </is>
       </c>
       <c r="AC221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE221" t="n">
         <v>-2</v>
@@ -27151,7 +27151,7 @@
       </c>
       <c r="J222" t="inlineStr">
         <is>
-          <t>['England', 'Croatia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Croatia', 'England']</t>
         </is>
       </c>
       <c r="K222" t="inlineStr">
@@ -27222,7 +27222,7 @@
         <v>1</v>
       </c>
       <c r="AD222" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE222" t="n">
         <v>-3</v>
@@ -27279,7 +27279,7 @@
       </c>
       <c r="J223" t="inlineStr">
         <is>
-          <t>['England', 'Croatia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Croatia', 'England']</t>
         </is>
       </c>
       <c r="K223" t="inlineStr">
@@ -27350,7 +27350,7 @@
         <v>1</v>
       </c>
       <c r="AD223" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE223" t="n">
         <v>-2</v>
@@ -27407,7 +27407,7 @@
       </c>
       <c r="J224" t="inlineStr">
         <is>
-          <t>['England', 'Croatia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Croatia', 'England']</t>
         </is>
       </c>
       <c r="K224" t="inlineStr">
@@ -27478,7 +27478,7 @@
         <v>1</v>
       </c>
       <c r="AD224" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE224" t="n">
         <v>-3</v>
@@ -27535,7 +27535,7 @@
       </c>
       <c r="J225" t="inlineStr">
         <is>
-          <t>['England', 'Czech Republic', 'Croatia']</t>
+          <t>['Czech Republic', 'Croatia', 'England']</t>
         </is>
       </c>
       <c r="K225" t="inlineStr">
@@ -27606,7 +27606,7 @@
         <v>0</v>
       </c>
       <c r="AD225" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE225" t="n">
         <v>-3</v>
@@ -27649,7 +27649,7 @@
       <c r="I226" t="inlineStr"/>
       <c r="J226" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden', 'Slovakia']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K226" t="inlineStr">
@@ -27745,7 +27745,7 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden', 'Slovakia']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K227" t="inlineStr">
@@ -27873,7 +27873,7 @@
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden', 'Slovakia']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
@@ -28001,7 +28001,7 @@
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden', 'Slovakia']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
@@ -28129,7 +28129,7 @@
       </c>
       <c r="J230" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden', 'Slovakia']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K230" t="inlineStr">
@@ -28257,7 +28257,7 @@
       </c>
       <c r="J231" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden', 'Slovakia']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K231" t="inlineStr">
@@ -28385,7 +28385,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden', 'Slovakia']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
@@ -28513,7 +28513,7 @@
       </c>
       <c r="J233" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden', 'Slovakia']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K233" t="inlineStr">
@@ -28641,7 +28641,7 @@
       </c>
       <c r="J234" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden', 'Slovakia']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K234" t="inlineStr">
@@ -28769,7 +28769,7 @@
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden', 'Slovakia']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K235" t="inlineStr">
@@ -28897,7 +28897,7 @@
       </c>
       <c r="J236" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden', 'Slovakia']</t>
+          <t>['Slovakia', 'Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K236" t="inlineStr">
@@ -29011,7 +29011,7 @@
       <c r="I237" t="inlineStr"/>
       <c r="J237" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Germany']</t>
+          <t>['France', 'Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K237" t="inlineStr">
@@ -29107,7 +29107,7 @@
       </c>
       <c r="J238" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Hungary']</t>
+          <t>['France', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K238" t="inlineStr">
@@ -29235,7 +29235,7 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Hungary']</t>
+          <t>['France', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K239" t="inlineStr">
@@ -29363,7 +29363,7 @@
       </c>
       <c r="J240" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Hungary']</t>
+          <t>['France', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K240" t="inlineStr">
@@ -29491,7 +29491,7 @@
       </c>
       <c r="J241" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Hungary']</t>
+          <t>['France', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K241" t="inlineStr">
@@ -29619,7 +29619,7 @@
       </c>
       <c r="J242" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Hungary']</t>
+          <t>['France', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K242" t="inlineStr">
@@ -29747,7 +29747,7 @@
       </c>
       <c r="J243" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Germany']</t>
+          <t>['France', 'Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K243" t="inlineStr">
@@ -29875,7 +29875,7 @@
       </c>
       <c r="J244" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Hungary']</t>
+          <t>['France', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K244" t="inlineStr">
@@ -30003,7 +30003,7 @@
       </c>
       <c r="J245" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Germany']</t>
+          <t>['France', 'Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K245" t="inlineStr">
@@ -30117,7 +30117,7 @@
       <c r="I246" t="inlineStr"/>
       <c r="J246" t="inlineStr">
         <is>
-          <t>['Scotland', 'Germany', 'Switzerland']</t>
+          <t>['Germany', 'Scotland', 'Switzerland']</t>
         </is>
       </c>
       <c r="K246" t="inlineStr">
@@ -30213,7 +30213,7 @@
       </c>
       <c r="J247" t="inlineStr">
         <is>
-          <t>['Scotland', 'Germany', 'Switzerland']</t>
+          <t>['Germany', 'Scotland', 'Switzerland']</t>
         </is>
       </c>
       <c r="K247" t="inlineStr">
@@ -30341,7 +30341,7 @@
       </c>
       <c r="J248" t="inlineStr">
         <is>
-          <t>['Scotland', 'Germany', 'Switzerland']</t>
+          <t>['Germany', 'Scotland', 'Switzerland']</t>
         </is>
       </c>
       <c r="K248" t="inlineStr">
@@ -30583,7 +30583,7 @@
       <c r="I250" t="inlineStr"/>
       <c r="J250" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy', 'Albania']</t>
+          <t>['Albania', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K250" t="inlineStr">
@@ -30619,11 +30619,11 @@
       <c r="Y250" t="inlineStr"/>
       <c r="Z250" t="inlineStr"/>
       <c r="AA250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB250" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Spain', 'Italy', 'Albania']</t>
         </is>
       </c>
       <c r="AC250" t="n">
@@ -30679,7 +30679,7 @@
       </c>
       <c r="J251" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Italy']</t>
+          <t>['Spain', 'Italy', 'Croatia']</t>
         </is>
       </c>
       <c r="K251" t="inlineStr">
@@ -30747,10 +30747,10 @@
         </is>
       </c>
       <c r="AC251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE251" t="n">
         <v>-2</v>
@@ -30878,7 +30878,7 @@
         <v>1</v>
       </c>
       <c r="AD252" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE252" t="n">
         <v>-2</v>
@@ -30935,7 +30935,7 @@
       </c>
       <c r="J253" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Italy']</t>
+          <t>['Spain', 'Italy', 'Croatia']</t>
         </is>
       </c>
       <c r="K253" t="inlineStr">
@@ -31006,7 +31006,7 @@
         <v>1</v>
       </c>
       <c r="AD253" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE253" t="n">
         <v>-2</v>
@@ -31049,7 +31049,7 @@
       <c r="I254" t="inlineStr"/>
       <c r="J254" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K254" t="inlineStr">
@@ -31273,7 +31273,7 @@
       </c>
       <c r="J256" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K256" t="inlineStr">
@@ -31401,7 +31401,7 @@
       </c>
       <c r="J257" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K257" t="inlineStr">
@@ -31657,7 +31657,7 @@
       </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K259" t="inlineStr">
@@ -31785,7 +31785,7 @@
       </c>
       <c r="J260" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K260" t="inlineStr">
@@ -32027,7 +32027,7 @@
       <c r="I262" t="inlineStr"/>
       <c r="J262" t="inlineStr">
         <is>
-          <t>['England', 'Slovenia', 'Denmark']</t>
+          <t>['Slovenia', 'Denmark', 'England']</t>
         </is>
       </c>
       <c r="K262" t="inlineStr">
@@ -32109,7 +32109,7 @@
       <c r="I263" t="inlineStr"/>
       <c r="J263" t="inlineStr">
         <is>
-          <t>['Belgium', 'Slovakia', 'Romania']</t>
+          <t>['Slovakia', 'Romania', 'Belgium']</t>
         </is>
       </c>
       <c r="K263" t="inlineStr">
@@ -32205,7 +32205,7 @@
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>['Belgium', 'Ukraine', 'Slovakia']</t>
+          <t>['Slovakia', 'Ukraine', 'Belgium']</t>
         </is>
       </c>
       <c r="K264" t="inlineStr">
@@ -32333,7 +32333,7 @@
       </c>
       <c r="J265" t="inlineStr">
         <is>
-          <t>['Belgium', 'Slovakia', 'Romania']</t>
+          <t>['Slovakia', 'Romania', 'Belgium']</t>
         </is>
       </c>
       <c r="K265" t="inlineStr">
@@ -32447,7 +32447,7 @@
       <c r="I266" t="inlineStr"/>
       <c r="J266" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal', 'Turkey']</t>
+          <t>['Turkey', 'Czech Republic', 'Portugal']</t>
         </is>
       </c>
       <c r="K266" t="inlineStr">
@@ -32483,11 +32483,11 @@
       <c r="Y266" t="inlineStr"/>
       <c r="Z266" t="inlineStr"/>
       <c r="AA266" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB266" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey']</t>
+          <t>['Portugal', 'Turkey', 'Czech Republic']</t>
         </is>
       </c>
       <c r="AC266" t="n">
@@ -32543,7 +32543,7 @@
       </c>
       <c r="J267" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Turkey', 'Georgia', 'Portugal']</t>
         </is>
       </c>
       <c r="K267" t="inlineStr">
@@ -32671,7 +32671,7 @@
       </c>
       <c r="J268" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Turkey', 'Georgia', 'Portugal']</t>
         </is>
       </c>
       <c r="K268" t="inlineStr">
@@ -32799,7 +32799,7 @@
       </c>
       <c r="J269" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Turkey', 'Georgia', 'Portugal']</t>
         </is>
       </c>
       <c r="K269" t="inlineStr">
@@ -32927,7 +32927,7 @@
       </c>
       <c r="J270" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Turkey', 'Georgia', 'Portugal']</t>
         </is>
       </c>
       <c r="K270" t="inlineStr">
@@ -33055,7 +33055,7 @@
       </c>
       <c r="J271" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Turkey', 'Georgia', 'Portugal']</t>
         </is>
       </c>
       <c r="K271" t="inlineStr">

</xml_diff>

<commit_message>
tie break three and four teams
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
+++ b/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
@@ -633,7 +633,7 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['France', 'Denmark']</t>
+          <t>['Denmark', 'France']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -729,7 +729,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -857,7 +857,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -1113,7 +1113,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>['France', 'Denmark']</t>
+          <t>['Denmark', 'France']</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>['France', 'Denmark']</t>
+          <t>['Denmark', 'France']</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1625,7 +1625,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>['France', 'Denmark']</t>
+          <t>['Denmark', 'France']</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>['France', 'Denmark']</t>
+          <t>['Denmark', 'France']</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>['France', 'Denmark']</t>
+          <t>['Denmark', 'France']</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1995,7 +1995,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t>['West Germany', 'Spain']</t>
+          <t>['Spain', 'West Germany']</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -2927,7 +2927,7 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -3279,7 +3279,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -3407,7 +3407,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -3649,7 +3649,7 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
-          <t>['France', 'Sweden']</t>
+          <t>['Sweden', 'France']</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -4129,7 +4129,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>['France', 'Sweden']</t>
+          <t>['Sweden', 'France']</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -6327,7 +6327,7 @@
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr">
         <is>
-          <t>['France', 'Bulgaria']</t>
+          <t>['Bulgaria', 'France']</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -6423,7 +6423,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Spain']</t>
+          <t>['Spain', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -6551,7 +6551,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>['France', 'Spain']</t>
+          <t>['Spain', 'France']</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -6679,7 +6679,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>['France', 'Bulgaria']</t>
+          <t>['Bulgaria', 'France']</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -6807,7 +6807,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>['France', 'Bulgaria']</t>
+          <t>['Bulgaria', 'France']</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -6935,7 +6935,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>['France', 'Bulgaria']</t>
+          <t>['Bulgaria', 'France']</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -7063,7 +7063,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>['France', 'Spain']</t>
+          <t>['Spain', 'France']</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -7191,7 +7191,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>['France', 'Spain']</t>
+          <t>['Spain', 'France']</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -7305,7 +7305,7 @@
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr">
         <is>
-          <t>['Germany', 'Italy']</t>
+          <t>['Italy', 'Germany']</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -7401,7 +7401,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -7529,7 +7529,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -7657,7 +7657,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -7785,7 +7785,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>['Germany', 'Italy']</t>
+          <t>['Italy', 'Germany']</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -7913,7 +7913,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>['Germany', 'Italy']</t>
+          <t>['Italy', 'Germany']</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -8041,7 +8041,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>['Germany', 'Italy']</t>
+          <t>['Italy', 'Germany']</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -8155,7 +8155,7 @@
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr">
         <is>
-          <t>['Croatia', 'Portugal']</t>
+          <t>['Portugal', 'Croatia']</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -8251,7 +8251,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>['Croatia', 'Portugal']</t>
+          <t>['Portugal', 'Croatia']</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -8379,7 +8379,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>['Croatia', 'Portugal']</t>
+          <t>['Portugal', 'Croatia']</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -8507,7 +8507,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>['Croatia', 'Portugal']</t>
+          <t>['Portugal', 'Croatia']</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -8635,7 +8635,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>['Croatia', 'Portugal']</t>
+          <t>['Portugal', 'Croatia']</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>['Croatia', 'Portugal']</t>
+          <t>['Portugal', 'Croatia']</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -8891,7 +8891,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>['Croatia', 'Portugal']</t>
+          <t>['Portugal', 'Croatia']</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -10335,7 +10335,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>['Turkey', 'Italy']</t>
+          <t>['Italy', 'Turkey']</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -10463,7 +10463,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>['Turkey', 'Italy']</t>
+          <t>['Italy', 'Turkey']</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -10591,7 +10591,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>['Turkey', 'Italy']</t>
+          <t>['Italy', 'Turkey']</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -10719,7 +10719,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>['Turkey', 'Italy']</t>
+          <t>['Italy', 'Turkey']</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -11811,7 +11811,7 @@
       <c r="I94" t="inlineStr"/>
       <c r="J94" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
@@ -11907,7 +11907,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
@@ -12035,7 +12035,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -12163,7 +12163,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K97" t="inlineStr">
@@ -12291,7 +12291,7 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K98" t="inlineStr">
@@ -12789,7 +12789,7 @@
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr">
         <is>
-          <t>['Greece', 'Spain']</t>
+          <t>['Spain', 'Greece']</t>
         </is>
       </c>
       <c r="K102" t="inlineStr">
@@ -12885,7 +12885,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -13013,7 +13013,7 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
@@ -13141,7 +13141,7 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
@@ -13383,7 +13383,7 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
@@ -13479,7 +13479,7 @@
       </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>['France', 'Croatia']</t>
+          <t>['Croatia', 'France']</t>
         </is>
       </c>
       <c r="K108" t="inlineStr">
@@ -13607,7 +13607,7 @@
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>['France', 'Croatia']</t>
+          <t>['Croatia', 'France']</t>
         </is>
       </c>
       <c r="K109" t="inlineStr">
@@ -13735,7 +13735,7 @@
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t>['France', 'Croatia']</t>
+          <t>['Croatia', 'France']</t>
         </is>
       </c>
       <c r="K110" t="inlineStr">
@@ -13863,7 +13863,7 @@
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K111" t="inlineStr">
@@ -14375,7 +14375,7 @@
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K115" t="inlineStr">
@@ -14503,7 +14503,7 @@
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K116" t="inlineStr">
@@ -14631,7 +14631,7 @@
       </c>
       <c r="J117" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K117" t="inlineStr">
@@ -15723,7 +15723,7 @@
       <c r="I126" t="inlineStr"/>
       <c r="J126" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="K126" t="inlineStr">
@@ -15819,7 +15819,7 @@
       </c>
       <c r="J127" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="K127" t="inlineStr">
@@ -15947,7 +15947,7 @@
       </c>
       <c r="J128" t="inlineStr">
         <is>
-          <t>['Germany', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Germany']</t>
         </is>
       </c>
       <c r="K128" t="inlineStr">
@@ -16573,7 +16573,7 @@
       <c r="I133" t="inlineStr"/>
       <c r="J133" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K133" t="inlineStr">
@@ -16669,7 +16669,7 @@
       </c>
       <c r="J134" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K134" t="inlineStr">
@@ -16797,7 +16797,7 @@
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K135" t="inlineStr">
@@ -16925,7 +16925,7 @@
       </c>
       <c r="J136" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K136" t="inlineStr">
@@ -17053,7 +17053,7 @@
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K137" t="inlineStr">
@@ -17181,7 +17181,7 @@
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K138" t="inlineStr">
@@ -17309,7 +17309,7 @@
       </c>
       <c r="J139" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K139" t="inlineStr">
@@ -17437,7 +17437,7 @@
       </c>
       <c r="J140" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal']</t>
+          <t>['Portugal', 'Turkey']</t>
         </is>
       </c>
       <c r="K140" t="inlineStr">
@@ -17551,7 +17551,7 @@
       <c r="I141" t="inlineStr"/>
       <c r="J141" t="inlineStr">
         <is>
-          <t>['Germany', 'Croatia']</t>
+          <t>['Croatia', 'Germany']</t>
         </is>
       </c>
       <c r="K141" t="inlineStr">
@@ -17647,7 +17647,7 @@
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>['Germany', 'Croatia']</t>
+          <t>['Croatia', 'Germany']</t>
         </is>
       </c>
       <c r="K142" t="inlineStr">
@@ -17775,7 +17775,7 @@
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>['Germany', 'Croatia']</t>
+          <t>['Croatia', 'Germany']</t>
         </is>
       </c>
       <c r="K143" t="inlineStr">
@@ -18483,7 +18483,7 @@
       <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K149" t="inlineStr">
@@ -18579,7 +18579,7 @@
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="K150" t="inlineStr">
@@ -18707,7 +18707,7 @@
       </c>
       <c r="J151" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="K151" t="inlineStr">
@@ -18835,7 +18835,7 @@
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="K152" t="inlineStr">
@@ -18963,7 +18963,7 @@
       </c>
       <c r="J153" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="K153" t="inlineStr">
@@ -19091,7 +19091,7 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="K154" t="inlineStr">
@@ -19205,7 +19205,7 @@
       <c r="I155" t="inlineStr"/>
       <c r="J155" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
@@ -19301,7 +19301,7 @@
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>['Russia', 'Greece']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="K156" t="inlineStr">
@@ -19320,31 +19320,31 @@
       </c>
       <c r="O156" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Czech Republic</t>
         </is>
       </c>
       <c r="P156" t="n">
         <v>4</v>
       </c>
       <c r="Q156" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="R156" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S156" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="T156" t="n">
         <v>4</v>
       </c>
       <c r="U156" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="V156" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W156" t="inlineStr">
         <is>
@@ -19365,20 +19365,20 @@
       </c>
       <c r="AB156" t="inlineStr">
         <is>
-          <t>['Russia', 'Greece']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="AC156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE156" t="n">
         <v>0</v>
       </c>
       <c r="AF156" t="n">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="AG156" t="n">
         <v>1780</v>
@@ -19497,10 +19497,10 @@
         </is>
       </c>
       <c r="AC157" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD157" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE157" t="n">
         <v>0</v>
@@ -19543,7 +19543,7 @@
       <c r="I158" t="inlineStr"/>
       <c r="J158" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K158" t="inlineStr">
@@ -19767,7 +19767,7 @@
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K160" t="inlineStr">
@@ -20023,7 +20023,7 @@
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K162" t="inlineStr">
@@ -20151,7 +20151,7 @@
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K163" t="inlineStr">
@@ -20279,7 +20279,7 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>['Germany', 'Portugal']</t>
+          <t>['Portugal', 'Germany']</t>
         </is>
       </c>
       <c r="K164" t="inlineStr">
@@ -20393,7 +20393,7 @@
       <c r="I165" t="inlineStr"/>
       <c r="J165" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K165" t="inlineStr">
@@ -20859,7 +20859,7 @@
       <c r="I169" t="inlineStr"/>
       <c r="J169" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K169" t="inlineStr">
@@ -21325,7 +21325,7 @@
       <c r="I173" t="inlineStr"/>
       <c r="J173" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France', 'Romania']</t>
+          <t>['Romania', 'Switzerland', 'France']</t>
         </is>
       </c>
       <c r="K173" t="inlineStr">
@@ -21421,7 +21421,7 @@
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France', 'Albania']</t>
+          <t>['Albania', 'Switzerland', 'France']</t>
         </is>
       </c>
       <c r="K174" t="inlineStr">
@@ -21535,7 +21535,7 @@
       <c r="I175" t="inlineStr"/>
       <c r="J175" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Wales', 'England']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K175" t="inlineStr">
@@ -21631,7 +21631,7 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>['England', 'Slovakia', 'Wales']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K176" t="inlineStr">
@@ -21759,7 +21759,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>['England', 'Slovakia', 'Wales']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -21887,7 +21887,7 @@
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>['England', 'Slovakia', 'Wales']</t>
+          <t>['Wales', 'England', 'Slovakia']</t>
         </is>
       </c>
       <c r="K178" t="inlineStr">
@@ -22001,7 +22001,7 @@
       <c r="I179" t="inlineStr"/>
       <c r="J179" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Poland', 'Northern Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K179" t="inlineStr">
@@ -22097,7 +22097,7 @@
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Poland', 'Northern Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K180" t="inlineStr">
@@ -22225,7 +22225,7 @@
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>['Germany', 'Poland', 'Northern Ireland']</t>
+          <t>['Poland', 'Northern Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
@@ -22339,7 +22339,7 @@
       <c r="I182" t="inlineStr"/>
       <c r="J182" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'Spain']</t>
+          <t>['Spain', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K182" t="inlineStr">
@@ -22435,7 +22435,7 @@
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'Spain']</t>
+          <t>['Spain', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K183" t="inlineStr">
@@ -22563,7 +22563,7 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>['Croatia', 'Turkey', 'Spain']</t>
+          <t>['Spain', 'Croatia', 'Turkey']</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
@@ -22691,7 +22691,7 @@
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>['Croatia', 'Turkey', 'Spain']</t>
+          <t>['Spain', 'Croatia', 'Turkey']</t>
         </is>
       </c>
       <c r="K185" t="inlineStr">
@@ -22819,7 +22819,7 @@
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>['Croatia', 'Turkey', 'Spain']</t>
+          <t>['Spain', 'Croatia', 'Turkey']</t>
         </is>
       </c>
       <c r="K186" t="inlineStr">
@@ -22947,7 +22947,7 @@
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>['Croatia', 'Turkey', 'Spain']</t>
+          <t>['Spain', 'Croatia', 'Turkey']</t>
         </is>
       </c>
       <c r="K187" t="inlineStr">
@@ -23061,7 +23061,7 @@
       <c r="I188" t="inlineStr"/>
       <c r="J188" t="inlineStr">
         <is>
-          <t>['Sweden', 'Italy', 'Belgium']</t>
+          <t>['Italy', 'Belgium', 'Sweden']</t>
         </is>
       </c>
       <c r="K188" t="inlineStr">
@@ -23157,7 +23157,7 @@
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>['Ireland', 'Italy', 'Belgium']</t>
+          <t>['Italy', 'Belgium', 'Ireland']</t>
         </is>
       </c>
       <c r="K189" t="inlineStr">
@@ -23285,7 +23285,7 @@
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>['Ireland', 'Italy', 'Belgium']</t>
+          <t>['Italy', 'Belgium', 'Ireland']</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
@@ -23399,7 +23399,7 @@
       <c r="I191" t="inlineStr"/>
       <c r="J191" t="inlineStr">
         <is>
-          <t>['Hungary', 'Portugal', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K191" t="inlineStr">
@@ -23495,7 +23495,7 @@
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>['Hungary', 'Portugal', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K192" t="inlineStr">
@@ -23623,7 +23623,7 @@
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>['Hungary', 'Portugal', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K193" t="inlineStr">
@@ -23751,7 +23751,7 @@
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>['Hungary', 'Portugal', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
@@ -23879,7 +23879,7 @@
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>['Hungary', 'Portugal', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K195" t="inlineStr">
@@ -24007,7 +24007,7 @@
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>['Hungary', 'Portugal', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K196" t="inlineStr">
@@ -24135,7 +24135,7 @@
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>['Hungary', 'Portugal', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K197" t="inlineStr">
@@ -24263,7 +24263,7 @@
       </c>
       <c r="J198" t="inlineStr">
         <is>
-          <t>['Hungary', 'Portugal', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K198" t="inlineStr">
@@ -24391,7 +24391,7 @@
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>['Hungary', 'Portugal', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K199" t="inlineStr">
@@ -24519,7 +24519,7 @@
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>['Hungary', 'Portugal', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K200" t="inlineStr">
@@ -24633,7 +24633,7 @@
       <c r="I201" t="inlineStr"/>
       <c r="J201" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="K201" t="inlineStr">
@@ -24729,7 +24729,7 @@
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="K202" t="inlineStr">
@@ -24857,7 +24857,7 @@
       </c>
       <c r="J203" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="K203" t="inlineStr">
@@ -24985,7 +24985,7 @@
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="K204" t="inlineStr">
@@ -25113,7 +25113,7 @@
       </c>
       <c r="J205" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="K205" t="inlineStr">
@@ -25241,7 +25241,7 @@
       </c>
       <c r="J206" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Italy', 'Wales', 'Switzerland']</t>
         </is>
       </c>
       <c r="K206" t="inlineStr">
@@ -25355,7 +25355,7 @@
       <c r="I207" t="inlineStr"/>
       <c r="J207" t="inlineStr">
         <is>
-          <t>['Russia', 'Finland', 'Belgium']</t>
+          <t>['Finland', 'Belgium', 'Russia']</t>
         </is>
       </c>
       <c r="K207" t="inlineStr">
@@ -25451,7 +25451,7 @@
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>['Denmark', 'Finland', 'Belgium']</t>
+          <t>['Finland', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="K208" t="inlineStr">
@@ -25579,7 +25579,7 @@
       </c>
       <c r="J209" t="inlineStr">
         <is>
-          <t>['Denmark', 'Finland', 'Belgium']</t>
+          <t>['Finland', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="K209" t="inlineStr">
@@ -25707,7 +25707,7 @@
       </c>
       <c r="J210" t="inlineStr">
         <is>
-          <t>['Denmark', 'Finland', 'Belgium']</t>
+          <t>['Finland', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="K210" t="inlineStr">
@@ -25835,7 +25835,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>['Denmark', 'Russia', 'Belgium']</t>
+          <t>['Belgium', 'Denmark', 'Russia']</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
@@ -25963,7 +25963,7 @@
       </c>
       <c r="J212" t="inlineStr">
         <is>
-          <t>['Denmark', 'Finland', 'Belgium']</t>
+          <t>['Belgium', 'Denmark', 'Russia']</t>
         </is>
       </c>
       <c r="K212" t="inlineStr">
@@ -25996,29 +25996,29 @@
       </c>
       <c r="S212" t="inlineStr">
         <is>
+          <t>Russia</t>
+        </is>
+      </c>
+      <c r="T212" t="n">
+        <v>3</v>
+      </c>
+      <c r="U212" t="n">
+        <v>-4</v>
+      </c>
+      <c r="V212" t="n">
+        <v>0</v>
+      </c>
+      <c r="W212" t="inlineStr">
+        <is>
           <t>Finland</t>
         </is>
       </c>
-      <c r="T212" t="n">
-        <v>3</v>
-      </c>
-      <c r="U212" t="n">
+      <c r="X212" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y212" t="n">
         <v>-1</v>
       </c>
-      <c r="V212" t="n">
-        <v>0</v>
-      </c>
-      <c r="W212" t="inlineStr">
-        <is>
-          <t>Russia</t>
-        </is>
-      </c>
-      <c r="X212" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y212" t="n">
-        <v>-4</v>
-      </c>
       <c r="Z212" t="n">
         <v>0</v>
       </c>
@@ -26027,20 +26027,20 @@
       </c>
       <c r="AB212" t="inlineStr">
         <is>
-          <t>['Belgium', 'Denmark', 'Finland']</t>
+          <t>['Belgium', 'Denmark', 'Russia']</t>
         </is>
       </c>
       <c r="AC212" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD212" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE212" t="n">
         <v>0</v>
       </c>
       <c r="AF212" t="n">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="AG212" t="n">
         <v>1744</v>
@@ -26091,7 +26091,7 @@
       </c>
       <c r="J213" t="inlineStr">
         <is>
-          <t>['Denmark', 'Finland', 'Belgium']</t>
+          <t>['Belgium', 'Denmark', 'Russia']</t>
         </is>
       </c>
       <c r="K213" t="inlineStr">
@@ -26124,29 +26124,29 @@
       </c>
       <c r="S213" t="inlineStr">
         <is>
+          <t>Russia</t>
+        </is>
+      </c>
+      <c r="T213" t="n">
+        <v>3</v>
+      </c>
+      <c r="U213" t="n">
+        <v>-4</v>
+      </c>
+      <c r="V213" t="n">
+        <v>0</v>
+      </c>
+      <c r="W213" t="inlineStr">
+        <is>
           <t>Finland</t>
         </is>
       </c>
-      <c r="T213" t="n">
-        <v>3</v>
-      </c>
-      <c r="U213" t="n">
+      <c r="X213" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y213" t="n">
         <v>-2</v>
       </c>
-      <c r="V213" t="n">
-        <v>0</v>
-      </c>
-      <c r="W213" t="inlineStr">
-        <is>
-          <t>Russia</t>
-        </is>
-      </c>
-      <c r="X213" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y213" t="n">
-        <v>-4</v>
-      </c>
       <c r="Z213" t="n">
         <v>0</v>
       </c>
@@ -26155,20 +26155,20 @@
       </c>
       <c r="AB213" t="inlineStr">
         <is>
-          <t>['Belgium', 'Denmark', 'Finland']</t>
+          <t>['Belgium', 'Denmark', 'Russia']</t>
         </is>
       </c>
       <c r="AC213" t="n">
         <v>0</v>
       </c>
       <c r="AD213" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE213" t="n">
         <v>0</v>
       </c>
       <c r="AF213" t="n">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="AG213" t="n">
         <v>1684</v>
@@ -26219,7 +26219,7 @@
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>['Denmark', 'Finland', 'Belgium']</t>
+          <t>['Belgium', 'Denmark', 'Russia']</t>
         </is>
       </c>
       <c r="K214" t="inlineStr">
@@ -26252,29 +26252,29 @@
       </c>
       <c r="S214" t="inlineStr">
         <is>
+          <t>Russia</t>
+        </is>
+      </c>
+      <c r="T214" t="n">
+        <v>3</v>
+      </c>
+      <c r="U214" t="n">
+        <v>-5</v>
+      </c>
+      <c r="V214" t="n">
+        <v>0</v>
+      </c>
+      <c r="W214" t="inlineStr">
+        <is>
           <t>Finland</t>
         </is>
       </c>
-      <c r="T214" t="n">
-        <v>3</v>
-      </c>
-      <c r="U214" t="n">
+      <c r="X214" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y214" t="n">
         <v>-2</v>
       </c>
-      <c r="V214" t="n">
-        <v>0</v>
-      </c>
-      <c r="W214" t="inlineStr">
-        <is>
-          <t>Russia</t>
-        </is>
-      </c>
-      <c r="X214" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y214" t="n">
-        <v>-5</v>
-      </c>
       <c r="Z214" t="n">
         <v>0</v>
       </c>
@@ -26283,20 +26283,20 @@
       </c>
       <c r="AB214" t="inlineStr">
         <is>
-          <t>['Belgium', 'Denmark', 'Finland']</t>
+          <t>['Belgium', 'Denmark', 'Russia']</t>
         </is>
       </c>
       <c r="AC214" t="n">
         <v>0</v>
       </c>
       <c r="AD214" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE214" t="n">
         <v>0</v>
       </c>
       <c r="AF214" t="n">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="AG214" t="n">
         <v>1744</v>
@@ -26333,7 +26333,7 @@
       <c r="I215" t="inlineStr"/>
       <c r="J215" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'Ukraine']</t>
+          <t>['Ukraine', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="K215" t="inlineStr">
@@ -26429,7 +26429,7 @@
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Netherlands', 'Austria']</t>
+          <t>['Ukraine', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="K216" t="inlineStr">
@@ -26557,7 +26557,7 @@
       </c>
       <c r="J217" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Netherlands', 'Austria']</t>
+          <t>['Ukraine', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="K217" t="inlineStr">
@@ -26685,7 +26685,7 @@
       </c>
       <c r="J218" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Netherlands', 'Austria']</t>
+          <t>['Ukraine', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="K218" t="inlineStr">
@@ -26813,7 +26813,7 @@
       </c>
       <c r="J219" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Netherlands', 'Austria']</t>
+          <t>['Ukraine', 'Austria', 'Netherlands']</t>
         </is>
       </c>
       <c r="K219" t="inlineStr">
@@ -27535,7 +27535,7 @@
       </c>
       <c r="J225" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['Croatia', 'Czech Republic', 'England']</t>
         </is>
       </c>
       <c r="K225" t="inlineStr">
@@ -27649,7 +27649,7 @@
       <c r="I226" t="inlineStr"/>
       <c r="J226" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia', 'Spain']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K226" t="inlineStr">
@@ -27745,7 +27745,7 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia', 'Spain']</t>
+          <t>['Slovakia', 'Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K227" t="inlineStr">
@@ -27873,7 +27873,7 @@
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia', 'Spain']</t>
+          <t>['Spain', 'Sweden', 'Slovakia']</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
@@ -28001,7 +28001,7 @@
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia', 'Spain']</t>
+          <t>['Spain', 'Sweden', 'Slovakia']</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
@@ -28129,7 +28129,7 @@
       </c>
       <c r="J230" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia', 'Spain']</t>
+          <t>['Spain', 'Sweden', 'Slovakia']</t>
         </is>
       </c>
       <c r="K230" t="inlineStr">
@@ -28257,7 +28257,7 @@
       </c>
       <c r="J231" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia', 'Spain']</t>
+          <t>['Spain', 'Sweden', 'Slovakia']</t>
         </is>
       </c>
       <c r="K231" t="inlineStr">
@@ -28385,7 +28385,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia', 'Spain']</t>
+          <t>['Spain', 'Sweden', 'Slovakia']</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
@@ -28513,7 +28513,7 @@
       </c>
       <c r="J233" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia', 'Spain']</t>
+          <t>['Spain', 'Sweden', 'Slovakia']</t>
         </is>
       </c>
       <c r="K233" t="inlineStr">
@@ -28641,7 +28641,7 @@
       </c>
       <c r="J234" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia', 'Spain']</t>
+          <t>['Spain', 'Sweden', 'Slovakia']</t>
         </is>
       </c>
       <c r="K234" t="inlineStr">
@@ -28769,7 +28769,7 @@
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia', 'Spain']</t>
+          <t>['Spain', 'Sweden', 'Slovakia']</t>
         </is>
       </c>
       <c r="K235" t="inlineStr">
@@ -28897,7 +28897,7 @@
       </c>
       <c r="J236" t="inlineStr">
         <is>
-          <t>['Sweden', 'Slovakia', 'Spain']</t>
+          <t>['Spain', 'Sweden', 'Slovakia']</t>
         </is>
       </c>
       <c r="K236" t="inlineStr">
@@ -29011,7 +29011,7 @@
       <c r="I237" t="inlineStr"/>
       <c r="J237" t="inlineStr">
         <is>
-          <t>['Germany', 'France', 'Portugal']</t>
+          <t>['Portugal', 'Germany', 'France']</t>
         </is>
       </c>
       <c r="K237" t="inlineStr">
@@ -29107,7 +29107,7 @@
       </c>
       <c r="J238" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Portugal']</t>
+          <t>['Portugal', 'Hungary', 'France']</t>
         </is>
       </c>
       <c r="K238" t="inlineStr">
@@ -29235,7 +29235,7 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Portugal']</t>
+          <t>['Portugal', 'Hungary', 'France']</t>
         </is>
       </c>
       <c r="K239" t="inlineStr">
@@ -29363,7 +29363,7 @@
       </c>
       <c r="J240" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Portugal']</t>
+          <t>['Portugal', 'Hungary', 'France']</t>
         </is>
       </c>
       <c r="K240" t="inlineStr">
@@ -29491,7 +29491,7 @@
       </c>
       <c r="J241" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Portugal']</t>
+          <t>['Portugal', 'Hungary', 'France']</t>
         </is>
       </c>
       <c r="K241" t="inlineStr">
@@ -29619,7 +29619,7 @@
       </c>
       <c r="J242" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Portugal']</t>
+          <t>['Portugal', 'Hungary', 'France']</t>
         </is>
       </c>
       <c r="K242" t="inlineStr">
@@ -29747,7 +29747,7 @@
       </c>
       <c r="J243" t="inlineStr">
         <is>
-          <t>['Germany', 'France', 'Portugal']</t>
+          <t>['Portugal', 'Germany', 'France']</t>
         </is>
       </c>
       <c r="K243" t="inlineStr">
@@ -29875,7 +29875,7 @@
       </c>
       <c r="J244" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Portugal']</t>
+          <t>['Portugal', 'Hungary', 'France']</t>
         </is>
       </c>
       <c r="K244" t="inlineStr">
@@ -30003,7 +30003,7 @@
       </c>
       <c r="J245" t="inlineStr">
         <is>
-          <t>['Germany', 'France', 'Portugal']</t>
+          <t>['Portugal', 'Germany', 'France']</t>
         </is>
       </c>
       <c r="K245" t="inlineStr">
@@ -30117,7 +30117,7 @@
       <c r="I246" t="inlineStr"/>
       <c r="J246" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Germany', 'Scotland']</t>
+          <t>['Scotland', 'Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="K246" t="inlineStr">
@@ -30213,7 +30213,7 @@
       </c>
       <c r="J247" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Germany', 'Scotland']</t>
+          <t>['Scotland', 'Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="K247" t="inlineStr">
@@ -30341,7 +30341,7 @@
       </c>
       <c r="J248" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Germany', 'Scotland']</t>
+          <t>['Scotland', 'Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="K248" t="inlineStr">
@@ -30469,7 +30469,7 @@
       </c>
       <c r="J249" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Germany', 'Hungary']</t>
+          <t>['Hungary', 'Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="K249" t="inlineStr">
@@ -30583,7 +30583,7 @@
       <c r="I250" t="inlineStr"/>
       <c r="J250" t="inlineStr">
         <is>
-          <t>['Albania', 'Italy', 'Spain']</t>
+          <t>['Italy', 'Spain', 'Albania']</t>
         </is>
       </c>
       <c r="K250" t="inlineStr">
@@ -30679,7 +30679,7 @@
       </c>
       <c r="J251" t="inlineStr">
         <is>
-          <t>['Croatia', 'Italy', 'Spain']</t>
+          <t>['Italy', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K251" t="inlineStr">
@@ -30807,7 +30807,7 @@
       </c>
       <c r="J252" t="inlineStr">
         <is>
-          <t>['Croatia', 'Italy', 'Spain']</t>
+          <t>['Italy', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K252" t="inlineStr">
@@ -30935,7 +30935,7 @@
       </c>
       <c r="J253" t="inlineStr">
         <is>
-          <t>['Croatia', 'Italy', 'Spain']</t>
+          <t>['Italy', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K253" t="inlineStr">
@@ -31049,7 +31049,7 @@
       <c r="I254" t="inlineStr"/>
       <c r="J254" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England', 'Denmark']</t>
+          <t>['Slovenia', 'Denmark', 'England']</t>
         </is>
       </c>
       <c r="K254" t="inlineStr">
@@ -31131,7 +31131,7 @@
       <c r="I255" t="inlineStr"/>
       <c r="J255" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands', 'Austria']</t>
+          <t>['Austria', 'France', 'Netherlands']</t>
         </is>
       </c>
       <c r="K255" t="inlineStr">
@@ -31227,7 +31227,7 @@
       </c>
       <c r="J256" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands', 'Austria']</t>
+          <t>['Austria', 'Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K256" t="inlineStr">
@@ -31355,7 +31355,7 @@
       </c>
       <c r="J257" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands', 'Austria']</t>
+          <t>['Austria', 'France', 'Netherlands']</t>
         </is>
       </c>
       <c r="K257" t="inlineStr">
@@ -31483,7 +31483,7 @@
       </c>
       <c r="J258" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands', 'Austria']</t>
+          <t>['Austria', 'Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K258" t="inlineStr">
@@ -31611,7 +31611,7 @@
       </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands', 'Austria']</t>
+          <t>['Austria', 'Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K259" t="inlineStr">
@@ -31739,7 +31739,7 @@
       </c>
       <c r="J260" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands', 'Austria']</t>
+          <t>['Austria', 'Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K260" t="inlineStr">
@@ -31867,7 +31867,7 @@
       </c>
       <c r="J261" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands', 'Austria']</t>
+          <t>['Austria', 'France', 'Netherlands']</t>
         </is>
       </c>
       <c r="K261" t="inlineStr">
@@ -31995,7 +31995,7 @@
       </c>
       <c r="J262" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands', 'Austria']</t>
+          <t>['Austria', 'Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K262" t="inlineStr">
@@ -32109,7 +32109,7 @@
       <c r="I263" t="inlineStr"/>
       <c r="J263" t="inlineStr">
         <is>
-          <t>['Romania', 'Slovakia', 'Belgium']</t>
+          <t>['Slovakia', 'Romania', 'Belgium']</t>
         </is>
       </c>
       <c r="K263" t="inlineStr">
@@ -32205,7 +32205,7 @@
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Slovakia', 'Belgium']</t>
+          <t>['Slovakia', 'Belgium', 'Ukraine']</t>
         </is>
       </c>
       <c r="K264" t="inlineStr">
@@ -32333,7 +32333,7 @@
       </c>
       <c r="J265" t="inlineStr">
         <is>
-          <t>['Romania', 'Slovakia', 'Belgium']</t>
+          <t>['Slovakia', 'Romania', 'Belgium']</t>
         </is>
       </c>
       <c r="K265" t="inlineStr">
@@ -32447,7 +32447,7 @@
       <c r="I266" t="inlineStr"/>
       <c r="J266" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Turkey', 'Portugal']</t>
+          <t>['Portugal', 'Turkey', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K266" t="inlineStr">
@@ -32543,7 +32543,7 @@
       </c>
       <c r="J267" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K267" t="inlineStr">
@@ -32671,7 +32671,7 @@
       </c>
       <c r="J268" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K268" t="inlineStr">
@@ -32799,7 +32799,7 @@
       </c>
       <c r="J269" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K269" t="inlineStr">
@@ -32927,7 +32927,7 @@
       </c>
       <c r="J270" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K270" t="inlineStr">
@@ -33055,7 +33055,7 @@
       </c>
       <c r="J271" t="inlineStr">
         <is>
-          <t>['Turkey', 'Portugal', 'Georgia']</t>
+          <t>['Portugal', 'Turkey', 'Georgia']</t>
         </is>
       </c>
       <c r="K271" t="inlineStr">

</xml_diff>

<commit_message>
best three and four tied
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
+++ b/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
@@ -633,7 +633,7 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['Denmark', 'France']</t>
+          <t>['Belgium', 'Denmark', 'France']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -729,7 +729,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France', 'Denmark']</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -857,7 +857,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France', 'Denmark']</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France', 'Denmark']</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -1113,7 +1113,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France', 'Denmark']</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France', 'Denmark']</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>['Denmark', 'France']</t>
+          <t>['Belgium', 'Denmark', 'France']</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>['Denmark', 'France']</t>
+          <t>['Belgium', 'Denmark', 'France']</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1625,7 +1625,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>['Denmark', 'France']</t>
+          <t>['Belgium', 'Denmark', 'France']</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>['Denmark', 'France']</t>
+          <t>['Belgium', 'Denmark', 'France']</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>['Denmark', 'France']</t>
+          <t>['Belgium', 'Denmark', 'France']</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1995,7 +1995,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t>['West Germany', 'Spain']</t>
+          <t>['West Germany', 'Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -2091,7 +2091,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>['Portugal', 'West Germany']</t>
+          <t>['West Germany', 'Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['West Germany', 'Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -2333,7 +2333,7 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t>['West Germany', 'Italy']</t>
+          <t>['West Germany', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -2429,7 +2429,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>['West Germany', 'Italy']</t>
+          <t>['West Germany', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>['West Germany', 'Italy']</t>
+          <t>['West Germany', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>['West Germany', 'Italy']</t>
+          <t>['West Germany', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>['West Germany', 'Italy']</t>
+          <t>['West Germany', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -2927,7 +2927,7 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Ireland']</t>
+          <t>['Netherlands', 'Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Ireland']</t>
+          <t>['Netherlands', 'Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Ireland']</t>
+          <t>['Netherlands', 'Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -3279,7 +3279,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Ireland']</t>
+          <t>['Netherlands', 'Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -3407,7 +3407,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Ireland']</t>
+          <t>['Netherlands', 'Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -3535,7 +3535,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Soviet Union']</t>
+          <t>['Netherlands', 'Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -3649,7 +3649,7 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
-          <t>['France', 'Sweden']</t>
+          <t>['England', 'Sweden', 'France']</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -3745,7 +3745,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>['England', 'Sweden']</t>
+          <t>['England', 'Sweden', 'France']</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>['England', 'Sweden']</t>
+          <t>['England', 'Sweden', 'Denmark']</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -4001,7 +4001,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>['England', 'Sweden']</t>
+          <t>['England', 'Sweden', 'Denmark']</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -4129,7 +4129,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>['France', 'Sweden']</t>
+          <t>['England', 'Sweden', 'France']</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>['Denmark', 'Sweden']</t>
+          <t>['Denmark', 'Sweden', 'England']</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -4385,7 +4385,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>['Denmark', 'Sweden']</t>
+          <t>['Denmark', 'Sweden', 'France']</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -4499,7 +4499,7 @@
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany']</t>
+          <t>['Netherlands', 'Commonwealth of Independent States', 'Germany']</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -4595,7 +4595,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany']</t>
+          <t>['Netherlands', 'Commonwealth of Independent States', 'Germany']</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -4723,7 +4723,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany']</t>
+          <t>['Netherlands', 'Commonwealth of Independent States', 'Germany']</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -4851,7 +4851,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany']</t>
+          <t>['Netherlands', 'Commonwealth of Independent States', 'Germany']</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -4979,7 +4979,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany']</t>
+          <t>['Netherlands', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -5107,7 +5107,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany']</t>
+          <t>['Netherlands', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -5235,7 +5235,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany']</t>
+          <t>['Netherlands', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -5363,7 +5363,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany']</t>
+          <t>['Netherlands', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -6455,7 +6455,7 @@
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr">
         <is>
-          <t>['Netherlands', 'England']</t>
+          <t>['England', 'Netherlands']</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -6551,7 +6551,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>['Netherlands', 'England']</t>
+          <t>['England', 'Netherlands']</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -6679,7 +6679,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>['Netherlands', 'England']</t>
+          <t>['England', 'Netherlands']</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -6807,7 +6807,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>['Netherlands', 'England']</t>
+          <t>['England', 'Netherlands']</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -6935,7 +6935,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>['Netherlands', 'England']</t>
+          <t>['England', 'Netherlands']</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -7063,7 +7063,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>['Scotland', 'England']</t>
+          <t>['England', 'Scotland']</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -7191,7 +7191,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>['Netherlands', 'England']</t>
+          <t>['England', 'Netherlands']</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -7401,7 +7401,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -7529,7 +7529,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -7657,7 +7657,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -7785,7 +7785,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -7913,7 +7913,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -8041,7 +8041,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>['Portugal', 'Croatia']</t>
+          <t>['Croatia', 'Portugal']</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -8155,7 +8155,7 @@
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr">
         <is>
-          <t>['Italy', 'Germany']</t>
+          <t>['Germany', 'Italy']</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -8251,7 +8251,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -8379,7 +8379,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -8507,7 +8507,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -8635,7 +8635,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>['Italy', 'Germany']</t>
+          <t>['Germany', 'Italy']</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>['Italy', 'Germany']</t>
+          <t>['Germany', 'Italy']</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -8891,7 +8891,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>['Italy', 'Germany']</t>
+          <t>['Germany', 'Italy']</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -9005,7 +9005,7 @@
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -9101,7 +9101,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -9727,7 +9727,7 @@
       <c r="I77" t="inlineStr"/>
       <c r="J77" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -9823,7 +9823,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>['Portugal', 'Romania']</t>
+          <t>['Romania', 'Portugal']</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -9951,7 +9951,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>['Portugal', 'Romania']</t>
+          <t>['Romania', 'Portugal']</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -10079,7 +10079,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -10207,7 +10207,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -10335,7 +10335,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -10463,7 +10463,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -10591,7 +10591,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -10719,7 +10719,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>['Portugal', 'Romania']</t>
+          <t>['Romania', 'Portugal']</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -10929,7 +10929,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>['Yugoslavia', 'Norway']</t>
+          <t>['Norway', 'Yugoslavia']</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -11185,7 +11185,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>['Yugoslavia', 'Norway']</t>
+          <t>['Norway', 'Yugoslavia']</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
@@ -11441,7 +11441,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>['Yugoslavia', 'Norway']</t>
+          <t>['Norway', 'Yugoslavia']</t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
@@ -12789,7 +12789,7 @@
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr">
         <is>
-          <t>['Spain', 'Greece']</t>
+          <t>['Greece', 'Spain']</t>
         </is>
       </c>
       <c r="K102" t="inlineStr">
@@ -12885,7 +12885,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -13013,7 +13013,7 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
@@ -13141,7 +13141,7 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
@@ -13269,7 +13269,7 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>['Portugal', 'Greece']</t>
+          <t>['Greece', 'Portugal']</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
@@ -13383,7 +13383,7 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
@@ -13863,7 +13863,7 @@
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K111" t="inlineStr">
@@ -13991,7 +13991,7 @@
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K112" t="inlineStr">
@@ -14119,7 +14119,7 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K113" t="inlineStr">
@@ -14247,7 +14247,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
@@ -14375,7 +14375,7 @@
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K115" t="inlineStr">
@@ -14503,7 +14503,7 @@
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K116" t="inlineStr">
@@ -14631,7 +14631,7 @@
       </c>
       <c r="J117" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K117" t="inlineStr">
@@ -15723,7 +15723,7 @@
       <c r="I126" t="inlineStr"/>
       <c r="J126" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K126" t="inlineStr">
@@ -15819,7 +15819,7 @@
       </c>
       <c r="J127" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K127" t="inlineStr">
@@ -15947,7 +15947,7 @@
       </c>
       <c r="J128" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K128" t="inlineStr">
@@ -16573,7 +16573,7 @@
       <c r="I133" t="inlineStr"/>
       <c r="J133" t="inlineStr">
         <is>
-          <t>['Portugal', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Portugal']</t>
         </is>
       </c>
       <c r="K133" t="inlineStr">
@@ -16669,7 +16669,7 @@
       </c>
       <c r="J134" t="inlineStr">
         <is>
-          <t>['Portugal', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Portugal']</t>
         </is>
       </c>
       <c r="K134" t="inlineStr">
@@ -16797,7 +16797,7 @@
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>['Portugal', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Portugal']</t>
         </is>
       </c>
       <c r="K135" t="inlineStr">
@@ -16925,7 +16925,7 @@
       </c>
       <c r="J136" t="inlineStr">
         <is>
-          <t>['Portugal', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Portugal']</t>
         </is>
       </c>
       <c r="K136" t="inlineStr">
@@ -17053,7 +17053,7 @@
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>['Portugal', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Portugal']</t>
         </is>
       </c>
       <c r="K137" t="inlineStr">
@@ -17181,7 +17181,7 @@
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>['Portugal', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Portugal']</t>
         </is>
       </c>
       <c r="K138" t="inlineStr">
@@ -17309,7 +17309,7 @@
       </c>
       <c r="J139" t="inlineStr">
         <is>
-          <t>['Portugal', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Portugal']</t>
         </is>
       </c>
       <c r="K139" t="inlineStr">
@@ -17437,7 +17437,7 @@
       </c>
       <c r="J140" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey']</t>
+          <t>['Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K140" t="inlineStr">
@@ -17551,7 +17551,7 @@
       <c r="I141" t="inlineStr"/>
       <c r="J141" t="inlineStr">
         <is>
-          <t>['Croatia', 'Germany']</t>
+          <t>['Germany', 'Croatia']</t>
         </is>
       </c>
       <c r="K141" t="inlineStr">
@@ -17647,7 +17647,7 @@
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>['Croatia', 'Germany']</t>
+          <t>['Germany', 'Croatia']</t>
         </is>
       </c>
       <c r="K142" t="inlineStr">
@@ -17775,7 +17775,7 @@
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>['Croatia', 'Germany']</t>
+          <t>['Germany', 'Croatia']</t>
         </is>
       </c>
       <c r="K143" t="inlineStr">
@@ -18483,7 +18483,7 @@
       <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K149" t="inlineStr">
@@ -18579,7 +18579,7 @@
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="K150" t="inlineStr">
@@ -18707,7 +18707,7 @@
       </c>
       <c r="J151" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="K151" t="inlineStr">
@@ -18835,7 +18835,7 @@
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="K152" t="inlineStr">
@@ -18963,7 +18963,7 @@
       </c>
       <c r="J153" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="K153" t="inlineStr">
@@ -19091,7 +19091,7 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>['Russia', 'Spain']</t>
+          <t>['Spain', 'Russia']</t>
         </is>
       </c>
       <c r="K154" t="inlineStr">
@@ -19205,7 +19205,7 @@
       <c r="I155" t="inlineStr"/>
       <c r="J155" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
@@ -19301,7 +19301,7 @@
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>['Russia', 'Greece']</t>
+          <t>['Greece', 'Russia']</t>
         </is>
       </c>
       <c r="K156" t="inlineStr">
@@ -19429,7 +19429,7 @@
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="K157" t="inlineStr">
@@ -19543,7 +19543,7 @@
       <c r="I158" t="inlineStr"/>
       <c r="J158" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany']</t>
+          <t>['Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K158" t="inlineStr">
@@ -19767,7 +19767,7 @@
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany']</t>
+          <t>['Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K160" t="inlineStr">
@@ -20023,7 +20023,7 @@
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany']</t>
+          <t>['Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K162" t="inlineStr">
@@ -20151,7 +20151,7 @@
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany']</t>
+          <t>['Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K163" t="inlineStr">
@@ -20279,7 +20279,7 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany']</t>
+          <t>['Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="K164" t="inlineStr">
@@ -20859,7 +20859,7 @@
       <c r="I169" t="inlineStr"/>
       <c r="J169" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K169" t="inlineStr">
@@ -20955,7 +20955,7 @@
       </c>
       <c r="J170" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K170" t="inlineStr">
@@ -21083,7 +21083,7 @@
       </c>
       <c r="J171" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K171" t="inlineStr">
@@ -21211,7 +21211,7 @@
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>['France', 'England']</t>
+          <t>['England', 'France']</t>
         </is>
       </c>
       <c r="K172" t="inlineStr">
@@ -21325,7 +21325,7 @@
       <c r="I173" t="inlineStr"/>
       <c r="J173" t="inlineStr">
         <is>
-          <t>['Romania', 'Switzerland', 'France']</t>
+          <t>['Switzerland', 'France']</t>
         </is>
       </c>
       <c r="K173" t="inlineStr">
@@ -21421,7 +21421,7 @@
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>['Albania', 'Switzerland', 'France']</t>
+          <t>['Switzerland', 'France']</t>
         </is>
       </c>
       <c r="K174" t="inlineStr">
@@ -21535,7 +21535,7 @@
       <c r="I175" t="inlineStr"/>
       <c r="J175" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Wales', 'England']</t>
+          <t>['England', 'Wales']</t>
         </is>
       </c>
       <c r="K175" t="inlineStr">
@@ -21631,7 +21631,7 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Wales', 'England']</t>
+          <t>['England', 'Wales']</t>
         </is>
       </c>
       <c r="K176" t="inlineStr">
@@ -21759,7 +21759,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Wales', 'England']</t>
+          <t>['England', 'Wales']</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -21887,7 +21887,7 @@
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Wales', 'England']</t>
+          <t>['England', 'Wales']</t>
         </is>
       </c>
       <c r="K178" t="inlineStr">
@@ -22001,7 +22001,7 @@
       <c r="I179" t="inlineStr"/>
       <c r="J179" t="inlineStr">
         <is>
-          <t>['Poland', 'Northern Ireland', 'Germany']</t>
+          <t>['Germany', 'Poland']</t>
         </is>
       </c>
       <c r="K179" t="inlineStr">
@@ -22097,7 +22097,7 @@
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>['Poland', 'Northern Ireland', 'Germany']</t>
+          <t>['Germany', 'Poland']</t>
         </is>
       </c>
       <c r="K180" t="inlineStr">
@@ -22225,7 +22225,7 @@
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>['Poland', 'Northern Ireland', 'Germany']</t>
+          <t>['Germany', 'Poland']</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
@@ -22339,7 +22339,7 @@
       <c r="I182" t="inlineStr"/>
       <c r="J182" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Spain', 'Croatia']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K182" t="inlineStr">
@@ -22435,7 +22435,7 @@
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Spain', 'Croatia']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K183" t="inlineStr">
@@ -22495,24 +22495,24 @@
         <v>1</v>
       </c>
       <c r="AA183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB183" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia']</t>
+          <t>['Spain', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="AC183" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD183" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE183" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="AF183" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AG183" t="n">
         <v>1818</v>
@@ -22563,7 +22563,7 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>['Turkey', 'Spain', 'Croatia']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
@@ -22634,7 +22634,7 @@
         <v>1</v>
       </c>
       <c r="AD184" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE184" t="n">
         <v>-2</v>
@@ -22691,7 +22691,7 @@
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>['Turkey', 'Spain', 'Croatia']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K185" t="inlineStr">
@@ -22762,7 +22762,7 @@
         <v>0</v>
       </c>
       <c r="AD185" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE185" t="n">
         <v>-2</v>
@@ -22819,7 +22819,7 @@
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>['Turkey', 'Spain', 'Croatia']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K186" t="inlineStr">
@@ -22890,7 +22890,7 @@
         <v>0</v>
       </c>
       <c r="AD186" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE186" t="n">
         <v>-2</v>
@@ -22947,7 +22947,7 @@
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>['Turkey', 'Spain', 'Croatia']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K187" t="inlineStr">
@@ -23018,7 +23018,7 @@
         <v>0</v>
       </c>
       <c r="AD187" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE187" t="n">
         <v>-2</v>
@@ -23061,7 +23061,7 @@
       <c r="I188" t="inlineStr"/>
       <c r="J188" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K188" t="inlineStr">
@@ -23097,11 +23097,11 @@
       <c r="Y188" t="inlineStr"/>
       <c r="Z188" t="inlineStr"/>
       <c r="AA188" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB188" t="inlineStr">
         <is>
-          <t>['Hungary', 'Iceland', 'Portugal']</t>
+          <t>['Hungary', 'Iceland']</t>
         </is>
       </c>
       <c r="AC188" t="n">
@@ -23157,7 +23157,7 @@
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K189" t="inlineStr">
@@ -23225,10 +23225,10 @@
         </is>
       </c>
       <c r="AC189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE189" t="n">
         <v>-2</v>
@@ -23285,7 +23285,7 @@
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
@@ -23356,7 +23356,7 @@
         <v>1</v>
       </c>
       <c r="AD190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE190" t="n">
         <v>-3</v>
@@ -23413,7 +23413,7 @@
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K191" t="inlineStr">
@@ -23484,7 +23484,7 @@
         <v>1</v>
       </c>
       <c r="AD191" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE191" t="n">
         <v>-2</v>
@@ -23541,7 +23541,7 @@
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K192" t="inlineStr">
@@ -23612,7 +23612,7 @@
         <v>1</v>
       </c>
       <c r="AD192" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE192" t="n">
         <v>-3</v>
@@ -23669,7 +23669,7 @@
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K193" t="inlineStr">
@@ -23740,7 +23740,7 @@
         <v>1</v>
       </c>
       <c r="AD193" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE193" t="n">
         <v>-2</v>
@@ -23797,7 +23797,7 @@
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
@@ -23868,7 +23868,7 @@
         <v>1</v>
       </c>
       <c r="AD194" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AE194" t="n">
         <v>-3</v>
@@ -23925,7 +23925,7 @@
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K195" t="inlineStr">
@@ -23996,7 +23996,7 @@
         <v>0</v>
       </c>
       <c r="AD195" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AE195" t="n">
         <v>-1</v>
@@ -24053,7 +24053,7 @@
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K196" t="inlineStr">
@@ -24124,7 +24124,7 @@
         <v>1</v>
       </c>
       <c r="AD196" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE196" t="n">
         <v>-1</v>
@@ -24181,7 +24181,7 @@
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K197" t="inlineStr">
@@ -24252,7 +24252,7 @@
         <v>0</v>
       </c>
       <c r="AD197" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE197" t="n">
         <v>-2</v>
@@ -24295,7 +24295,7 @@
       <c r="I198" t="inlineStr"/>
       <c r="J198" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium', 'Sweden']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K198" t="inlineStr">
@@ -24391,7 +24391,7 @@
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>['Ireland', 'Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K199" t="inlineStr">
@@ -24519,7 +24519,7 @@
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>['Ireland', 'Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K200" t="inlineStr">
@@ -24633,7 +24633,7 @@
       <c r="I201" t="inlineStr"/>
       <c r="J201" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Wales', 'Italy']</t>
+          <t>['Wales', 'Italy']</t>
         </is>
       </c>
       <c r="K201" t="inlineStr">
@@ -24729,7 +24729,7 @@
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Wales', 'Italy']</t>
+          <t>['Wales', 'Italy']</t>
         </is>
       </c>
       <c r="K202" t="inlineStr">
@@ -24857,7 +24857,7 @@
       </c>
       <c r="J203" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Wales', 'Italy']</t>
+          <t>['Wales', 'Italy']</t>
         </is>
       </c>
       <c r="K203" t="inlineStr">
@@ -24985,7 +24985,7 @@
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Wales', 'Italy']</t>
+          <t>['Wales', 'Italy']</t>
         </is>
       </c>
       <c r="K204" t="inlineStr">
@@ -25113,7 +25113,7 @@
       </c>
       <c r="J205" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Wales', 'Italy']</t>
+          <t>['Wales', 'Italy']</t>
         </is>
       </c>
       <c r="K205" t="inlineStr">
@@ -25241,7 +25241,7 @@
       </c>
       <c r="J206" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Wales', 'Italy']</t>
+          <t>['Wales', 'Italy']</t>
         </is>
       </c>
       <c r="K206" t="inlineStr">
@@ -25355,7 +25355,7 @@
       <c r="I207" t="inlineStr"/>
       <c r="J207" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'Ukraine']</t>
+          <t>['Ukraine', 'Netherlands']</t>
         </is>
       </c>
       <c r="K207" t="inlineStr">
@@ -25451,7 +25451,7 @@
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'Ukraine']</t>
+          <t>['Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K208" t="inlineStr">
@@ -25579,7 +25579,7 @@
       </c>
       <c r="J209" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'Ukraine']</t>
+          <t>['Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K209" t="inlineStr">
@@ -25707,7 +25707,7 @@
       </c>
       <c r="J210" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'Ukraine']</t>
+          <t>['Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K210" t="inlineStr">
@@ -25835,7 +25835,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'Ukraine']</t>
+          <t>['Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
@@ -25949,7 +25949,7 @@
       <c r="I212" t="inlineStr"/>
       <c r="J212" t="inlineStr">
         <is>
-          <t>['Russia', 'Finland', 'Belgium']</t>
+          <t>['Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K212" t="inlineStr">
@@ -26045,7 +26045,7 @@
       </c>
       <c r="J213" t="inlineStr">
         <is>
-          <t>['Finland', 'Denmark', 'Belgium']</t>
+          <t>['Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K213" t="inlineStr">
@@ -26173,7 +26173,7 @@
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>['Finland', 'Denmark', 'Belgium']</t>
+          <t>['Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K214" t="inlineStr">
@@ -26301,7 +26301,7 @@
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>['Finland', 'Denmark', 'Belgium']</t>
+          <t>['Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K215" t="inlineStr">
@@ -26429,7 +26429,7 @@
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>['Russia', 'Denmark', 'Belgium']</t>
+          <t>['Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="K216" t="inlineStr">
@@ -26557,7 +26557,7 @@
       </c>
       <c r="J217" t="inlineStr">
         <is>
-          <t>['Finland', 'Denmark', 'Belgium']</t>
+          <t>['Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="K217" t="inlineStr">
@@ -26685,7 +26685,7 @@
       </c>
       <c r="J218" t="inlineStr">
         <is>
-          <t>['Finland', 'Denmark', 'Belgium']</t>
+          <t>['Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="K218" t="inlineStr">
@@ -26813,7 +26813,7 @@
       </c>
       <c r="J219" t="inlineStr">
         <is>
-          <t>['Finland', 'Denmark', 'Belgium']</t>
+          <t>['Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="K219" t="inlineStr">
@@ -26927,7 +26927,7 @@
       <c r="I220" t="inlineStr"/>
       <c r="J220" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K220" t="inlineStr">
@@ -27023,7 +27023,7 @@
       </c>
       <c r="J221" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K221" t="inlineStr">
@@ -27151,7 +27151,7 @@
       </c>
       <c r="J222" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K222" t="inlineStr">
@@ -27279,7 +27279,7 @@
       </c>
       <c r="J223" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K223" t="inlineStr">
@@ -27407,7 +27407,7 @@
       </c>
       <c r="J224" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['England', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K224" t="inlineStr">
@@ -27535,7 +27535,7 @@
       </c>
       <c r="J225" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Croatia', 'England']</t>
+          <t>['England', 'Croatia']</t>
         </is>
       </c>
       <c r="K225" t="inlineStr">
@@ -27649,7 +27649,7 @@
       <c r="I226" t="inlineStr"/>
       <c r="J226" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K226" t="inlineStr">
@@ -27745,7 +27745,7 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K227" t="inlineStr">
@@ -27873,7 +27873,7 @@
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
@@ -27933,24 +27933,24 @@
         <v>0</v>
       </c>
       <c r="AA228" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB228" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="AC228" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD228" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE228" t="n">
         <v>-2</v>
       </c>
       <c r="AF228" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="AG228" t="n">
         <v>1656</v>
@@ -28001,7 +28001,7 @@
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
@@ -28061,24 +28061,24 @@
         <v>0</v>
       </c>
       <c r="AA229" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB229" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="AC229" t="n">
         <v>0</v>
       </c>
       <c r="AD229" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE229" t="n">
         <v>-2</v>
       </c>
       <c r="AF229" t="n">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="AG229" t="n">
         <v>1656</v>
@@ -28129,7 +28129,7 @@
       </c>
       <c r="J230" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K230" t="inlineStr">
@@ -28197,7 +28197,7 @@
         </is>
       </c>
       <c r="AC230" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD230" t="n">
         <v>1</v>
@@ -28257,7 +28257,7 @@
       </c>
       <c r="J231" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K231" t="inlineStr">
@@ -28385,7 +28385,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
@@ -28513,7 +28513,7 @@
       </c>
       <c r="J233" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K233" t="inlineStr">
@@ -28641,7 +28641,7 @@
       </c>
       <c r="J234" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K234" t="inlineStr">
@@ -28769,7 +28769,7 @@
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K235" t="inlineStr">
@@ -28897,7 +28897,7 @@
       </c>
       <c r="J236" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K236" t="inlineStr">
@@ -29011,7 +29011,7 @@
       <c r="I237" t="inlineStr"/>
       <c r="J237" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Germany']</t>
+          <t>['Portugal', 'France']</t>
         </is>
       </c>
       <c r="K237" t="inlineStr">
@@ -29047,11 +29047,11 @@
       <c r="Y237" t="inlineStr"/>
       <c r="Z237" t="inlineStr"/>
       <c r="AA237" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB237" t="inlineStr">
         <is>
-          <t>['France', 'Portugal', 'Germany']</t>
+          <t>['France', 'Portugal']</t>
         </is>
       </c>
       <c r="AC237" t="n">
@@ -29107,7 +29107,7 @@
       </c>
       <c r="J238" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France']</t>
         </is>
       </c>
       <c r="K238" t="inlineStr">
@@ -29235,7 +29235,7 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France']</t>
         </is>
       </c>
       <c r="K239" t="inlineStr">
@@ -29363,7 +29363,7 @@
       </c>
       <c r="J240" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France']</t>
         </is>
       </c>
       <c r="K240" t="inlineStr">
@@ -29491,7 +29491,7 @@
       </c>
       <c r="J241" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['France', 'Hungary']</t>
         </is>
       </c>
       <c r="K241" t="inlineStr">
@@ -29619,7 +29619,7 @@
       </c>
       <c r="J242" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France']</t>
         </is>
       </c>
       <c r="K242" t="inlineStr">
@@ -29747,7 +29747,7 @@
       </c>
       <c r="J243" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Germany']</t>
+          <t>['Portugal', 'France']</t>
         </is>
       </c>
       <c r="K243" t="inlineStr">
@@ -29875,7 +29875,7 @@
       </c>
       <c r="J244" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France']</t>
         </is>
       </c>
       <c r="K244" t="inlineStr">
@@ -30003,7 +30003,7 @@
       </c>
       <c r="J245" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Germany']</t>
+          <t>['Portugal', 'France']</t>
         </is>
       </c>
       <c r="K245" t="inlineStr">
@@ -30117,7 +30117,7 @@
       <c r="I246" t="inlineStr"/>
       <c r="J246" t="inlineStr">
         <is>
-          <t>['Scotland', 'Switzerland', 'Germany']</t>
+          <t>['Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="K246" t="inlineStr">
@@ -30213,7 +30213,7 @@
       </c>
       <c r="J247" t="inlineStr">
         <is>
-          <t>['Scotland', 'Switzerland', 'Germany']</t>
+          <t>['Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="K247" t="inlineStr">
@@ -30273,24 +30273,24 @@
         <v>1</v>
       </c>
       <c r="AA247" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB247" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Germany', 'Scotland']</t>
+          <t>['Switzerland', 'Germany']</t>
         </is>
       </c>
       <c r="AC247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE247" t="n">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="AF247" t="n">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="AG247" t="n">
         <v>1805</v>
@@ -30341,7 +30341,7 @@
       </c>
       <c r="J248" t="inlineStr">
         <is>
-          <t>['Scotland', 'Switzerland', 'Germany']</t>
+          <t>['Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="K248" t="inlineStr">
@@ -30401,24 +30401,24 @@
         <v>1</v>
       </c>
       <c r="AA248" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB248" t="inlineStr">
         <is>
-          <t>['Germany', 'Switzerland', 'Scotland']</t>
+          <t>['Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="AC248" t="n">
         <v>0</v>
       </c>
       <c r="AD248" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE248" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AF248" t="n">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="AG248" t="n">
         <v>1805</v>
@@ -30469,7 +30469,7 @@
       </c>
       <c r="J249" t="inlineStr">
         <is>
-          <t>['Hungary', 'Switzerland', 'Germany']</t>
+          <t>['Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="K249" t="inlineStr">
@@ -30540,7 +30540,7 @@
         <v>1</v>
       </c>
       <c r="AD249" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE249" t="n">
         <v>-2</v>
@@ -30583,7 +30583,7 @@
       <c r="I250" t="inlineStr"/>
       <c r="J250" t="inlineStr">
         <is>
-          <t>['Albania', 'Spain', 'Italy']</t>
+          <t>['Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K250" t="inlineStr">
@@ -30679,7 +30679,7 @@
       </c>
       <c r="J251" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain', 'Italy']</t>
+          <t>['Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K251" t="inlineStr">
@@ -30807,7 +30807,7 @@
       </c>
       <c r="J252" t="inlineStr">
         <is>
-          <t>['Italy', 'Spain', 'Croatia']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K252" t="inlineStr">
@@ -30935,7 +30935,7 @@
       </c>
       <c r="J253" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain', 'Italy']</t>
+          <t>['Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K253" t="inlineStr">
@@ -31049,7 +31049,7 @@
       <c r="I254" t="inlineStr"/>
       <c r="J254" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K254" t="inlineStr">
@@ -31085,11 +31085,11 @@
       <c r="Y254" t="inlineStr"/>
       <c r="Z254" t="inlineStr"/>
       <c r="AA254" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB254" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="AC254" t="n">
@@ -31145,7 +31145,7 @@
       </c>
       <c r="J255" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['Austria', 'France']</t>
         </is>
       </c>
       <c r="K255" t="inlineStr">
@@ -31213,10 +31213,10 @@
         </is>
       </c>
       <c r="AC255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE255" t="n">
         <v>-3</v>
@@ -31273,7 +31273,7 @@
       </c>
       <c r="J256" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K256" t="inlineStr">
@@ -31344,7 +31344,7 @@
         <v>0</v>
       </c>
       <c r="AD256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE256" t="n">
         <v>-3</v>
@@ -31401,7 +31401,7 @@
       </c>
       <c r="J257" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K257" t="inlineStr">
@@ -31472,7 +31472,7 @@
         <v>0</v>
       </c>
       <c r="AD257" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE257" t="n">
         <v>-4</v>
@@ -31529,7 +31529,7 @@
       </c>
       <c r="J258" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['Austria', 'France']</t>
         </is>
       </c>
       <c r="K258" t="inlineStr">
@@ -31600,7 +31600,7 @@
         <v>0</v>
       </c>
       <c r="AD258" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE258" t="n">
         <v>-4</v>
@@ -31657,7 +31657,7 @@
       </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K259" t="inlineStr">
@@ -31728,7 +31728,7 @@
         <v>0</v>
       </c>
       <c r="AD259" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE259" t="n">
         <v>-4</v>
@@ -31785,7 +31785,7 @@
       </c>
       <c r="J260" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K260" t="inlineStr">
@@ -31856,7 +31856,7 @@
         <v>0</v>
       </c>
       <c r="AD260" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE260" t="n">
         <v>-3</v>
@@ -31913,7 +31913,7 @@
       </c>
       <c r="J261" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['Austria', 'France']</t>
         </is>
       </c>
       <c r="K261" t="inlineStr">
@@ -31984,7 +31984,7 @@
         <v>0</v>
       </c>
       <c r="AD261" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE261" t="n">
         <v>-3</v>
@@ -32027,7 +32027,7 @@
       <c r="I262" t="inlineStr"/>
       <c r="J262" t="inlineStr">
         <is>
-          <t>['Slovenia', 'Denmark', 'England']</t>
+          <t>['England', 'Denmark']</t>
         </is>
       </c>
       <c r="K262" t="inlineStr">
@@ -32109,7 +32109,7 @@
       <c r="I263" t="inlineStr"/>
       <c r="J263" t="inlineStr">
         <is>
-          <t>['Romania', 'Slovakia', 'Belgium']</t>
+          <t>['Belgium', 'Romania']</t>
         </is>
       </c>
       <c r="K263" t="inlineStr">
@@ -32205,7 +32205,7 @@
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Belgium', 'Ukraine']</t>
+          <t>['Belgium', 'Slovakia']</t>
         </is>
       </c>
       <c r="K264" t="inlineStr">
@@ -32333,7 +32333,7 @@
       </c>
       <c r="J265" t="inlineStr">
         <is>
-          <t>['Romania', 'Slovakia', 'Belgium']</t>
+          <t>['Belgium', 'Romania']</t>
         </is>
       </c>
       <c r="K265" t="inlineStr">
@@ -32447,7 +32447,7 @@
       <c r="I266" t="inlineStr"/>
       <c r="J266" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Czech Republic']</t>
+          <t>['Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K266" t="inlineStr">
@@ -32543,7 +32543,7 @@
       </c>
       <c r="J267" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K267" t="inlineStr">
@@ -32671,7 +32671,7 @@
       </c>
       <c r="J268" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K268" t="inlineStr">
@@ -32799,7 +32799,7 @@
       </c>
       <c r="J269" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K269" t="inlineStr">
@@ -32927,7 +32927,7 @@
       </c>
       <c r="J270" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Georgia', 'Portugal']</t>
         </is>
       </c>
       <c r="K270" t="inlineStr">
@@ -33055,7 +33055,7 @@
       </c>
       <c r="J271" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K271" t="inlineStr">

</xml_diff>

<commit_message>
suspense tie three eu
evaluate suspense for three teams tied in European Championships
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
+++ b/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
@@ -683,7 +683,7 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['Denmark', 'France']</t>
+          <t>['France', 'Denmark']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>['Denmark', 'France']</t>
+          <t>['France', 'Denmark']</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>['Denmark', 'France']</t>
+          <t>['France', 'Denmark']</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>['Denmark', 'France']</t>
+          <t>['France', 'Denmark']</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>['Denmark', 'France']</t>
+          <t>['France', 'Denmark']</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -2259,7 +2259,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>['Denmark', 'France']</t>
+          <t>['France', 'Denmark']</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -2715,7 +2715,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal']</t>
+          <t>['Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -3631,7 +3631,7 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Ireland']</t>
+          <t>['Ireland', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -3895,7 +3895,7 @@
         <v>1976</v>
       </c>
       <c r="AQ22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR22" t="n">
         <v>1</v>
@@ -4053,7 +4053,7 @@
         <v>1976</v>
       </c>
       <c r="AQ23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR23" t="n">
         <v>1</v>
@@ -4211,7 +4211,7 @@
         <v>1976</v>
       </c>
       <c r="AQ24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR24" t="n">
         <v>1</v>
@@ -4369,7 +4369,7 @@
         <v>1976</v>
       </c>
       <c r="AQ25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR25" t="n">
         <v>1</v>
@@ -4417,7 +4417,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Netherlands']</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -4527,10 +4527,10 @@
         <v>1935</v>
       </c>
       <c r="AQ26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -4986,7 +4986,7 @@
         <v>0</v>
       </c>
       <c r="AR29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -5144,7 +5144,7 @@
         <v>0</v>
       </c>
       <c r="AR30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -5615,7 +5615,7 @@
         <v>2006</v>
       </c>
       <c r="AQ33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR33" t="n">
         <v>1</v>
@@ -5916,7 +5916,7 @@
         <v>0</v>
       </c>
       <c r="AR35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -6895,7 +6895,7 @@
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'France']</t>
+          <t>['France', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -7159,10 +7159,10 @@
         <v>1990</v>
       </c>
       <c r="AQ43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -7207,7 +7207,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>['Spain', 'France']</t>
+          <t>['France', 'Spain']</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -7320,7 +7320,7 @@
         <v>0</v>
       </c>
       <c r="AR44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -7365,7 +7365,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'France']</t>
+          <t>['France', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -7523,7 +7523,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'France']</t>
+          <t>['France', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -7681,7 +7681,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'France']</t>
+          <t>['France', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -7839,7 +7839,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>['Spain', 'France']</t>
+          <t>['France', 'Spain']</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -7952,7 +7952,7 @@
         <v>0</v>
       </c>
       <c r="AR48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -7997,7 +7997,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>['Spain', 'France']</t>
+          <t>['France', 'Spain']</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -8882,7 +8882,7 @@
         <v>0</v>
       </c>
       <c r="AR54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -9198,7 +9198,7 @@
         <v>0</v>
       </c>
       <c r="AR56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -12489,7 +12489,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>['Portugal', 'Romania']</t>
+          <t>['Romania', 'Portugal']</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -12599,7 +12599,7 @@
         <v>1856</v>
       </c>
       <c r="AQ78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR78" t="n">
         <v>1</v>
@@ -12647,7 +12647,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>['Portugal', 'Romania']</t>
+          <t>['Romania', 'Portugal']</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -12757,7 +12757,7 @@
         <v>1889</v>
       </c>
       <c r="AQ79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR79" t="n">
         <v>1</v>
@@ -12915,10 +12915,10 @@
         <v>1856</v>
       </c>
       <c r="AQ80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -13073,7 +13073,7 @@
         <v>1856</v>
       </c>
       <c r="AQ81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR81" t="n">
         <v>0</v>
@@ -13231,10 +13231,10 @@
         <v>1856</v>
       </c>
       <c r="AQ82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -13389,10 +13389,10 @@
         <v>1889</v>
       </c>
       <c r="AQ83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -13547,10 +13547,10 @@
         <v>1889</v>
       </c>
       <c r="AQ84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -13595,7 +13595,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>['Portugal', 'Romania']</t>
+          <t>['Romania', 'Portugal']</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -13705,7 +13705,7 @@
         <v>1856</v>
       </c>
       <c r="AQ85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR85" t="n">
         <v>1</v>
@@ -14164,7 +14164,7 @@
         <v>0</v>
       </c>
       <c r="AR88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -14480,7 +14480,7 @@
         <v>0</v>
       </c>
       <c r="AR90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -14796,7 +14796,7 @@
         <v>0</v>
       </c>
       <c r="AR92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -14954,7 +14954,7 @@
         <v>0</v>
       </c>
       <c r="AR93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -16385,7 +16385,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal']</t>
+          <t>['Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -16495,7 +16495,7 @@
         <v>1796</v>
       </c>
       <c r="AQ103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR103" t="n">
         <v>1</v>
@@ -16543,7 +16543,7 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal']</t>
+          <t>['Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
@@ -16653,10 +16653,10 @@
         <v>1796</v>
       </c>
       <c r="AQ104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -16701,7 +16701,7 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal']</t>
+          <t>['Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
@@ -16811,7 +16811,7 @@
         <v>1796</v>
       </c>
       <c r="AQ105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR105" t="n">
         <v>1</v>
@@ -16969,7 +16969,7 @@
         <v>1899</v>
       </c>
       <c r="AQ106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR106" t="n">
         <v>1</v>
@@ -17003,7 +17003,7 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
@@ -17157,7 +17157,7 @@
       </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>['Croatia', 'France']</t>
+          <t>['France', 'Croatia']</t>
         </is>
       </c>
       <c r="K108" t="inlineStr">
@@ -17315,7 +17315,7 @@
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>['Croatia', 'France']</t>
+          <t>['France', 'Croatia']</t>
         </is>
       </c>
       <c r="K109" t="inlineStr">
@@ -17473,7 +17473,7 @@
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t>['Croatia', 'France']</t>
+          <t>['France', 'Croatia']</t>
         </is>
       </c>
       <c r="K110" t="inlineStr">
@@ -17631,7 +17631,7 @@
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K111" t="inlineStr">
@@ -17899,7 +17899,7 @@
         <v>1939</v>
       </c>
       <c r="AQ112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR112" t="n">
         <v>0</v>
@@ -18057,7 +18057,7 @@
         <v>1939</v>
       </c>
       <c r="AQ113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR113" t="n">
         <v>0</v>
@@ -18215,7 +18215,7 @@
         <v>1939</v>
       </c>
       <c r="AQ114" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR114" t="n">
         <v>0</v>
@@ -18263,7 +18263,7 @@
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K115" t="inlineStr">
@@ -18421,7 +18421,7 @@
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K116" t="inlineStr">
@@ -18579,7 +18579,7 @@
       </c>
       <c r="J117" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K117" t="inlineStr">
@@ -21324,7 +21324,7 @@
         <v>1</v>
       </c>
       <c r="AR134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
@@ -21637,7 +21637,7 @@
         <v>1860</v>
       </c>
       <c r="AQ136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR136" t="n">
         <v>0</v>
@@ -21795,7 +21795,7 @@
         <v>1921</v>
       </c>
       <c r="AQ137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR137" t="n">
         <v>0</v>
@@ -21953,7 +21953,7 @@
         <v>1860</v>
       </c>
       <c r="AQ138" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR138" t="n">
         <v>0</v>
@@ -22269,7 +22269,7 @@
         <v>1921</v>
       </c>
       <c r="AQ140" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR140" t="n">
         <v>0</v>
@@ -22567,7 +22567,7 @@
         <v>1961</v>
       </c>
       <c r="AQ142" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR142" t="n">
         <v>0</v>
@@ -22759,7 +22759,7 @@
       <c r="I144" t="inlineStr"/>
       <c r="J144" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Romania']</t>
+          <t>['Romania', 'Netherlands']</t>
         </is>
       </c>
       <c r="K144" t="inlineStr">
@@ -23531,7 +23531,7 @@
       <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="K149" t="inlineStr">
@@ -24615,7 +24615,7 @@
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>['Greece', 'Russia']</t>
+          <t>['Russia', 'Greece']</t>
         </is>
       </c>
       <c r="K156" t="inlineStr">
@@ -24725,7 +24725,7 @@
         <v>1850</v>
       </c>
       <c r="AQ156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR156" t="n">
         <v>1</v>
@@ -25342,7 +25342,7 @@
         <v>0</v>
       </c>
       <c r="AR160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -25658,7 +25658,7 @@
         <v>0</v>
       </c>
       <c r="AR162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
@@ -26005,7 +26005,7 @@
       <c r="I165" t="inlineStr"/>
       <c r="J165" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia']</t>
+          <t>['Croatia', 'Spain']</t>
         </is>
       </c>
       <c r="K165" t="inlineStr">
@@ -26269,10 +26269,10 @@
         <v>1805</v>
       </c>
       <c r="AQ166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167">
@@ -26619,7 +26619,7 @@
       <c r="I169" t="inlineStr"/>
       <c r="J169" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="K169" t="inlineStr">
@@ -26883,10 +26883,10 @@
         <v>1756</v>
       </c>
       <c r="AQ170" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR170" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -27233,7 +27233,7 @@
       <c r="I173" t="inlineStr"/>
       <c r="J173" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Romania', 'France']</t>
+          <t>['Romania', 'France', 'Switzerland']</t>
         </is>
       </c>
       <c r="K173" t="inlineStr">
@@ -27387,7 +27387,7 @@
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Albania', 'France']</t>
+          <t>['France', 'Switzerland', 'Albania']</t>
         </is>
       </c>
       <c r="K174" t="inlineStr">
@@ -28145,7 +28145,7 @@
       <c r="I179" t="inlineStr"/>
       <c r="J179" t="inlineStr">
         <is>
-          <t>['Poland', 'Northern Ireland', 'Germany']</t>
+          <t>['Northern Ireland', 'Poland', 'Germany']</t>
         </is>
       </c>
       <c r="K179" t="inlineStr">
@@ -28299,7 +28299,7 @@
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>['Poland', 'Northern Ireland', 'Germany']</t>
+          <t>['Northern Ireland', 'Poland', 'Germany']</t>
         </is>
       </c>
       <c r="K180" t="inlineStr">
@@ -28457,7 +28457,7 @@
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>['Poland', 'Northern Ireland', 'Germany']</t>
+          <t>['Northern Ireland', 'Poland', 'Germany']</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
@@ -28601,7 +28601,7 @@
       <c r="I182" t="inlineStr"/>
       <c r="J182" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Czech Republic']</t>
+          <t>['Croatia', 'Czech Republic', 'Spain']</t>
         </is>
       </c>
       <c r="K182" t="inlineStr">
@@ -28755,7 +28755,7 @@
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Czech Republic']</t>
+          <t>['Croatia', 'Czech Republic', 'Spain']</t>
         </is>
       </c>
       <c r="K183" t="inlineStr">
@@ -28865,10 +28865,10 @@
         <v>1993</v>
       </c>
       <c r="AQ183" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184">
@@ -28913,7 +28913,7 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Turkey']</t>
+          <t>['Croatia', 'Spain', 'Turkey']</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
@@ -29071,7 +29071,7 @@
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Turkey']</t>
+          <t>['Croatia', 'Spain', 'Turkey']</t>
         </is>
       </c>
       <c r="K185" t="inlineStr">
@@ -29229,7 +29229,7 @@
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Turkey']</t>
+          <t>['Croatia', 'Spain', 'Turkey']</t>
         </is>
       </c>
       <c r="K186" t="inlineStr">
@@ -29387,7 +29387,7 @@
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Turkey']</t>
+          <t>['Croatia', 'Spain', 'Turkey']</t>
         </is>
       </c>
       <c r="K187" t="inlineStr">
@@ -29531,7 +29531,7 @@
       <c r="I188" t="inlineStr"/>
       <c r="J188" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K188" t="inlineStr">
@@ -29685,7 +29685,7 @@
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K189" t="inlineStr">
@@ -29843,7 +29843,7 @@
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
@@ -30001,7 +30001,7 @@
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K191" t="inlineStr">
@@ -30159,7 +30159,7 @@
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K192" t="inlineStr">
@@ -30317,7 +30317,7 @@
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K193" t="inlineStr">
@@ -30475,7 +30475,7 @@
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
@@ -30633,7 +30633,7 @@
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K195" t="inlineStr">
@@ -30791,7 +30791,7 @@
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K196" t="inlineStr">
@@ -30901,7 +30901,7 @@
         <v>1910</v>
       </c>
       <c r="AQ196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR196" t="n">
         <v>1</v>
@@ -30949,7 +30949,7 @@
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'Iceland']</t>
+          <t>['Iceland', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="K197" t="inlineStr">
@@ -31093,7 +31093,7 @@
       <c r="I198" t="inlineStr"/>
       <c r="J198" t="inlineStr">
         <is>
-          <t>['Sweden', 'Belgium', 'Italy']</t>
+          <t>['Belgium', 'Sweden', 'Italy']</t>
         </is>
       </c>
       <c r="K198" t="inlineStr">
@@ -31405,7 +31405,7 @@
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>['Italy', 'Ireland', 'Belgium']</t>
+          <t>['Belgium', 'Ireland', 'Italy']</t>
         </is>
       </c>
       <c r="K200" t="inlineStr">
@@ -32479,7 +32479,7 @@
       <c r="I207" t="inlineStr"/>
       <c r="J207" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'Ukraine']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K207" t="inlineStr">
@@ -32633,7 +32633,7 @@
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'Ukraine']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K208" t="inlineStr">
@@ -32791,7 +32791,7 @@
       </c>
       <c r="J209" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'Ukraine']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K209" t="inlineStr">
@@ -32949,7 +32949,7 @@
       </c>
       <c r="J210" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'Ukraine']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K210" t="inlineStr">
@@ -33107,7 +33107,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'Ukraine']</t>
+          <t>['Ukraine', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
@@ -33251,7 +33251,7 @@
       <c r="I212" t="inlineStr"/>
       <c r="J212" t="inlineStr">
         <is>
-          <t>['Russia', 'Belgium', 'Finland']</t>
+          <t>['Belgium', 'Finland', 'Russia']</t>
         </is>
       </c>
       <c r="K212" t="inlineStr">
@@ -33405,7 +33405,7 @@
       </c>
       <c r="J213" t="inlineStr">
         <is>
-          <t>['Denmark', 'Belgium', 'Finland']</t>
+          <t>['Belgium', 'Finland', 'Denmark']</t>
         </is>
       </c>
       <c r="K213" t="inlineStr">
@@ -33563,7 +33563,7 @@
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>['Denmark', 'Belgium', 'Finland']</t>
+          <t>['Belgium', 'Finland', 'Denmark']</t>
         </is>
       </c>
       <c r="K214" t="inlineStr">
@@ -33721,7 +33721,7 @@
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>['Denmark', 'Belgium', 'Finland']</t>
+          <t>['Belgium', 'Finland', 'Denmark']</t>
         </is>
       </c>
       <c r="K215" t="inlineStr">
@@ -33879,7 +33879,7 @@
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>['Denmark', 'Belgium', 'Russia']</t>
+          <t>['Belgium', 'Russia', 'Denmark']</t>
         </is>
       </c>
       <c r="K216" t="inlineStr">
@@ -33989,7 +33989,7 @@
         <v>2100</v>
       </c>
       <c r="AQ216" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR216" t="n">
         <v>1</v>
@@ -34037,7 +34037,7 @@
       </c>
       <c r="J217" t="inlineStr">
         <is>
-          <t>['Denmark', 'Belgium', 'Finland']</t>
+          <t>['Belgium', 'Finland', 'Denmark']</t>
         </is>
       </c>
       <c r="K217" t="inlineStr">
@@ -34147,10 +34147,10 @@
         <v>1973</v>
       </c>
       <c r="AQ217" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218">
@@ -34195,7 +34195,7 @@
       </c>
       <c r="J218" t="inlineStr">
         <is>
-          <t>['Denmark', 'Belgium', 'Finland']</t>
+          <t>['Belgium', 'Finland', 'Denmark']</t>
         </is>
       </c>
       <c r="K218" t="inlineStr">
@@ -34305,10 +34305,10 @@
         <v>2100</v>
       </c>
       <c r="AQ218" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR218" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219">
@@ -34353,7 +34353,7 @@
       </c>
       <c r="J219" t="inlineStr">
         <is>
-          <t>['Denmark', 'Belgium', 'Finland']</t>
+          <t>['Belgium', 'Finland', 'Denmark']</t>
         </is>
       </c>
       <c r="K219" t="inlineStr">
@@ -34463,10 +34463,10 @@
         <v>1973</v>
       </c>
       <c r="AQ219" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220">
@@ -34761,10 +34761,10 @@
         <v>1982</v>
       </c>
       <c r="AQ221" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR221" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222">
@@ -35077,10 +35077,10 @@
         <v>1678</v>
       </c>
       <c r="AQ223" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR223" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224">
@@ -35393,7 +35393,7 @@
         <v>1678</v>
       </c>
       <c r="AQ225" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR225" t="n">
         <v>0</v>
@@ -35427,7 +35427,7 @@
       <c r="I226" t="inlineStr"/>
       <c r="J226" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="K226" t="inlineStr">
@@ -35581,7 +35581,7 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="K227" t="inlineStr">
@@ -35739,7 +35739,7 @@
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
@@ -35849,10 +35849,10 @@
         <v>2033</v>
       </c>
       <c r="AQ228" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR228" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229">
@@ -35897,7 +35897,7 @@
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
@@ -36007,7 +36007,7 @@
         <v>2033</v>
       </c>
       <c r="AQ229" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR229" t="n">
         <v>0</v>
@@ -36055,7 +36055,7 @@
       </c>
       <c r="J230" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="K230" t="inlineStr">
@@ -36165,7 +36165,7 @@
         <v>2033</v>
       </c>
       <c r="AQ230" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR230" t="n">
         <v>0</v>
@@ -36213,7 +36213,7 @@
       </c>
       <c r="J231" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="K231" t="inlineStr">
@@ -36323,7 +36323,7 @@
         <v>1796</v>
       </c>
       <c r="AQ231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR231" t="n">
         <v>0</v>
@@ -36371,7 +36371,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
@@ -36481,7 +36481,7 @@
         <v>1796</v>
       </c>
       <c r="AQ232" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR232" t="n">
         <v>0</v>
@@ -36529,7 +36529,7 @@
       </c>
       <c r="J233" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="K233" t="inlineStr">
@@ -36639,7 +36639,7 @@
         <v>2033</v>
       </c>
       <c r="AQ233" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR233" t="n">
         <v>0</v>
@@ -36687,7 +36687,7 @@
       </c>
       <c r="J234" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="K234" t="inlineStr">
@@ -36797,7 +36797,7 @@
         <v>2033</v>
       </c>
       <c r="AQ234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR234" t="n">
         <v>0</v>
@@ -36845,7 +36845,7 @@
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="K235" t="inlineStr">
@@ -37003,7 +37003,7 @@
       </c>
       <c r="J236" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="K236" t="inlineStr">
@@ -37113,7 +37113,7 @@
         <v>1796</v>
       </c>
       <c r="AQ236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR236" t="n">
         <v>0</v>
@@ -37147,7 +37147,7 @@
       <c r="I237" t="inlineStr"/>
       <c r="J237" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany', 'France']</t>
+          <t>['Portugal', 'France', 'Germany']</t>
         </is>
       </c>
       <c r="K237" t="inlineStr">
@@ -37301,7 +37301,7 @@
       </c>
       <c r="J238" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K238" t="inlineStr">
@@ -37459,7 +37459,7 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K239" t="inlineStr">
@@ -37617,7 +37617,7 @@
       </c>
       <c r="J240" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K240" t="inlineStr">
@@ -37775,7 +37775,7 @@
       </c>
       <c r="J241" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K241" t="inlineStr">
@@ -37885,7 +37885,7 @@
         <v>2087</v>
       </c>
       <c r="AQ241" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR241" t="n">
         <v>1</v>
@@ -37933,7 +37933,7 @@
       </c>
       <c r="J242" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K242" t="inlineStr">
@@ -38091,7 +38091,7 @@
       </c>
       <c r="J243" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany', 'France']</t>
+          <t>['Portugal', 'France', 'Germany']</t>
         </is>
       </c>
       <c r="K243" t="inlineStr">
@@ -38249,7 +38249,7 @@
       </c>
       <c r="J244" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['Portugal', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K244" t="inlineStr">
@@ -38407,7 +38407,7 @@
       </c>
       <c r="J245" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany', 'France']</t>
+          <t>['Portugal', 'France', 'Germany']</t>
         </is>
       </c>
       <c r="K245" t="inlineStr">
@@ -38551,7 +38551,7 @@
       <c r="I246" t="inlineStr"/>
       <c r="J246" t="inlineStr">
         <is>
-          <t>['Scotland', 'Switzerland', 'Germany']</t>
+          <t>['Switzerland', 'Scotland', 'Germany']</t>
         </is>
       </c>
       <c r="K246" t="inlineStr">
@@ -38705,7 +38705,7 @@
       </c>
       <c r="J247" t="inlineStr">
         <is>
-          <t>['Scotland', 'Switzerland', 'Germany']</t>
+          <t>['Switzerland', 'Scotland', 'Germany']</t>
         </is>
       </c>
       <c r="K247" t="inlineStr">
@@ -38863,7 +38863,7 @@
       </c>
       <c r="J248" t="inlineStr">
         <is>
-          <t>['Scotland', 'Switzerland', 'Germany']</t>
+          <t>['Switzerland', 'Scotland', 'Germany']</t>
         </is>
       </c>
       <c r="K248" t="inlineStr">
@@ -39165,7 +39165,7 @@
       <c r="I250" t="inlineStr"/>
       <c r="J250" t="inlineStr">
         <is>
-          <t>['Spain', 'Albania', 'Italy']</t>
+          <t>['Albania', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K250" t="inlineStr">
@@ -39319,7 +39319,7 @@
       </c>
       <c r="J251" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Italy']</t>
+          <t>['Croatia', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K251" t="inlineStr">
@@ -39429,10 +39429,10 @@
         <v>2020</v>
       </c>
       <c r="AQ251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252">
@@ -39477,7 +39477,7 @@
       </c>
       <c r="J252" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Italy']</t>
+          <t>['Croatia', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K252" t="inlineStr">
@@ -39635,7 +39635,7 @@
       </c>
       <c r="J253" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Italy']</t>
+          <t>['Croatia', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K253" t="inlineStr">
@@ -39745,10 +39745,10 @@
         <v>1949</v>
       </c>
       <c r="AQ253" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR253" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="254">
@@ -39779,7 +39779,7 @@
       <c r="I254" t="inlineStr"/>
       <c r="J254" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'France']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K254" t="inlineStr">
@@ -39933,7 +39933,7 @@
       </c>
       <c r="J255" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'France']</t>
+          <t>['Netherlands', 'Austria', 'France']</t>
         </is>
       </c>
       <c r="K255" t="inlineStr">
@@ -40091,7 +40091,7 @@
       </c>
       <c r="J256" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'France']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K256" t="inlineStr">
@@ -40249,7 +40249,7 @@
       </c>
       <c r="J257" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'France']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K257" t="inlineStr">
@@ -40407,7 +40407,7 @@
       </c>
       <c r="J258" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'France']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K258" t="inlineStr">
@@ -40565,7 +40565,7 @@
       </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'France']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K259" t="inlineStr">
@@ -40723,7 +40723,7 @@
       </c>
       <c r="J260" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'France']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K260" t="inlineStr">
@@ -40881,7 +40881,7 @@
       </c>
       <c r="J261" t="inlineStr">
         <is>
-          <t>['Austria', 'Netherlands', 'France']</t>
+          <t>['Netherlands', 'Austria', 'France']</t>
         </is>
       </c>
       <c r="K261" t="inlineStr">
@@ -41025,7 +41025,7 @@
       <c r="I262" t="inlineStr"/>
       <c r="J262" t="inlineStr">
         <is>
-          <t>['Denmark', 'Slovenia', 'England']</t>
+          <t>['Slovenia', 'England', 'Denmark']</t>
         </is>
       </c>
       <c r="K262" t="inlineStr">
@@ -41165,7 +41165,7 @@
       <c r="I263" t="inlineStr"/>
       <c r="J263" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Romania', 'Belgium']</t>
+          <t>['Romania', 'Slovakia', 'Belgium']</t>
         </is>
       </c>
       <c r="K263" t="inlineStr">
@@ -41319,7 +41319,7 @@
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Ukraine', 'Belgium']</t>
+          <t>['Belgium', 'Ukraine', 'Slovakia']</t>
         </is>
       </c>
       <c r="K264" t="inlineStr">
@@ -41477,7 +41477,7 @@
       </c>
       <c r="J265" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Romania', 'Belgium']</t>
+          <t>['Romania', 'Slovakia', 'Belgium']</t>
         </is>
       </c>
       <c r="K265" t="inlineStr">
@@ -41590,7 +41590,7 @@
         <v>0</v>
       </c>
       <c r="AR265" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="266">
@@ -41775,7 +41775,7 @@
       </c>
       <c r="J267" t="inlineStr">
         <is>
-          <t>['Portugal', 'Georgia', 'Turkey']</t>
+          <t>['Georgia', 'Portugal', 'Turkey']</t>
         </is>
       </c>
       <c r="K267" t="inlineStr">
@@ -41933,7 +41933,7 @@
       </c>
       <c r="J268" t="inlineStr">
         <is>
-          <t>['Portugal', 'Georgia', 'Turkey']</t>
+          <t>['Georgia', 'Portugal', 'Turkey']</t>
         </is>
       </c>
       <c r="K268" t="inlineStr">
@@ -42091,7 +42091,7 @@
       </c>
       <c r="J269" t="inlineStr">
         <is>
-          <t>['Portugal', 'Georgia', 'Turkey']</t>
+          <t>['Georgia', 'Portugal', 'Turkey']</t>
         </is>
       </c>
       <c r="K269" t="inlineStr">
@@ -42359,7 +42359,7 @@
         <v>1749</v>
       </c>
       <c r="AQ270" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR270" t="n">
         <v>1</v>
@@ -42407,7 +42407,7 @@
       </c>
       <c r="J271" t="inlineStr">
         <is>
-          <t>['Portugal', 'Georgia', 'Turkey']</t>
+          <t>['Georgia', 'Portugal', 'Turkey']</t>
         </is>
       </c>
       <c r="K271" t="inlineStr">

</xml_diff>

<commit_message>
update eu fifa cases
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
+++ b/data/out/wiki/men/fifa/eu/goals_eu_fifa_men.xlsx
@@ -837,7 +837,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['Belgium', 'France']</t>
+          <t>['France', 'Belgium']</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -995,7 +995,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['Belgium', 'France']</t>
+          <t>['France', 'Belgium']</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>['Belgium', 'France']</t>
+          <t>['France', 'Belgium']</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['Belgium', 'France']</t>
+          <t>['France', 'Belgium']</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['Belgium', 'France']</t>
+          <t>['France', 'Belgium']</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -2715,7 +2715,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -3631,7 +3631,7 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
-          <t>['Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Ireland']</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -3785,7 +3785,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Ireland']</t>
+          <t>['Ireland', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -3943,7 +3943,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Ireland']</t>
+          <t>['Ireland', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -4101,7 +4101,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Ireland']</t>
+          <t>['Ireland', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -4259,7 +4259,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Ireland']</t>
+          <t>['Ireland', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -4417,7 +4417,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Netherlands']</t>
+          <t>['Netherlands', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -4561,7 +4561,7 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
-          <t>['Sweden', 'France']</t>
+          <t>['France', 'Sweden']</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -4715,7 +4715,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -4873,7 +4873,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -5031,7 +5031,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>['Sweden', 'France']</t>
+          <t>['France', 'Sweden']</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -5347,7 +5347,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -5505,7 +5505,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -7207,7 +7207,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>['France', 'Spain']</t>
+          <t>['Spain', 'France']</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -7839,7 +7839,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>['France', 'Spain']</t>
+          <t>['Spain', 'France']</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -7997,7 +7997,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>['France', 'Spain']</t>
+          <t>['Spain', 'France']</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -10317,7 +10317,7 @@
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr">
         <is>
-          <t>['Italy', 'Germany']</t>
+          <t>['Germany', 'Italy']</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -10471,7 +10471,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -10629,7 +10629,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -10787,7 +10787,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -10945,7 +10945,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>['Italy', 'Germany']</t>
+          <t>['Germany', 'Italy']</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -11103,7 +11103,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>['Italy', 'Germany']</t>
+          <t>['Germany', 'Italy']</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -11261,7 +11261,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>['Italy', 'Germany']</t>
+          <t>['Germany', 'Italy']</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -12489,7 +12489,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>['Romania', 'Portugal']</t>
+          <t>['Portugal', 'Romania']</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -12647,7 +12647,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>['Romania', 'Portugal']</t>
+          <t>['Portugal', 'Romania']</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -13595,7 +13595,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>['Romania', 'Portugal']</t>
+          <t>['Portugal', 'Romania']</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -13893,7 +13893,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>['Norway', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Norway']</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -14209,7 +14209,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>['Norway', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Norway']</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
@@ -14525,7 +14525,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>['Norway', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Norway']</t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
@@ -16231,7 +16231,7 @@
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr">
         <is>
-          <t>['Spain', 'Greece']</t>
+          <t>['Greece', 'Spain']</t>
         </is>
       </c>
       <c r="K102" t="inlineStr">
@@ -16385,7 +16385,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -16543,7 +16543,7 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
@@ -16701,7 +16701,7 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
@@ -16859,7 +16859,7 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>['Portugal', 'Greece']</t>
+          <t>['Greece', 'Portugal']</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
@@ -18723,7 +18723,7 @@
       <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="K118" t="inlineStr">
@@ -18877,7 +18877,7 @@
       </c>
       <c r="J119" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="K119" t="inlineStr">
@@ -19035,7 +19035,7 @@
       </c>
       <c r="J120" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="K120" t="inlineStr">
@@ -19193,7 +19193,7 @@
       </c>
       <c r="J121" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="K121" t="inlineStr">
@@ -19351,7 +19351,7 @@
       </c>
       <c r="J122" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="K122" t="inlineStr">
@@ -19509,7 +19509,7 @@
       </c>
       <c r="J123" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="K123" t="inlineStr">
@@ -19667,7 +19667,7 @@
       </c>
       <c r="J124" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="K124" t="inlineStr">
@@ -19825,7 +19825,7 @@
       </c>
       <c r="J125" t="inlineStr">
         <is>
-          <t>['Sweden', 'Denmark']</t>
+          <t>['Denmark', 'Sweden']</t>
         </is>
       </c>
       <c r="K125" t="inlineStr">
@@ -19969,7 +19969,7 @@
       <c r="I126" t="inlineStr"/>
       <c r="J126" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K126" t="inlineStr">
@@ -20123,7 +20123,7 @@
       </c>
       <c r="J127" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K127" t="inlineStr">
@@ -20281,7 +20281,7 @@
       </c>
       <c r="J128" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K128" t="inlineStr">
@@ -22303,7 +22303,7 @@
       <c r="I141" t="inlineStr"/>
       <c r="J141" t="inlineStr">
         <is>
-          <t>['Croatia', 'Germany']</t>
+          <t>['Germany', 'Croatia']</t>
         </is>
       </c>
       <c r="K141" t="inlineStr">
@@ -22457,7 +22457,7 @@
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>['Croatia', 'Germany']</t>
+          <t>['Germany', 'Croatia']</t>
         </is>
       </c>
       <c r="K142" t="inlineStr">
@@ -22615,7 +22615,7 @@
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>['Croatia', 'Germany']</t>
+          <t>['Germany', 'Croatia']</t>
         </is>
       </c>
       <c r="K143" t="inlineStr">
@@ -22759,7 +22759,7 @@
       <c r="I144" t="inlineStr"/>
       <c r="J144" t="inlineStr">
         <is>
-          <t>['Romania', 'Netherlands']</t>
+          <t>['Netherlands', 'Romania']</t>
         </is>
       </c>
       <c r="K144" t="inlineStr">
@@ -23531,7 +23531,7 @@
       <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K149" t="inlineStr">
@@ -24461,7 +24461,7 @@
       <c r="I155" t="inlineStr"/>
       <c r="J155" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Russia']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
@@ -24615,7 +24615,7 @@
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>['Russia', 'Greece']</t>
+          <t>['Greece', 'Russia']</t>
         </is>
       </c>
       <c r="K156" t="inlineStr">
@@ -24773,7 +24773,7 @@
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Russia']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K157" t="inlineStr">
@@ -25071,7 +25071,7 @@
       </c>
       <c r="J159" t="inlineStr">
         <is>
-          <t>['Denmark', 'Germany']</t>
+          <t>['Germany', 'Denmark']</t>
         </is>
       </c>
       <c r="K159" t="inlineStr">
@@ -25387,7 +25387,7 @@
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>['Denmark', 'Germany']</t>
+          <t>['Germany', 'Denmark']</t>
         </is>
       </c>
       <c r="K161" t="inlineStr">
@@ -26005,7 +26005,7 @@
       <c r="I165" t="inlineStr"/>
       <c r="J165" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K165" t="inlineStr">
@@ -26114,7 +26114,7 @@
         <v>0</v>
       </c>
       <c r="AR165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166">
@@ -27233,7 +27233,7 @@
       <c r="I173" t="inlineStr"/>
       <c r="J173" t="inlineStr">
         <is>
-          <t>['Romania', 'France', 'Switzerland']</t>
+          <t>['France', 'Romania', 'Switzerland']</t>
         </is>
       </c>
       <c r="K173" t="inlineStr">
@@ -27387,7 +27387,7 @@
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>['France', 'Switzerland', 'Albania']</t>
+          <t>['France', 'Albania', 'Switzerland']</t>
         </is>
       </c>
       <c r="K174" t="inlineStr">
@@ -27531,7 +27531,7 @@
       <c r="I175" t="inlineStr"/>
       <c r="J175" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Wales', 'England']</t>
+          <t>['Wales', 'Slovakia', 'England']</t>
         </is>
       </c>
       <c r="K175" t="inlineStr">
@@ -27685,7 +27685,7 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Wales', 'England']</t>
+          <t>['Wales', 'Slovakia', 'England']</t>
         </is>
       </c>
       <c r="K176" t="inlineStr">
@@ -27843,7 +27843,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Wales', 'England']</t>
+          <t>['Wales', 'Slovakia', 'England']</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -28001,7 +28001,7 @@
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Wales', 'England']</t>
+          <t>['Wales', 'Slovakia', 'England']</t>
         </is>
       </c>
       <c r="K178" t="inlineStr">
@@ -28145,7 +28145,7 @@
       <c r="I179" t="inlineStr"/>
       <c r="J179" t="inlineStr">
         <is>
-          <t>['Northern Ireland', 'Poland', 'Germany']</t>
+          <t>['Poland', 'Germany', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K179" t="inlineStr">
@@ -28299,7 +28299,7 @@
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>['Northern Ireland', 'Poland', 'Germany']</t>
+          <t>['Poland', 'Germany', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K180" t="inlineStr">
@@ -28457,7 +28457,7 @@
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>['Northern Ireland', 'Poland', 'Germany']</t>
+          <t>['Poland', 'Germany', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
@@ -28601,7 +28601,7 @@
       <c r="I182" t="inlineStr"/>
       <c r="J182" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'Spain']</t>
+          <t>['Spain', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K182" t="inlineStr">
@@ -28755,7 +28755,7 @@
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'Spain']</t>
+          <t>['Spain', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K183" t="inlineStr">
@@ -28913,7 +28913,7 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain', 'Turkey']</t>
+          <t>['Spain', 'Croatia', 'Turkey']</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
@@ -29071,7 +29071,7 @@
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain', 'Turkey']</t>
+          <t>['Spain', 'Croatia', 'Turkey']</t>
         </is>
       </c>
       <c r="K185" t="inlineStr">
@@ -29229,7 +29229,7 @@
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain', 'Turkey']</t>
+          <t>['Spain', 'Croatia', 'Turkey']</t>
         </is>
       </c>
       <c r="K186" t="inlineStr">
@@ -29387,7 +29387,7 @@
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain', 'Turkey']</t>
+          <t>['Spain', 'Croatia', 'Turkey']</t>
         </is>
       </c>
       <c r="K187" t="inlineStr">
@@ -29531,7 +29531,7 @@
       <c r="I188" t="inlineStr"/>
       <c r="J188" t="inlineStr">
         <is>
-          <t>['Iceland', 'Portugal', 'Hungary']</t>
+          <t>['Iceland', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K188" t="inlineStr">
@@ -29685,7 +29685,7 @@
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>['Iceland', 'Portugal', 'Hungary']</t>
+          <t>['Iceland', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K189" t="inlineStr">
@@ -29843,7 +29843,7 @@
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>['Iceland', 'Portugal', 'Hungary']</t>
+          <t>['Iceland', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
@@ -30001,7 +30001,7 @@
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>['Iceland', 'Portugal', 'Hungary']</t>
+          <t>['Iceland', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K191" t="inlineStr">
@@ -30159,7 +30159,7 @@
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>['Iceland', 'Portugal', 'Hungary']</t>
+          <t>['Iceland', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K192" t="inlineStr">
@@ -30317,7 +30317,7 @@
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>['Iceland', 'Portugal', 'Hungary']</t>
+          <t>['Iceland', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K193" t="inlineStr">
@@ -30475,7 +30475,7 @@
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>['Iceland', 'Portugal', 'Hungary']</t>
+          <t>['Iceland', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
@@ -30633,7 +30633,7 @@
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>['Iceland', 'Portugal', 'Hungary']</t>
+          <t>['Iceland', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K195" t="inlineStr">
@@ -30791,7 +30791,7 @@
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>['Iceland', 'Portugal', 'Hungary']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="K196" t="inlineStr">
@@ -30949,7 +30949,7 @@
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>['Iceland', 'Portugal', 'Hungary']</t>
+          <t>['Iceland', 'Hungary', 'Portugal']</t>
         </is>
       </c>
       <c r="K197" t="inlineStr">
@@ -31093,7 +31093,7 @@
       <c r="I198" t="inlineStr"/>
       <c r="J198" t="inlineStr">
         <is>
-          <t>['Belgium', 'Sweden', 'Italy']</t>
+          <t>['Belgium', 'Italy', 'Sweden']</t>
         </is>
       </c>
       <c r="K198" t="inlineStr">
@@ -31247,7 +31247,7 @@
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>['Belgium', 'Ireland', 'Italy']</t>
+          <t>['Ireland', 'Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K199" t="inlineStr">
@@ -31405,7 +31405,7 @@
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>['Belgium', 'Ireland', 'Italy']</t>
+          <t>['Ireland', 'Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K200" t="inlineStr">
@@ -32479,7 +32479,7 @@
       <c r="I207" t="inlineStr"/>
       <c r="J207" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Netherlands', 'Austria']</t>
+          <t>['Netherlands', 'Austria', 'Ukraine']</t>
         </is>
       </c>
       <c r="K207" t="inlineStr">
@@ -32633,7 +32633,7 @@
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Netherlands', 'Austria']</t>
+          <t>['Netherlands', 'Austria', 'Ukraine']</t>
         </is>
       </c>
       <c r="K208" t="inlineStr">
@@ -32791,7 +32791,7 @@
       </c>
       <c r="J209" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Netherlands', 'Austria']</t>
+          <t>['Netherlands', 'Austria', 'Ukraine']</t>
         </is>
       </c>
       <c r="K209" t="inlineStr">
@@ -32949,7 +32949,7 @@
       </c>
       <c r="J210" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Netherlands', 'Austria']</t>
+          <t>['Netherlands', 'Austria', 'Ukraine']</t>
         </is>
       </c>
       <c r="K210" t="inlineStr">
@@ -33107,7 +33107,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Netherlands', 'Austria']</t>
+          <t>['Netherlands', 'Austria', 'Ukraine']</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
@@ -33405,7 +33405,7 @@
       </c>
       <c r="J213" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Denmark', 'Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K213" t="inlineStr">
@@ -33563,7 +33563,7 @@
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Denmark', 'Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K214" t="inlineStr">
@@ -33721,7 +33721,7 @@
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Denmark', 'Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="K215" t="inlineStr">
@@ -33879,7 +33879,7 @@
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>['Belgium', 'Russia', 'Denmark']</t>
+          <t>['Belgium', 'Denmark', 'Russia']</t>
         </is>
       </c>
       <c r="K216" t="inlineStr">
@@ -34037,7 +34037,7 @@
       </c>
       <c r="J217" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Finland', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="K217" t="inlineStr">
@@ -34195,7 +34195,7 @@
       </c>
       <c r="J218" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Finland', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="K218" t="inlineStr">
@@ -34353,7 +34353,7 @@
       </c>
       <c r="J219" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Finland', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="K219" t="inlineStr">
@@ -34497,7 +34497,7 @@
       <c r="I220" t="inlineStr"/>
       <c r="J220" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'England']</t>
+          <t>['England', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K220" t="inlineStr">
@@ -34651,7 +34651,7 @@
       </c>
       <c r="J221" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'England']</t>
+          <t>['England', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K221" t="inlineStr">
@@ -34809,7 +34809,7 @@
       </c>
       <c r="J222" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'England']</t>
+          <t>['England', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K222" t="inlineStr">
@@ -34967,7 +34967,7 @@
       </c>
       <c r="J223" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'England']</t>
+          <t>['England', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K223" t="inlineStr">
@@ -35125,7 +35125,7 @@
       </c>
       <c r="J224" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'England']</t>
+          <t>['England', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K224" t="inlineStr">
@@ -35283,7 +35283,7 @@
       </c>
       <c r="J225" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'England']</t>
+          <t>['England', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K225" t="inlineStr">
@@ -35427,7 +35427,7 @@
       <c r="I226" t="inlineStr"/>
       <c r="J226" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K226" t="inlineStr">
@@ -35581,7 +35581,7 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K227" t="inlineStr">
@@ -35739,7 +35739,7 @@
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
@@ -35897,7 +35897,7 @@
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
@@ -36055,7 +36055,7 @@
       </c>
       <c r="J230" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K230" t="inlineStr">
@@ -36213,7 +36213,7 @@
       </c>
       <c r="J231" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K231" t="inlineStr">
@@ -36371,7 +36371,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
@@ -36529,7 +36529,7 @@
       </c>
       <c r="J233" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K233" t="inlineStr">
@@ -36687,7 +36687,7 @@
       </c>
       <c r="J234" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K234" t="inlineStr">
@@ -36845,7 +36845,7 @@
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K235" t="inlineStr">
@@ -37003,7 +37003,7 @@
       </c>
       <c r="J236" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain', 'Slovakia']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K236" t="inlineStr">
@@ -38551,7 +38551,7 @@
       <c r="I246" t="inlineStr"/>
       <c r="J246" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Scotland', 'Germany']</t>
+          <t>['Scotland', 'Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="K246" t="inlineStr">
@@ -38705,7 +38705,7 @@
       </c>
       <c r="J247" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Scotland', 'Germany']</t>
+          <t>['Scotland', 'Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="K247" t="inlineStr">
@@ -38863,7 +38863,7 @@
       </c>
       <c r="J248" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Scotland', 'Germany']</t>
+          <t>['Scotland', 'Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="K248" t="inlineStr">
@@ -39021,7 +39021,7 @@
       </c>
       <c r="J249" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Hungary', 'Germany']</t>
+          <t>['Germany', 'Switzerland', 'Hungary']</t>
         </is>
       </c>
       <c r="K249" t="inlineStr">
@@ -39165,7 +39165,7 @@
       <c r="I250" t="inlineStr"/>
       <c r="J250" t="inlineStr">
         <is>
-          <t>['Albania', 'Spain', 'Italy']</t>
+          <t>['Spain', 'Albania', 'Italy']</t>
         </is>
       </c>
       <c r="K250" t="inlineStr">
@@ -39319,7 +39319,7 @@
       </c>
       <c r="J251" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain', 'Italy']</t>
+          <t>['Spain', 'Italy', 'Croatia']</t>
         </is>
       </c>
       <c r="K251" t="inlineStr">
@@ -39477,7 +39477,7 @@
       </c>
       <c r="J252" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain', 'Italy']</t>
+          <t>['Spain', 'Italy', 'Croatia']</t>
         </is>
       </c>
       <c r="K252" t="inlineStr">
@@ -39635,7 +39635,7 @@
       </c>
       <c r="J253" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain', 'Italy']</t>
+          <t>['Spain', 'Italy', 'Croatia']</t>
         </is>
       </c>
       <c r="K253" t="inlineStr">
@@ -40407,7 +40407,7 @@
       </c>
       <c r="J258" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France', 'Austria']</t>
+          <t>['Austria', 'France', 'Netherlands']</t>
         </is>
       </c>
       <c r="K258" t="inlineStr">
@@ -41025,7 +41025,7 @@
       <c r="I262" t="inlineStr"/>
       <c r="J262" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England', 'Denmark']</t>
+          <t>['England', 'Denmark', 'Slovenia']</t>
         </is>
       </c>
       <c r="K262" t="inlineStr">
@@ -41165,7 +41165,7 @@
       <c r="I263" t="inlineStr"/>
       <c r="J263" t="inlineStr">
         <is>
-          <t>['Romania', 'Slovakia', 'Belgium']</t>
+          <t>['Belgium', 'Slovakia', 'Romania']</t>
         </is>
       </c>
       <c r="K263" t="inlineStr">
@@ -41319,7 +41319,7 @@
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>['Belgium', 'Ukraine', 'Slovakia']</t>
+          <t>['Slovakia', 'Belgium', 'Ukraine']</t>
         </is>
       </c>
       <c r="K264" t="inlineStr">
@@ -41477,7 +41477,7 @@
       </c>
       <c r="J265" t="inlineStr">
         <is>
-          <t>['Romania', 'Slovakia', 'Belgium']</t>
+          <t>['Belgium', 'Slovakia', 'Romania']</t>
         </is>
       </c>
       <c r="K265" t="inlineStr">
@@ -41775,7 +41775,7 @@
       </c>
       <c r="J267" t="inlineStr">
         <is>
-          <t>['Georgia', 'Portugal', 'Turkey']</t>
+          <t>['Portugal', 'Georgia', 'Turkey']</t>
         </is>
       </c>
       <c r="K267" t="inlineStr">
@@ -41933,7 +41933,7 @@
       </c>
       <c r="J268" t="inlineStr">
         <is>
-          <t>['Georgia', 'Portugal', 'Turkey']</t>
+          <t>['Portugal', 'Georgia', 'Turkey']</t>
         </is>
       </c>
       <c r="K268" t="inlineStr">
@@ -42091,7 +42091,7 @@
       </c>
       <c r="J269" t="inlineStr">
         <is>
-          <t>['Georgia', 'Portugal', 'Turkey']</t>
+          <t>['Portugal', 'Georgia', 'Turkey']</t>
         </is>
       </c>
       <c r="K269" t="inlineStr">
@@ -42407,7 +42407,7 @@
       </c>
       <c r="J271" t="inlineStr">
         <is>
-          <t>['Georgia', 'Portugal', 'Turkey']</t>
+          <t>['Portugal', 'Georgia', 'Turkey']</t>
         </is>
       </c>
       <c r="K271" t="inlineStr">

</xml_diff>